<commit_message>
Reverting TES-tab in CONVERSION.xlsx
In the last update, I accidentally deleted the information on PCM-Storages from the Swiss database. The table was now reset.
</commit_message>
<xml_diff>
--- a/cea/databases/CH/components/CONVERSION.xlsx
+++ b/cea/databases/CH/components/CONVERSION.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10814"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\luis.santos\Documents\CityEnergyAnalyst\CityEnergyAnalyst\cea\databases\CH\components\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mathiasniffeler/Documents/GitHub/CityEnergyAnalyst/cea/databases/CH/components/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BCEA663-B35A-45F7-872E-36245FB693A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E90840EC-012D-934C-89E2-987B2DBD4565}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="993" activeTab="15" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="10740" tabRatio="993" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PV" sheetId="1" r:id="rId1"/>
@@ -34,23 +34,12 @@
     <definedName name="__xlfn_AGGREGATE">#N/A</definedName>
     <definedName name="__xlfn_STDEV_S">#N/A</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="522" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="560" uniqueCount="171">
   <si>
     <t>Description</t>
   </si>
@@ -400,9 +389,6 @@
     <t>cap_min, cap_max</t>
   </si>
   <si>
-    <t>short-term storage tank</t>
-  </si>
-  <si>
     <t>TES2</t>
   </si>
   <si>
@@ -500,6 +486,72 @@
   </si>
   <si>
     <t>G_VALUE</t>
+  </si>
+  <si>
+    <t>LT_mat_yr</t>
+  </si>
+  <si>
+    <t>C_mat_%</t>
+  </si>
+  <si>
+    <t>T_PHCH_C</t>
+  </si>
+  <si>
+    <t>T_min_C</t>
+  </si>
+  <si>
+    <t>T_max_C</t>
+  </si>
+  <si>
+    <t>HL_kJkg</t>
+  </si>
+  <si>
+    <t>Rho_T_PHCH_kgm3</t>
+  </si>
+  <si>
+    <t>Cp_kJkgK</t>
+  </si>
+  <si>
+    <t>n_ch</t>
+  </si>
+  <si>
+    <t>n_disch</t>
+  </si>
+  <si>
+    <t>HEATING</t>
+  </si>
+  <si>
+    <t>short-term storage tank - water</t>
+  </si>
+  <si>
+    <t>COOLING</t>
+  </si>
+  <si>
+    <t>kWh</t>
+  </si>
+  <si>
+    <t>short-term storage tank- ice</t>
+  </si>
+  <si>
+    <t>TES3</t>
+  </si>
+  <si>
+    <t>short-term storage tank - eutectic salt</t>
+  </si>
+  <si>
+    <t>TES4</t>
+  </si>
+  <si>
+    <t>short-term storage tank - PEG400</t>
+  </si>
+  <si>
+    <t>TES5</t>
+  </si>
+  <si>
+    <t>short-term storage tank - Paraffin C14</t>
+  </si>
+  <si>
+    <t>TES6</t>
   </si>
 </sst>
 </file>
@@ -557,7 +609,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -604,6 +656,21 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -611,7 +678,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -648,6 +715,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1086,33 +1159,33 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AA10"/>
   <sheetViews>
-    <sheetView topLeftCell="N1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="N1" sqref="N1:Q2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="38.7265625" customWidth="1"/>
-    <col min="4" max="4" width="15.7265625" customWidth="1"/>
+    <col min="1" max="1" width="38.6640625" customWidth="1"/>
+    <col min="4" max="4" width="15.6640625" customWidth="1"/>
     <col min="5" max="6" width="12" customWidth="1"/>
-    <col min="7" max="7" width="14.54296875" customWidth="1"/>
-    <col min="8" max="8" width="9.26953125" customWidth="1"/>
-    <col min="9" max="9" width="8.54296875" customWidth="1"/>
-    <col min="10" max="10" width="8.7265625" customWidth="1"/>
-    <col min="12" max="12" width="16.453125" customWidth="1"/>
-    <col min="13" max="13" width="18.54296875" customWidth="1"/>
-    <col min="14" max="14" width="16.26953125" customWidth="1"/>
-    <col min="15" max="15" width="14.7265625" customWidth="1"/>
-    <col min="16" max="17" width="12.453125" customWidth="1"/>
-    <col min="19" max="19" width="10.453125" customWidth="1"/>
-    <col min="20" max="20" width="13.7265625" customWidth="1"/>
-    <col min="21" max="23" width="10.453125" customWidth="1"/>
-    <col min="24" max="24" width="14.7265625" customWidth="1"/>
-    <col min="25" max="25" width="12.7265625" customWidth="1"/>
-    <col min="27" max="27" width="13.26953125" customWidth="1"/>
+    <col min="7" max="7" width="14.5" customWidth="1"/>
+    <col min="8" max="8" width="9.33203125" customWidth="1"/>
+    <col min="9" max="9" width="8.5" customWidth="1"/>
+    <col min="10" max="10" width="8.6640625" customWidth="1"/>
+    <col min="12" max="12" width="16.5" customWidth="1"/>
+    <col min="13" max="13" width="18.5" customWidth="1"/>
+    <col min="14" max="14" width="16.33203125" customWidth="1"/>
+    <col min="15" max="15" width="14.6640625" customWidth="1"/>
+    <col min="16" max="17" width="12.5" customWidth="1"/>
+    <col min="19" max="19" width="10.5" customWidth="1"/>
+    <col min="20" max="20" width="13.6640625" customWidth="1"/>
+    <col min="21" max="23" width="10.5" customWidth="1"/>
+    <col min="24" max="24" width="14.6640625" customWidth="1"/>
+    <col min="25" max="25" width="12.6640625" customWidth="1"/>
+    <col min="27" max="27" width="13.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1195,7 +1268,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>27</v>
       </c>
@@ -1279,7 +1352,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>27</v>
       </c>
@@ -1363,7 +1436,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>27</v>
       </c>
@@ -1447,7 +1520,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="5" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>33</v>
       </c>
@@ -1531,7 +1604,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>33</v>
       </c>
@@ -1615,7 +1688,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>33</v>
       </c>
@@ -1699,7 +1772,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="8" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>35</v>
       </c>
@@ -1783,7 +1856,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="9" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>35</v>
       </c>
@@ -1867,7 +1940,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="10" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>35</v>
       </c>
@@ -1967,13 +2040,13 @@
       <selection activeCell="J29" sqref="J29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="27.7265625" customWidth="1"/>
-    <col min="5" max="5" width="9.7265625" customWidth="1"/>
+    <col min="1" max="1" width="27.6640625" customWidth="1"/>
+    <col min="5" max="5" width="9.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2053,7 +2126,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>87</v>
       </c>
@@ -2133,7 +2206,7 @@
         <v>0.33300000000000002</v>
       </c>
     </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>87</v>
       </c>
@@ -2213,7 +2286,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>91</v>
       </c>
@@ -2293,7 +2366,7 @@
         <v>0.33300000000000002</v>
       </c>
     </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>94</v>
       </c>
@@ -2373,7 +2446,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>94</v>
       </c>
@@ -2453,7 +2526,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>96</v>
       </c>
@@ -2549,15 +2622,15 @@
       <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="26.453125" customWidth="1"/>
-    <col min="3" max="3" width="18.453125" customWidth="1"/>
-    <col min="4" max="5" width="15.26953125" customWidth="1"/>
+    <col min="1" max="1" width="26.5" customWidth="1"/>
+    <col min="3" max="3" width="18.5" customWidth="1"/>
+    <col min="4" max="5" width="15.33203125" customWidth="1"/>
     <col min="15" max="15" width="29" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2604,7 +2677,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>99</v>
       </c>
@@ -2651,7 +2724,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>99</v>
       </c>
@@ -2714,16 +2787,16 @@
       <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="28.7265625" customWidth="1"/>
-    <col min="2" max="2" width="16.453125" customWidth="1"/>
-    <col min="3" max="3" width="16.7265625" customWidth="1"/>
+    <col min="1" max="1" width="28.6640625" customWidth="1"/>
+    <col min="2" max="2" width="16.5" customWidth="1"/>
+    <col min="3" max="3" width="16.6640625" customWidth="1"/>
     <col min="4" max="5" width="23" customWidth="1"/>
     <col min="12" max="12" width="19" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2758,19 +2831,19 @@
         <v>22</v>
       </c>
       <c r="L1" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="M1" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>127</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>128</v>
       </c>
       <c r="Q1" s="1" t="s">
         <v>23</v>
@@ -2785,7 +2858,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>103</v>
       </c>
@@ -2847,7 +2920,7 @@
       </c>
       <c r="T2" s="2"/>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>103</v>
       </c>
@@ -2908,7 +2981,7 @@
       </c>
       <c r="T3" s="2"/>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>103</v>
       </c>
@@ -2970,12 +3043,12 @@
       </c>
       <c r="T4" s="2"/>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>120</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>121</v>
       </c>
       <c r="C5" s="2">
         <v>0</v>
@@ -2984,7 +3057,7 @@
         <v>500</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="F5" s="2" t="s">
         <v>31</v>
@@ -3029,7 +3102,7 @@
         <v>5</v>
       </c>
       <c r="T5" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
   </sheetData>
@@ -3048,16 +3121,16 @@
       <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="23" customWidth="1"/>
-    <col min="2" max="2" width="15.26953125" customWidth="1"/>
-    <col min="3" max="3" width="16.7265625" customWidth="1"/>
+    <col min="2" max="2" width="15.33203125" customWidth="1"/>
+    <col min="3" max="3" width="16.6640625" customWidth="1"/>
     <col min="4" max="4" width="13" customWidth="1"/>
-    <col min="15" max="15" width="29.7265625" customWidth="1"/>
+    <col min="15" max="15" width="29.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3104,7 +3177,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>105</v>
       </c>
@@ -3166,17 +3239,17 @@
       <selection activeCell="O6" sqref="O6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="29" customWidth="1"/>
-    <col min="3" max="3" width="17.453125" customWidth="1"/>
-    <col min="4" max="5" width="20.54296875" customWidth="1"/>
-    <col min="7" max="7" width="11.26953125" customWidth="1"/>
-    <col min="9" max="9" width="12.453125" customWidth="1"/>
+    <col min="3" max="3" width="17.5" customWidth="1"/>
+    <col min="4" max="5" width="20.5" customWidth="1"/>
+    <col min="7" max="7" width="11.33203125" customWidth="1"/>
+    <col min="9" max="9" width="12.5" customWidth="1"/>
     <col min="10" max="10" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3223,7 +3296,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>107</v>
       </c>
@@ -3269,7 +3342,7 @@
       </c>
       <c r="O2" s="2"/>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>109</v>
       </c>
@@ -3332,16 +3405,16 @@
       <selection activeCell="N32" sqref="N32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="17.453125" customWidth="1"/>
+    <col min="1" max="1" width="17.5" customWidth="1"/>
     <col min="3" max="3" width="18" customWidth="1"/>
-    <col min="4" max="5" width="21.7265625" customWidth="1"/>
-    <col min="8" max="8" width="11.7265625" customWidth="1"/>
+    <col min="4" max="5" width="21.6640625" customWidth="1"/>
+    <col min="8" max="8" width="11.6640625" customWidth="1"/>
     <col min="10" max="10" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3388,12 +3461,12 @@
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>118</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>119</v>
       </c>
       <c r="C2" s="2">
         <v>500</v>
@@ -3436,12 +3509,12 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>118</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>119</v>
       </c>
       <c r="C3" s="2">
         <v>4000</v>
@@ -3484,12 +3557,12 @@
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>118</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>119</v>
       </c>
       <c r="C4" s="2">
         <v>37000</v>
@@ -3532,12 +3605,12 @@
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>118</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>119</v>
       </c>
       <c r="C5" s="2">
         <v>37000</v>
@@ -3590,21 +3663,657 @@
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
-  <dimension ref="A1:O4"/>
+  <dimension ref="A1:Z8"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="A41" sqref="A41"/>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="43.26953125" customWidth="1"/>
-    <col min="2" max="2" width="12.7265625" customWidth="1"/>
-    <col min="3" max="3" width="19.7265625" customWidth="1"/>
-    <col min="4" max="5" width="19.26953125" customWidth="1"/>
+    <col min="1" max="1" width="43.33203125" customWidth="1"/>
+    <col min="2" max="2" width="12.6640625" customWidth="1"/>
+    <col min="3" max="3" width="19.6640625" customWidth="1"/>
+    <col min="4" max="5" width="19.33203125" customWidth="1"/>
+    <col min="14" max="14" width="10" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="10" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="7" customWidth="1"/>
+    <col min="26" max="26" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="257" max="257" width="43.33203125" customWidth="1"/>
+    <col min="258" max="258" width="12.6640625" customWidth="1"/>
+    <col min="259" max="259" width="19.6640625" customWidth="1"/>
+    <col min="260" max="261" width="19.33203125" customWidth="1"/>
+    <col min="270" max="270" width="10" bestFit="1" customWidth="1"/>
+    <col min="271" max="271" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="274" max="274" width="10" bestFit="1" customWidth="1"/>
+    <col min="278" max="278" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="280" max="280" width="7" customWidth="1"/>
+    <col min="282" max="282" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="513" max="513" width="43.33203125" customWidth="1"/>
+    <col min="514" max="514" width="12.6640625" customWidth="1"/>
+    <col min="515" max="515" width="19.6640625" customWidth="1"/>
+    <col min="516" max="517" width="19.33203125" customWidth="1"/>
+    <col min="526" max="526" width="10" bestFit="1" customWidth="1"/>
+    <col min="527" max="527" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="530" max="530" width="10" bestFit="1" customWidth="1"/>
+    <col min="534" max="534" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="536" max="536" width="7" customWidth="1"/>
+    <col min="538" max="538" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="769" max="769" width="43.33203125" customWidth="1"/>
+    <col min="770" max="770" width="12.6640625" customWidth="1"/>
+    <col min="771" max="771" width="19.6640625" customWidth="1"/>
+    <col min="772" max="773" width="19.33203125" customWidth="1"/>
+    <col min="782" max="782" width="10" bestFit="1" customWidth="1"/>
+    <col min="783" max="783" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="786" max="786" width="10" bestFit="1" customWidth="1"/>
+    <col min="790" max="790" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="792" max="792" width="7" customWidth="1"/>
+    <col min="794" max="794" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="1025" max="1025" width="43.33203125" customWidth="1"/>
+    <col min="1026" max="1026" width="12.6640625" customWidth="1"/>
+    <col min="1027" max="1027" width="19.6640625" customWidth="1"/>
+    <col min="1028" max="1029" width="19.33203125" customWidth="1"/>
+    <col min="1038" max="1038" width="10" bestFit="1" customWidth="1"/>
+    <col min="1039" max="1039" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="1042" max="1042" width="10" bestFit="1" customWidth="1"/>
+    <col min="1046" max="1046" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="1048" max="1048" width="7" customWidth="1"/>
+    <col min="1050" max="1050" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="1281" max="1281" width="43.33203125" customWidth="1"/>
+    <col min="1282" max="1282" width="12.6640625" customWidth="1"/>
+    <col min="1283" max="1283" width="19.6640625" customWidth="1"/>
+    <col min="1284" max="1285" width="19.33203125" customWidth="1"/>
+    <col min="1294" max="1294" width="10" bestFit="1" customWidth="1"/>
+    <col min="1295" max="1295" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="1298" max="1298" width="10" bestFit="1" customWidth="1"/>
+    <col min="1302" max="1302" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="1304" max="1304" width="7" customWidth="1"/>
+    <col min="1306" max="1306" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="1537" max="1537" width="43.33203125" customWidth="1"/>
+    <col min="1538" max="1538" width="12.6640625" customWidth="1"/>
+    <col min="1539" max="1539" width="19.6640625" customWidth="1"/>
+    <col min="1540" max="1541" width="19.33203125" customWidth="1"/>
+    <col min="1550" max="1550" width="10" bestFit="1" customWidth="1"/>
+    <col min="1551" max="1551" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="1554" max="1554" width="10" bestFit="1" customWidth="1"/>
+    <col min="1558" max="1558" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="1560" max="1560" width="7" customWidth="1"/>
+    <col min="1562" max="1562" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="1793" max="1793" width="43.33203125" customWidth="1"/>
+    <col min="1794" max="1794" width="12.6640625" customWidth="1"/>
+    <col min="1795" max="1795" width="19.6640625" customWidth="1"/>
+    <col min="1796" max="1797" width="19.33203125" customWidth="1"/>
+    <col min="1806" max="1806" width="10" bestFit="1" customWidth="1"/>
+    <col min="1807" max="1807" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="1810" max="1810" width="10" bestFit="1" customWidth="1"/>
+    <col min="1814" max="1814" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="1816" max="1816" width="7" customWidth="1"/>
+    <col min="1818" max="1818" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="2049" max="2049" width="43.33203125" customWidth="1"/>
+    <col min="2050" max="2050" width="12.6640625" customWidth="1"/>
+    <col min="2051" max="2051" width="19.6640625" customWidth="1"/>
+    <col min="2052" max="2053" width="19.33203125" customWidth="1"/>
+    <col min="2062" max="2062" width="10" bestFit="1" customWidth="1"/>
+    <col min="2063" max="2063" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="2066" max="2066" width="10" bestFit="1" customWidth="1"/>
+    <col min="2070" max="2070" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="2072" max="2072" width="7" customWidth="1"/>
+    <col min="2074" max="2074" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="2305" max="2305" width="43.33203125" customWidth="1"/>
+    <col min="2306" max="2306" width="12.6640625" customWidth="1"/>
+    <col min="2307" max="2307" width="19.6640625" customWidth="1"/>
+    <col min="2308" max="2309" width="19.33203125" customWidth="1"/>
+    <col min="2318" max="2318" width="10" bestFit="1" customWidth="1"/>
+    <col min="2319" max="2319" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="2322" max="2322" width="10" bestFit="1" customWidth="1"/>
+    <col min="2326" max="2326" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="2328" max="2328" width="7" customWidth="1"/>
+    <col min="2330" max="2330" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="2561" max="2561" width="43.33203125" customWidth="1"/>
+    <col min="2562" max="2562" width="12.6640625" customWidth="1"/>
+    <col min="2563" max="2563" width="19.6640625" customWidth="1"/>
+    <col min="2564" max="2565" width="19.33203125" customWidth="1"/>
+    <col min="2574" max="2574" width="10" bestFit="1" customWidth="1"/>
+    <col min="2575" max="2575" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="2578" max="2578" width="10" bestFit="1" customWidth="1"/>
+    <col min="2582" max="2582" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="2584" max="2584" width="7" customWidth="1"/>
+    <col min="2586" max="2586" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="2817" max="2817" width="43.33203125" customWidth="1"/>
+    <col min="2818" max="2818" width="12.6640625" customWidth="1"/>
+    <col min="2819" max="2819" width="19.6640625" customWidth="1"/>
+    <col min="2820" max="2821" width="19.33203125" customWidth="1"/>
+    <col min="2830" max="2830" width="10" bestFit="1" customWidth="1"/>
+    <col min="2831" max="2831" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="2834" max="2834" width="10" bestFit="1" customWidth="1"/>
+    <col min="2838" max="2838" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="2840" max="2840" width="7" customWidth="1"/>
+    <col min="2842" max="2842" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="3073" max="3073" width="43.33203125" customWidth="1"/>
+    <col min="3074" max="3074" width="12.6640625" customWidth="1"/>
+    <col min="3075" max="3075" width="19.6640625" customWidth="1"/>
+    <col min="3076" max="3077" width="19.33203125" customWidth="1"/>
+    <col min="3086" max="3086" width="10" bestFit="1" customWidth="1"/>
+    <col min="3087" max="3087" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="3090" max="3090" width="10" bestFit="1" customWidth="1"/>
+    <col min="3094" max="3094" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="3096" max="3096" width="7" customWidth="1"/>
+    <col min="3098" max="3098" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="3329" max="3329" width="43.33203125" customWidth="1"/>
+    <col min="3330" max="3330" width="12.6640625" customWidth="1"/>
+    <col min="3331" max="3331" width="19.6640625" customWidth="1"/>
+    <col min="3332" max="3333" width="19.33203125" customWidth="1"/>
+    <col min="3342" max="3342" width="10" bestFit="1" customWidth="1"/>
+    <col min="3343" max="3343" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="3346" max="3346" width="10" bestFit="1" customWidth="1"/>
+    <col min="3350" max="3350" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="3352" max="3352" width="7" customWidth="1"/>
+    <col min="3354" max="3354" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="3585" max="3585" width="43.33203125" customWidth="1"/>
+    <col min="3586" max="3586" width="12.6640625" customWidth="1"/>
+    <col min="3587" max="3587" width="19.6640625" customWidth="1"/>
+    <col min="3588" max="3589" width="19.33203125" customWidth="1"/>
+    <col min="3598" max="3598" width="10" bestFit="1" customWidth="1"/>
+    <col min="3599" max="3599" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="3602" max="3602" width="10" bestFit="1" customWidth="1"/>
+    <col min="3606" max="3606" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="3608" max="3608" width="7" customWidth="1"/>
+    <col min="3610" max="3610" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="3841" max="3841" width="43.33203125" customWidth="1"/>
+    <col min="3842" max="3842" width="12.6640625" customWidth="1"/>
+    <col min="3843" max="3843" width="19.6640625" customWidth="1"/>
+    <col min="3844" max="3845" width="19.33203125" customWidth="1"/>
+    <col min="3854" max="3854" width="10" bestFit="1" customWidth="1"/>
+    <col min="3855" max="3855" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="3858" max="3858" width="10" bestFit="1" customWidth="1"/>
+    <col min="3862" max="3862" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="3864" max="3864" width="7" customWidth="1"/>
+    <col min="3866" max="3866" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="4097" max="4097" width="43.33203125" customWidth="1"/>
+    <col min="4098" max="4098" width="12.6640625" customWidth="1"/>
+    <col min="4099" max="4099" width="19.6640625" customWidth="1"/>
+    <col min="4100" max="4101" width="19.33203125" customWidth="1"/>
+    <col min="4110" max="4110" width="10" bestFit="1" customWidth="1"/>
+    <col min="4111" max="4111" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="4114" max="4114" width="10" bestFit="1" customWidth="1"/>
+    <col min="4118" max="4118" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="4120" max="4120" width="7" customWidth="1"/>
+    <col min="4122" max="4122" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="4353" max="4353" width="43.33203125" customWidth="1"/>
+    <col min="4354" max="4354" width="12.6640625" customWidth="1"/>
+    <col min="4355" max="4355" width="19.6640625" customWidth="1"/>
+    <col min="4356" max="4357" width="19.33203125" customWidth="1"/>
+    <col min="4366" max="4366" width="10" bestFit="1" customWidth="1"/>
+    <col min="4367" max="4367" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="4370" max="4370" width="10" bestFit="1" customWidth="1"/>
+    <col min="4374" max="4374" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="4376" max="4376" width="7" customWidth="1"/>
+    <col min="4378" max="4378" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="4609" max="4609" width="43.33203125" customWidth="1"/>
+    <col min="4610" max="4610" width="12.6640625" customWidth="1"/>
+    <col min="4611" max="4611" width="19.6640625" customWidth="1"/>
+    <col min="4612" max="4613" width="19.33203125" customWidth="1"/>
+    <col min="4622" max="4622" width="10" bestFit="1" customWidth="1"/>
+    <col min="4623" max="4623" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="4626" max="4626" width="10" bestFit="1" customWidth="1"/>
+    <col min="4630" max="4630" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="4632" max="4632" width="7" customWidth="1"/>
+    <col min="4634" max="4634" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="4865" max="4865" width="43.33203125" customWidth="1"/>
+    <col min="4866" max="4866" width="12.6640625" customWidth="1"/>
+    <col min="4867" max="4867" width="19.6640625" customWidth="1"/>
+    <col min="4868" max="4869" width="19.33203125" customWidth="1"/>
+    <col min="4878" max="4878" width="10" bestFit="1" customWidth="1"/>
+    <col min="4879" max="4879" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="4882" max="4882" width="10" bestFit="1" customWidth="1"/>
+    <col min="4886" max="4886" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="4888" max="4888" width="7" customWidth="1"/>
+    <col min="4890" max="4890" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="5121" max="5121" width="43.33203125" customWidth="1"/>
+    <col min="5122" max="5122" width="12.6640625" customWidth="1"/>
+    <col min="5123" max="5123" width="19.6640625" customWidth="1"/>
+    <col min="5124" max="5125" width="19.33203125" customWidth="1"/>
+    <col min="5134" max="5134" width="10" bestFit="1" customWidth="1"/>
+    <col min="5135" max="5135" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="5138" max="5138" width="10" bestFit="1" customWidth="1"/>
+    <col min="5142" max="5142" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="5144" max="5144" width="7" customWidth="1"/>
+    <col min="5146" max="5146" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="5377" max="5377" width="43.33203125" customWidth="1"/>
+    <col min="5378" max="5378" width="12.6640625" customWidth="1"/>
+    <col min="5379" max="5379" width="19.6640625" customWidth="1"/>
+    <col min="5380" max="5381" width="19.33203125" customWidth="1"/>
+    <col min="5390" max="5390" width="10" bestFit="1" customWidth="1"/>
+    <col min="5391" max="5391" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="5394" max="5394" width="10" bestFit="1" customWidth="1"/>
+    <col min="5398" max="5398" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="5400" max="5400" width="7" customWidth="1"/>
+    <col min="5402" max="5402" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="5633" max="5633" width="43.33203125" customWidth="1"/>
+    <col min="5634" max="5634" width="12.6640625" customWidth="1"/>
+    <col min="5635" max="5635" width="19.6640625" customWidth="1"/>
+    <col min="5636" max="5637" width="19.33203125" customWidth="1"/>
+    <col min="5646" max="5646" width="10" bestFit="1" customWidth="1"/>
+    <col min="5647" max="5647" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="5650" max="5650" width="10" bestFit="1" customWidth="1"/>
+    <col min="5654" max="5654" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="5656" max="5656" width="7" customWidth="1"/>
+    <col min="5658" max="5658" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="5889" max="5889" width="43.33203125" customWidth="1"/>
+    <col min="5890" max="5890" width="12.6640625" customWidth="1"/>
+    <col min="5891" max="5891" width="19.6640625" customWidth="1"/>
+    <col min="5892" max="5893" width="19.33203125" customWidth="1"/>
+    <col min="5902" max="5902" width="10" bestFit="1" customWidth="1"/>
+    <col min="5903" max="5903" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="5906" max="5906" width="10" bestFit="1" customWidth="1"/>
+    <col min="5910" max="5910" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="5912" max="5912" width="7" customWidth="1"/>
+    <col min="5914" max="5914" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="6145" max="6145" width="43.33203125" customWidth="1"/>
+    <col min="6146" max="6146" width="12.6640625" customWidth="1"/>
+    <col min="6147" max="6147" width="19.6640625" customWidth="1"/>
+    <col min="6148" max="6149" width="19.33203125" customWidth="1"/>
+    <col min="6158" max="6158" width="10" bestFit="1" customWidth="1"/>
+    <col min="6159" max="6159" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="6162" max="6162" width="10" bestFit="1" customWidth="1"/>
+    <col min="6166" max="6166" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="6168" max="6168" width="7" customWidth="1"/>
+    <col min="6170" max="6170" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="6401" max="6401" width="43.33203125" customWidth="1"/>
+    <col min="6402" max="6402" width="12.6640625" customWidth="1"/>
+    <col min="6403" max="6403" width="19.6640625" customWidth="1"/>
+    <col min="6404" max="6405" width="19.33203125" customWidth="1"/>
+    <col min="6414" max="6414" width="10" bestFit="1" customWidth="1"/>
+    <col min="6415" max="6415" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="6418" max="6418" width="10" bestFit="1" customWidth="1"/>
+    <col min="6422" max="6422" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="6424" max="6424" width="7" customWidth="1"/>
+    <col min="6426" max="6426" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="6657" max="6657" width="43.33203125" customWidth="1"/>
+    <col min="6658" max="6658" width="12.6640625" customWidth="1"/>
+    <col min="6659" max="6659" width="19.6640625" customWidth="1"/>
+    <col min="6660" max="6661" width="19.33203125" customWidth="1"/>
+    <col min="6670" max="6670" width="10" bestFit="1" customWidth="1"/>
+    <col min="6671" max="6671" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="6674" max="6674" width="10" bestFit="1" customWidth="1"/>
+    <col min="6678" max="6678" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="6680" max="6680" width="7" customWidth="1"/>
+    <col min="6682" max="6682" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="6913" max="6913" width="43.33203125" customWidth="1"/>
+    <col min="6914" max="6914" width="12.6640625" customWidth="1"/>
+    <col min="6915" max="6915" width="19.6640625" customWidth="1"/>
+    <col min="6916" max="6917" width="19.33203125" customWidth="1"/>
+    <col min="6926" max="6926" width="10" bestFit="1" customWidth="1"/>
+    <col min="6927" max="6927" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="6930" max="6930" width="10" bestFit="1" customWidth="1"/>
+    <col min="6934" max="6934" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="6936" max="6936" width="7" customWidth="1"/>
+    <col min="6938" max="6938" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="7169" max="7169" width="43.33203125" customWidth="1"/>
+    <col min="7170" max="7170" width="12.6640625" customWidth="1"/>
+    <col min="7171" max="7171" width="19.6640625" customWidth="1"/>
+    <col min="7172" max="7173" width="19.33203125" customWidth="1"/>
+    <col min="7182" max="7182" width="10" bestFit="1" customWidth="1"/>
+    <col min="7183" max="7183" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="7186" max="7186" width="10" bestFit="1" customWidth="1"/>
+    <col min="7190" max="7190" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="7192" max="7192" width="7" customWidth="1"/>
+    <col min="7194" max="7194" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="7425" max="7425" width="43.33203125" customWidth="1"/>
+    <col min="7426" max="7426" width="12.6640625" customWidth="1"/>
+    <col min="7427" max="7427" width="19.6640625" customWidth="1"/>
+    <col min="7428" max="7429" width="19.33203125" customWidth="1"/>
+    <col min="7438" max="7438" width="10" bestFit="1" customWidth="1"/>
+    <col min="7439" max="7439" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="7442" max="7442" width="10" bestFit="1" customWidth="1"/>
+    <col min="7446" max="7446" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="7448" max="7448" width="7" customWidth="1"/>
+    <col min="7450" max="7450" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="7681" max="7681" width="43.33203125" customWidth="1"/>
+    <col min="7682" max="7682" width="12.6640625" customWidth="1"/>
+    <col min="7683" max="7683" width="19.6640625" customWidth="1"/>
+    <col min="7684" max="7685" width="19.33203125" customWidth="1"/>
+    <col min="7694" max="7694" width="10" bestFit="1" customWidth="1"/>
+    <col min="7695" max="7695" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="7698" max="7698" width="10" bestFit="1" customWidth="1"/>
+    <col min="7702" max="7702" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="7704" max="7704" width="7" customWidth="1"/>
+    <col min="7706" max="7706" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="7937" max="7937" width="43.33203125" customWidth="1"/>
+    <col min="7938" max="7938" width="12.6640625" customWidth="1"/>
+    <col min="7939" max="7939" width="19.6640625" customWidth="1"/>
+    <col min="7940" max="7941" width="19.33203125" customWidth="1"/>
+    <col min="7950" max="7950" width="10" bestFit="1" customWidth="1"/>
+    <col min="7951" max="7951" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="7954" max="7954" width="10" bestFit="1" customWidth="1"/>
+    <col min="7958" max="7958" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="7960" max="7960" width="7" customWidth="1"/>
+    <col min="7962" max="7962" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="8193" max="8193" width="43.33203125" customWidth="1"/>
+    <col min="8194" max="8194" width="12.6640625" customWidth="1"/>
+    <col min="8195" max="8195" width="19.6640625" customWidth="1"/>
+    <col min="8196" max="8197" width="19.33203125" customWidth="1"/>
+    <col min="8206" max="8206" width="10" bestFit="1" customWidth="1"/>
+    <col min="8207" max="8207" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="8210" max="8210" width="10" bestFit="1" customWidth="1"/>
+    <col min="8214" max="8214" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="8216" max="8216" width="7" customWidth="1"/>
+    <col min="8218" max="8218" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="8449" max="8449" width="43.33203125" customWidth="1"/>
+    <col min="8450" max="8450" width="12.6640625" customWidth="1"/>
+    <col min="8451" max="8451" width="19.6640625" customWidth="1"/>
+    <col min="8452" max="8453" width="19.33203125" customWidth="1"/>
+    <col min="8462" max="8462" width="10" bestFit="1" customWidth="1"/>
+    <col min="8463" max="8463" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="8466" max="8466" width="10" bestFit="1" customWidth="1"/>
+    <col min="8470" max="8470" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="8472" max="8472" width="7" customWidth="1"/>
+    <col min="8474" max="8474" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="8705" max="8705" width="43.33203125" customWidth="1"/>
+    <col min="8706" max="8706" width="12.6640625" customWidth="1"/>
+    <col min="8707" max="8707" width="19.6640625" customWidth="1"/>
+    <col min="8708" max="8709" width="19.33203125" customWidth="1"/>
+    <col min="8718" max="8718" width="10" bestFit="1" customWidth="1"/>
+    <col min="8719" max="8719" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="8722" max="8722" width="10" bestFit="1" customWidth="1"/>
+    <col min="8726" max="8726" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="8728" max="8728" width="7" customWidth="1"/>
+    <col min="8730" max="8730" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="8961" max="8961" width="43.33203125" customWidth="1"/>
+    <col min="8962" max="8962" width="12.6640625" customWidth="1"/>
+    <col min="8963" max="8963" width="19.6640625" customWidth="1"/>
+    <col min="8964" max="8965" width="19.33203125" customWidth="1"/>
+    <col min="8974" max="8974" width="10" bestFit="1" customWidth="1"/>
+    <col min="8975" max="8975" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="8978" max="8978" width="10" bestFit="1" customWidth="1"/>
+    <col min="8982" max="8982" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="8984" max="8984" width="7" customWidth="1"/>
+    <col min="8986" max="8986" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="9217" max="9217" width="43.33203125" customWidth="1"/>
+    <col min="9218" max="9218" width="12.6640625" customWidth="1"/>
+    <col min="9219" max="9219" width="19.6640625" customWidth="1"/>
+    <col min="9220" max="9221" width="19.33203125" customWidth="1"/>
+    <col min="9230" max="9230" width="10" bestFit="1" customWidth="1"/>
+    <col min="9231" max="9231" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="9234" max="9234" width="10" bestFit="1" customWidth="1"/>
+    <col min="9238" max="9238" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="9240" max="9240" width="7" customWidth="1"/>
+    <col min="9242" max="9242" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="9473" max="9473" width="43.33203125" customWidth="1"/>
+    <col min="9474" max="9474" width="12.6640625" customWidth="1"/>
+    <col min="9475" max="9475" width="19.6640625" customWidth="1"/>
+    <col min="9476" max="9477" width="19.33203125" customWidth="1"/>
+    <col min="9486" max="9486" width="10" bestFit="1" customWidth="1"/>
+    <col min="9487" max="9487" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="9490" max="9490" width="10" bestFit="1" customWidth="1"/>
+    <col min="9494" max="9494" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="9496" max="9496" width="7" customWidth="1"/>
+    <col min="9498" max="9498" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="9729" max="9729" width="43.33203125" customWidth="1"/>
+    <col min="9730" max="9730" width="12.6640625" customWidth="1"/>
+    <col min="9731" max="9731" width="19.6640625" customWidth="1"/>
+    <col min="9732" max="9733" width="19.33203125" customWidth="1"/>
+    <col min="9742" max="9742" width="10" bestFit="1" customWidth="1"/>
+    <col min="9743" max="9743" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="9746" max="9746" width="10" bestFit="1" customWidth="1"/>
+    <col min="9750" max="9750" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="9752" max="9752" width="7" customWidth="1"/>
+    <col min="9754" max="9754" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="9985" max="9985" width="43.33203125" customWidth="1"/>
+    <col min="9986" max="9986" width="12.6640625" customWidth="1"/>
+    <col min="9987" max="9987" width="19.6640625" customWidth="1"/>
+    <col min="9988" max="9989" width="19.33203125" customWidth="1"/>
+    <col min="9998" max="9998" width="10" bestFit="1" customWidth="1"/>
+    <col min="9999" max="9999" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="10002" max="10002" width="10" bestFit="1" customWidth="1"/>
+    <col min="10006" max="10006" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="10008" max="10008" width="7" customWidth="1"/>
+    <col min="10010" max="10010" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="10241" max="10241" width="43.33203125" customWidth="1"/>
+    <col min="10242" max="10242" width="12.6640625" customWidth="1"/>
+    <col min="10243" max="10243" width="19.6640625" customWidth="1"/>
+    <col min="10244" max="10245" width="19.33203125" customWidth="1"/>
+    <col min="10254" max="10254" width="10" bestFit="1" customWidth="1"/>
+    <col min="10255" max="10255" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="10258" max="10258" width="10" bestFit="1" customWidth="1"/>
+    <col min="10262" max="10262" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="10264" max="10264" width="7" customWidth="1"/>
+    <col min="10266" max="10266" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="10497" max="10497" width="43.33203125" customWidth="1"/>
+    <col min="10498" max="10498" width="12.6640625" customWidth="1"/>
+    <col min="10499" max="10499" width="19.6640625" customWidth="1"/>
+    <col min="10500" max="10501" width="19.33203125" customWidth="1"/>
+    <col min="10510" max="10510" width="10" bestFit="1" customWidth="1"/>
+    <col min="10511" max="10511" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="10514" max="10514" width="10" bestFit="1" customWidth="1"/>
+    <col min="10518" max="10518" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="10520" max="10520" width="7" customWidth="1"/>
+    <col min="10522" max="10522" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="10753" max="10753" width="43.33203125" customWidth="1"/>
+    <col min="10754" max="10754" width="12.6640625" customWidth="1"/>
+    <col min="10755" max="10755" width="19.6640625" customWidth="1"/>
+    <col min="10756" max="10757" width="19.33203125" customWidth="1"/>
+    <col min="10766" max="10766" width="10" bestFit="1" customWidth="1"/>
+    <col min="10767" max="10767" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="10770" max="10770" width="10" bestFit="1" customWidth="1"/>
+    <col min="10774" max="10774" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="10776" max="10776" width="7" customWidth="1"/>
+    <col min="10778" max="10778" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="11009" max="11009" width="43.33203125" customWidth="1"/>
+    <col min="11010" max="11010" width="12.6640625" customWidth="1"/>
+    <col min="11011" max="11011" width="19.6640625" customWidth="1"/>
+    <col min="11012" max="11013" width="19.33203125" customWidth="1"/>
+    <col min="11022" max="11022" width="10" bestFit="1" customWidth="1"/>
+    <col min="11023" max="11023" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="11026" max="11026" width="10" bestFit="1" customWidth="1"/>
+    <col min="11030" max="11030" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="11032" max="11032" width="7" customWidth="1"/>
+    <col min="11034" max="11034" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="11265" max="11265" width="43.33203125" customWidth="1"/>
+    <col min="11266" max="11266" width="12.6640625" customWidth="1"/>
+    <col min="11267" max="11267" width="19.6640625" customWidth="1"/>
+    <col min="11268" max="11269" width="19.33203125" customWidth="1"/>
+    <col min="11278" max="11278" width="10" bestFit="1" customWidth="1"/>
+    <col min="11279" max="11279" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="11282" max="11282" width="10" bestFit="1" customWidth="1"/>
+    <col min="11286" max="11286" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="11288" max="11288" width="7" customWidth="1"/>
+    <col min="11290" max="11290" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="11521" max="11521" width="43.33203125" customWidth="1"/>
+    <col min="11522" max="11522" width="12.6640625" customWidth="1"/>
+    <col min="11523" max="11523" width="19.6640625" customWidth="1"/>
+    <col min="11524" max="11525" width="19.33203125" customWidth="1"/>
+    <col min="11534" max="11534" width="10" bestFit="1" customWidth="1"/>
+    <col min="11535" max="11535" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="11538" max="11538" width="10" bestFit="1" customWidth="1"/>
+    <col min="11542" max="11542" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="11544" max="11544" width="7" customWidth="1"/>
+    <col min="11546" max="11546" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="11777" max="11777" width="43.33203125" customWidth="1"/>
+    <col min="11778" max="11778" width="12.6640625" customWidth="1"/>
+    <col min="11779" max="11779" width="19.6640625" customWidth="1"/>
+    <col min="11780" max="11781" width="19.33203125" customWidth="1"/>
+    <col min="11790" max="11790" width="10" bestFit="1" customWidth="1"/>
+    <col min="11791" max="11791" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="11794" max="11794" width="10" bestFit="1" customWidth="1"/>
+    <col min="11798" max="11798" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="11800" max="11800" width="7" customWidth="1"/>
+    <col min="11802" max="11802" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="12033" max="12033" width="43.33203125" customWidth="1"/>
+    <col min="12034" max="12034" width="12.6640625" customWidth="1"/>
+    <col min="12035" max="12035" width="19.6640625" customWidth="1"/>
+    <col min="12036" max="12037" width="19.33203125" customWidth="1"/>
+    <col min="12046" max="12046" width="10" bestFit="1" customWidth="1"/>
+    <col min="12047" max="12047" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="12050" max="12050" width="10" bestFit="1" customWidth="1"/>
+    <col min="12054" max="12054" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="12056" max="12056" width="7" customWidth="1"/>
+    <col min="12058" max="12058" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="12289" max="12289" width="43.33203125" customWidth="1"/>
+    <col min="12290" max="12290" width="12.6640625" customWidth="1"/>
+    <col min="12291" max="12291" width="19.6640625" customWidth="1"/>
+    <col min="12292" max="12293" width="19.33203125" customWidth="1"/>
+    <col min="12302" max="12302" width="10" bestFit="1" customWidth="1"/>
+    <col min="12303" max="12303" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="12306" max="12306" width="10" bestFit="1" customWidth="1"/>
+    <col min="12310" max="12310" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="12312" max="12312" width="7" customWidth="1"/>
+    <col min="12314" max="12314" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="12545" max="12545" width="43.33203125" customWidth="1"/>
+    <col min="12546" max="12546" width="12.6640625" customWidth="1"/>
+    <col min="12547" max="12547" width="19.6640625" customWidth="1"/>
+    <col min="12548" max="12549" width="19.33203125" customWidth="1"/>
+    <col min="12558" max="12558" width="10" bestFit="1" customWidth="1"/>
+    <col min="12559" max="12559" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="12562" max="12562" width="10" bestFit="1" customWidth="1"/>
+    <col min="12566" max="12566" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="12568" max="12568" width="7" customWidth="1"/>
+    <col min="12570" max="12570" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="12801" max="12801" width="43.33203125" customWidth="1"/>
+    <col min="12802" max="12802" width="12.6640625" customWidth="1"/>
+    <col min="12803" max="12803" width="19.6640625" customWidth="1"/>
+    <col min="12804" max="12805" width="19.33203125" customWidth="1"/>
+    <col min="12814" max="12814" width="10" bestFit="1" customWidth="1"/>
+    <col min="12815" max="12815" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="12818" max="12818" width="10" bestFit="1" customWidth="1"/>
+    <col min="12822" max="12822" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="12824" max="12824" width="7" customWidth="1"/>
+    <col min="12826" max="12826" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="13057" max="13057" width="43.33203125" customWidth="1"/>
+    <col min="13058" max="13058" width="12.6640625" customWidth="1"/>
+    <col min="13059" max="13059" width="19.6640625" customWidth="1"/>
+    <col min="13060" max="13061" width="19.33203125" customWidth="1"/>
+    <col min="13070" max="13070" width="10" bestFit="1" customWidth="1"/>
+    <col min="13071" max="13071" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="13074" max="13074" width="10" bestFit="1" customWidth="1"/>
+    <col min="13078" max="13078" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="13080" max="13080" width="7" customWidth="1"/>
+    <col min="13082" max="13082" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="13313" max="13313" width="43.33203125" customWidth="1"/>
+    <col min="13314" max="13314" width="12.6640625" customWidth="1"/>
+    <col min="13315" max="13315" width="19.6640625" customWidth="1"/>
+    <col min="13316" max="13317" width="19.33203125" customWidth="1"/>
+    <col min="13326" max="13326" width="10" bestFit="1" customWidth="1"/>
+    <col min="13327" max="13327" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="13330" max="13330" width="10" bestFit="1" customWidth="1"/>
+    <col min="13334" max="13334" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="13336" max="13336" width="7" customWidth="1"/>
+    <col min="13338" max="13338" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="13569" max="13569" width="43.33203125" customWidth="1"/>
+    <col min="13570" max="13570" width="12.6640625" customWidth="1"/>
+    <col min="13571" max="13571" width="19.6640625" customWidth="1"/>
+    <col min="13572" max="13573" width="19.33203125" customWidth="1"/>
+    <col min="13582" max="13582" width="10" bestFit="1" customWidth="1"/>
+    <col min="13583" max="13583" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="13586" max="13586" width="10" bestFit="1" customWidth="1"/>
+    <col min="13590" max="13590" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="13592" max="13592" width="7" customWidth="1"/>
+    <col min="13594" max="13594" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="13825" max="13825" width="43.33203125" customWidth="1"/>
+    <col min="13826" max="13826" width="12.6640625" customWidth="1"/>
+    <col min="13827" max="13827" width="19.6640625" customWidth="1"/>
+    <col min="13828" max="13829" width="19.33203125" customWidth="1"/>
+    <col min="13838" max="13838" width="10" bestFit="1" customWidth="1"/>
+    <col min="13839" max="13839" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="13842" max="13842" width="10" bestFit="1" customWidth="1"/>
+    <col min="13846" max="13846" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="13848" max="13848" width="7" customWidth="1"/>
+    <col min="13850" max="13850" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="14081" max="14081" width="43.33203125" customWidth="1"/>
+    <col min="14082" max="14082" width="12.6640625" customWidth="1"/>
+    <col min="14083" max="14083" width="19.6640625" customWidth="1"/>
+    <col min="14084" max="14085" width="19.33203125" customWidth="1"/>
+    <col min="14094" max="14094" width="10" bestFit="1" customWidth="1"/>
+    <col min="14095" max="14095" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="14098" max="14098" width="10" bestFit="1" customWidth="1"/>
+    <col min="14102" max="14102" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="14104" max="14104" width="7" customWidth="1"/>
+    <col min="14106" max="14106" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="14337" max="14337" width="43.33203125" customWidth="1"/>
+    <col min="14338" max="14338" width="12.6640625" customWidth="1"/>
+    <col min="14339" max="14339" width="19.6640625" customWidth="1"/>
+    <col min="14340" max="14341" width="19.33203125" customWidth="1"/>
+    <col min="14350" max="14350" width="10" bestFit="1" customWidth="1"/>
+    <col min="14351" max="14351" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="14354" max="14354" width="10" bestFit="1" customWidth="1"/>
+    <col min="14358" max="14358" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="14360" max="14360" width="7" customWidth="1"/>
+    <col min="14362" max="14362" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="14593" max="14593" width="43.33203125" customWidth="1"/>
+    <col min="14594" max="14594" width="12.6640625" customWidth="1"/>
+    <col min="14595" max="14595" width="19.6640625" customWidth="1"/>
+    <col min="14596" max="14597" width="19.33203125" customWidth="1"/>
+    <col min="14606" max="14606" width="10" bestFit="1" customWidth="1"/>
+    <col min="14607" max="14607" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="14610" max="14610" width="10" bestFit="1" customWidth="1"/>
+    <col min="14614" max="14614" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="14616" max="14616" width="7" customWidth="1"/>
+    <col min="14618" max="14618" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="14849" max="14849" width="43.33203125" customWidth="1"/>
+    <col min="14850" max="14850" width="12.6640625" customWidth="1"/>
+    <col min="14851" max="14851" width="19.6640625" customWidth="1"/>
+    <col min="14852" max="14853" width="19.33203125" customWidth="1"/>
+    <col min="14862" max="14862" width="10" bestFit="1" customWidth="1"/>
+    <col min="14863" max="14863" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="14866" max="14866" width="10" bestFit="1" customWidth="1"/>
+    <col min="14870" max="14870" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="14872" max="14872" width="7" customWidth="1"/>
+    <col min="14874" max="14874" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="15105" max="15105" width="43.33203125" customWidth="1"/>
+    <col min="15106" max="15106" width="12.6640625" customWidth="1"/>
+    <col min="15107" max="15107" width="19.6640625" customWidth="1"/>
+    <col min="15108" max="15109" width="19.33203125" customWidth="1"/>
+    <col min="15118" max="15118" width="10" bestFit="1" customWidth="1"/>
+    <col min="15119" max="15119" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="15122" max="15122" width="10" bestFit="1" customWidth="1"/>
+    <col min="15126" max="15126" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="15128" max="15128" width="7" customWidth="1"/>
+    <col min="15130" max="15130" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="15361" max="15361" width="43.33203125" customWidth="1"/>
+    <col min="15362" max="15362" width="12.6640625" customWidth="1"/>
+    <col min="15363" max="15363" width="19.6640625" customWidth="1"/>
+    <col min="15364" max="15365" width="19.33203125" customWidth="1"/>
+    <col min="15374" max="15374" width="10" bestFit="1" customWidth="1"/>
+    <col min="15375" max="15375" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="15378" max="15378" width="10" bestFit="1" customWidth="1"/>
+    <col min="15382" max="15382" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="15384" max="15384" width="7" customWidth="1"/>
+    <col min="15386" max="15386" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="15617" max="15617" width="43.33203125" customWidth="1"/>
+    <col min="15618" max="15618" width="12.6640625" customWidth="1"/>
+    <col min="15619" max="15619" width="19.6640625" customWidth="1"/>
+    <col min="15620" max="15621" width="19.33203125" customWidth="1"/>
+    <col min="15630" max="15630" width="10" bestFit="1" customWidth="1"/>
+    <col min="15631" max="15631" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="15634" max="15634" width="10" bestFit="1" customWidth="1"/>
+    <col min="15638" max="15638" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="15640" max="15640" width="7" customWidth="1"/>
+    <col min="15642" max="15642" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="15873" max="15873" width="43.33203125" customWidth="1"/>
+    <col min="15874" max="15874" width="12.6640625" customWidth="1"/>
+    <col min="15875" max="15875" width="19.6640625" customWidth="1"/>
+    <col min="15876" max="15877" width="19.33203125" customWidth="1"/>
+    <col min="15886" max="15886" width="10" bestFit="1" customWidth="1"/>
+    <col min="15887" max="15887" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="15890" max="15890" width="10" bestFit="1" customWidth="1"/>
+    <col min="15894" max="15894" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="15896" max="15896" width="7" customWidth="1"/>
+    <col min="15898" max="15898" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="16129" max="16129" width="43.33203125" customWidth="1"/>
+    <col min="16130" max="16130" width="12.6640625" customWidth="1"/>
+    <col min="16131" max="16131" width="19.6640625" customWidth="1"/>
+    <col min="16132" max="16133" width="19.33203125" customWidth="1"/>
+    <col min="16142" max="16142" width="10" bestFit="1" customWidth="1"/>
+    <col min="16143" max="16143" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="16146" max="16146" width="10" bestFit="1" customWidth="1"/>
+    <col min="16150" max="16150" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="16152" max="16152" width="7" customWidth="1"/>
+    <col min="16154" max="16154" width="17.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3612,188 +4321,639 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="O1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="Z1" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>112</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="C2" s="2">
+      <c r="C2" s="14" t="s">
+        <v>159</v>
+      </c>
+      <c r="D2" s="2">
         <v>100</v>
       </c>
-      <c r="D2" s="2">
+      <c r="E2" s="2">
         <v>12000</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="F2" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="G2" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="G2" s="2">
-        <v>0</v>
-      </c>
       <c r="H2" s="2">
+        <v>0</v>
+      </c>
+      <c r="I2" s="2">
         <f>2771.2/0.962</f>
         <v>2880.6652806652805</v>
       </c>
-      <c r="I2" s="2">
-        <v>1</v>
-      </c>
       <c r="J2" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K2" s="2">
+        <v>0</v>
+      </c>
+      <c r="L2" s="2">
         <f>-284.2/0.962</f>
         <v>-295.42619542619542</v>
       </c>
-      <c r="L2" s="2">
+      <c r="M2" s="2">
         <v>25</v>
       </c>
-      <c r="M2" s="2">
-        <v>1</v>
-      </c>
-      <c r="N2" s="2">
+      <c r="N2" s="14">
+        <v>25</v>
+      </c>
+      <c r="O2" s="2">
+        <v>1</v>
+      </c>
+      <c r="P2" s="2">
         <v>6</v>
       </c>
-      <c r="O2" s="2" t="s">
+      <c r="Q2" s="14">
+        <v>0</v>
+      </c>
+      <c r="R2" s="14">
+        <v>0</v>
+      </c>
+      <c r="S2" s="14">
+        <v>70</v>
+      </c>
+      <c r="T2" s="14">
+        <v>90</v>
+      </c>
+      <c r="U2" s="14">
+        <v>0</v>
+      </c>
+      <c r="V2" s="14">
+        <v>997</v>
+      </c>
+      <c r="W2" s="14">
+        <v>4.1900000000000004</v>
+      </c>
+      <c r="X2" s="14">
+        <v>0.98</v>
+      </c>
+      <c r="Y2" s="14">
+        <v>0.96</v>
+      </c>
+      <c r="Z2" s="2" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>112</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="C3" s="2">
+      <c r="C3" s="14" t="s">
+        <v>159</v>
+      </c>
+      <c r="D3" s="2">
         <v>12000</v>
       </c>
-      <c r="D3" s="5">
+      <c r="E3" s="5">
         <v>10000000000</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="F3" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="G3" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="G3" s="2">
-        <v>0</v>
-      </c>
       <c r="H3" s="2">
+        <v>0</v>
+      </c>
+      <c r="I3" s="2">
         <f>2771.2/0.962</f>
         <v>2880.6652806652805</v>
       </c>
-      <c r="I3" s="2">
-        <v>1</v>
-      </c>
       <c r="J3" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K3" s="2">
+        <v>0</v>
+      </c>
+      <c r="L3" s="2">
         <f>-284.2/0.962</f>
         <v>-295.42619542619542</v>
       </c>
-      <c r="L3" s="2">
+      <c r="M3" s="2">
         <v>25</v>
       </c>
-      <c r="M3" s="2">
-        <v>1</v>
-      </c>
-      <c r="N3" s="2">
+      <c r="N3" s="14">
+        <v>25</v>
+      </c>
+      <c r="O3" s="2">
+        <v>1</v>
+      </c>
+      <c r="P3" s="2">
         <v>6</v>
       </c>
-      <c r="O3" s="2" t="s">
+      <c r="Q3" s="14">
+        <v>0</v>
+      </c>
+      <c r="R3" s="14">
+        <v>0</v>
+      </c>
+      <c r="S3" s="14">
+        <v>70</v>
+      </c>
+      <c r="T3" s="14">
+        <v>90</v>
+      </c>
+      <c r="U3" s="14">
+        <v>0</v>
+      </c>
+      <c r="V3" s="14">
+        <v>997</v>
+      </c>
+      <c r="W3" s="14">
+        <v>4.1900000000000004</v>
+      </c>
+      <c r="X3" s="14">
+        <v>0.98</v>
+      </c>
+      <c r="Y3" s="14">
+        <v>0.96</v>
+      </c>
+      <c r="Z3" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="B4" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="C4" s="2">
-        <v>0</v>
-      </c>
-      <c r="D4" s="5">
+      <c r="C4" s="14" t="s">
+        <v>161</v>
+      </c>
+      <c r="D4" s="14">
+        <v>0</v>
+      </c>
+      <c r="E4" s="15">
         <v>10000000000</v>
       </c>
-      <c r="E4" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="F4" s="2" t="s">
+      <c r="F4" s="14" t="s">
+        <v>162</v>
+      </c>
+      <c r="G4" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="G4" s="2">
-        <v>0</v>
-      </c>
-      <c r="H4" s="2">
-        <f>931/1.331</f>
-        <v>699.47407963936894</v>
-      </c>
-      <c r="I4" s="2">
-        <v>1</v>
-      </c>
-      <c r="J4" s="2">
-        <v>0</v>
-      </c>
-      <c r="K4" s="2">
-        <v>0</v>
-      </c>
-      <c r="L4" s="2">
+      <c r="H4" s="14">
+        <v>0</v>
+      </c>
+      <c r="I4" s="14">
+        <v>108</v>
+      </c>
+      <c r="J4" s="14">
+        <v>1</v>
+      </c>
+      <c r="K4" s="14">
+        <v>0</v>
+      </c>
+      <c r="L4" s="14">
+        <v>0</v>
+      </c>
+      <c r="M4" s="14">
         <v>25</v>
       </c>
-      <c r="M4" s="2">
-        <v>1</v>
-      </c>
-      <c r="N4" s="2">
+      <c r="N4" s="14">
+        <v>25</v>
+      </c>
+      <c r="O4" s="14">
+        <v>2</v>
+      </c>
+      <c r="P4" s="14">
         <v>6</v>
       </c>
-      <c r="O4" s="2" t="s">
+      <c r="Q4" s="14">
+        <v>0</v>
+      </c>
+      <c r="R4" s="14">
+        <v>0</v>
+      </c>
+      <c r="S4" s="14">
+        <v>4</v>
+      </c>
+      <c r="T4" s="14">
+        <v>13</v>
+      </c>
+      <c r="U4" s="14">
+        <v>0</v>
+      </c>
+      <c r="V4" s="14">
+        <v>997</v>
+      </c>
+      <c r="W4" s="14">
+        <v>4.1900000000000004</v>
+      </c>
+      <c r="X4" s="14">
+        <v>0.98</v>
+      </c>
+      <c r="Y4" s="14">
+        <v>0.96</v>
+      </c>
+      <c r="Z4" s="14" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="5" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="C5" s="14" t="s">
+        <v>161</v>
+      </c>
+      <c r="D5" s="14">
+        <v>0</v>
+      </c>
+      <c r="E5" s="15">
+        <v>10000000000</v>
+      </c>
+      <c r="F5" s="14" t="s">
+        <v>162</v>
+      </c>
+      <c r="G5" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="H5" s="14">
+        <v>0</v>
+      </c>
+      <c r="I5" s="14">
+        <v>117.9</v>
+      </c>
+      <c r="J5" s="14">
+        <v>1</v>
+      </c>
+      <c r="K5" s="14">
+        <v>0</v>
+      </c>
+      <c r="L5" s="14">
+        <v>0</v>
+      </c>
+      <c r="M5" s="14">
+        <v>25</v>
+      </c>
+      <c r="N5" s="14">
+        <v>25</v>
+      </c>
+      <c r="O5" s="14">
+        <v>2</v>
+      </c>
+      <c r="P5" s="14">
+        <v>6</v>
+      </c>
+      <c r="Q5" s="14">
+        <v>4.8</v>
+      </c>
+      <c r="R5" s="14">
+        <v>0</v>
+      </c>
+      <c r="S5" s="14">
+        <v>-0.5</v>
+      </c>
+      <c r="T5" s="14">
+        <v>0.5</v>
+      </c>
+      <c r="U5" s="14">
+        <v>334</v>
+      </c>
+      <c r="V5" s="14">
+        <v>917</v>
+      </c>
+      <c r="W5" s="14">
+        <v>2.11</v>
+      </c>
+      <c r="X5" s="14">
+        <v>0.98</v>
+      </c>
+      <c r="Y5" s="14">
+        <v>0.96</v>
+      </c>
+      <c r="Z5" s="14" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="6" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="C6" s="14" t="s">
+        <v>161</v>
+      </c>
+      <c r="D6" s="14">
+        <v>0</v>
+      </c>
+      <c r="E6" s="15">
+        <v>10000000000</v>
+      </c>
+      <c r="F6" s="14" t="s">
+        <v>162</v>
+      </c>
+      <c r="G6" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="H6" s="14">
+        <v>0</v>
+      </c>
+      <c r="I6" s="14">
+        <v>117.9</v>
+      </c>
+      <c r="J6" s="14">
+        <v>1</v>
+      </c>
+      <c r="K6" s="14">
+        <v>0</v>
+      </c>
+      <c r="L6" s="14">
+        <v>0</v>
+      </c>
+      <c r="M6" s="14">
+        <v>25</v>
+      </c>
+      <c r="N6" s="14">
+        <v>7</v>
+      </c>
+      <c r="O6" s="14">
+        <v>2</v>
+      </c>
+      <c r="P6" s="14">
+        <v>6</v>
+      </c>
+      <c r="Q6" s="14">
+        <v>4.8</v>
+      </c>
+      <c r="R6" s="14">
+        <v>4</v>
+      </c>
+      <c r="S6" s="14">
+        <v>3.5</v>
+      </c>
+      <c r="T6" s="14">
+        <v>4.5</v>
+      </c>
+      <c r="U6" s="14">
+        <v>234</v>
+      </c>
+      <c r="V6" s="14">
+        <v>1600</v>
+      </c>
+      <c r="W6" s="14">
+        <v>2</v>
+      </c>
+      <c r="X6" s="14">
+        <v>0.98</v>
+      </c>
+      <c r="Y6" s="14">
+        <v>0.96</v>
+      </c>
+      <c r="Z6" s="14" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="7" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="C7" s="14" t="s">
+        <v>161</v>
+      </c>
+      <c r="D7" s="14">
+        <v>0</v>
+      </c>
+      <c r="E7" s="15">
+        <v>10000000000</v>
+      </c>
+      <c r="F7" s="14" t="s">
+        <v>162</v>
+      </c>
+      <c r="G7" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="H7" s="14">
+        <v>0</v>
+      </c>
+      <c r="I7" s="14">
+        <v>156.30000000000001</v>
+      </c>
+      <c r="J7" s="14">
+        <v>1</v>
+      </c>
+      <c r="K7" s="14">
+        <v>0</v>
+      </c>
+      <c r="L7" s="14">
+        <v>0</v>
+      </c>
+      <c r="M7" s="14">
+        <v>25</v>
+      </c>
+      <c r="N7" s="14">
+        <v>7</v>
+      </c>
+      <c r="O7" s="14">
+        <v>2</v>
+      </c>
+      <c r="P7" s="14">
+        <v>6</v>
+      </c>
+      <c r="Q7" s="14">
+        <v>27.3</v>
+      </c>
+      <c r="R7" s="14">
+        <v>5.4</v>
+      </c>
+      <c r="S7" s="14">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="T7" s="14">
+        <v>5.9</v>
+      </c>
+      <c r="U7" s="14">
+        <v>105</v>
+      </c>
+      <c r="V7" s="14">
+        <v>1125</v>
+      </c>
+      <c r="W7" s="14">
+        <v>2.09</v>
+      </c>
+      <c r="X7" s="14">
+        <v>0.98</v>
+      </c>
+      <c r="Y7" s="14">
+        <v>0.96</v>
+      </c>
+      <c r="Z7" s="14" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="8" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="C8" s="14" t="s">
+        <v>161</v>
+      </c>
+      <c r="D8" s="14">
+        <v>0</v>
+      </c>
+      <c r="E8" s="15">
+        <v>10000000000</v>
+      </c>
+      <c r="F8" s="14" t="s">
+        <v>162</v>
+      </c>
+      <c r="G8" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="H8" s="14">
+        <v>0</v>
+      </c>
+      <c r="I8" s="14">
+        <v>141.5</v>
+      </c>
+      <c r="J8" s="14">
+        <v>1</v>
+      </c>
+      <c r="K8" s="14">
+        <v>0</v>
+      </c>
+      <c r="L8" s="14">
+        <v>0</v>
+      </c>
+      <c r="M8" s="14">
+        <v>25</v>
+      </c>
+      <c r="N8" s="14">
+        <v>7</v>
+      </c>
+      <c r="O8" s="14">
+        <v>2</v>
+      </c>
+      <c r="P8" s="14">
+        <v>6</v>
+      </c>
+      <c r="Q8" s="14">
+        <v>19.7</v>
+      </c>
+      <c r="R8" s="14">
+        <v>5</v>
+      </c>
+      <c r="S8" s="14">
+        <v>4.5</v>
+      </c>
+      <c r="T8" s="14">
+        <v>5.5</v>
+      </c>
+      <c r="U8" s="14">
+        <v>230</v>
+      </c>
+      <c r="V8" s="14">
+        <v>760</v>
+      </c>
+      <c r="W8" s="14">
+        <v>2.14</v>
+      </c>
+      <c r="X8" s="14">
+        <v>0.98</v>
+      </c>
+      <c r="Y8" s="14">
+        <v>0.96</v>
+      </c>
+      <c r="Z8" s="14" t="s">
         <v>115</v>
       </c>
     </row>
@@ -3809,20 +4969,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AG3"/>
   <sheetViews>
-    <sheetView topLeftCell="O1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="16.7265625" customWidth="1"/>
+    <col min="1" max="1" width="16.6640625" customWidth="1"/>
     <col min="4" max="4" width="42" customWidth="1"/>
-    <col min="21" max="21" width="14.26953125" customWidth="1"/>
-    <col min="22" max="22" width="12.7265625" customWidth="1"/>
-    <col min="23" max="23" width="10.54296875" customWidth="1"/>
+    <col min="21" max="21" width="14.33203125" customWidth="1"/>
+    <col min="22" max="22" width="12.6640625" customWidth="1"/>
+    <col min="23" max="23" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3923,7 +5083,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>53</v>
       </c>
@@ -4028,7 +5188,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>57</v>
       </c>
@@ -4145,19 +5305,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:O2"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="18.453125" customWidth="1"/>
-    <col min="3" max="3" width="9.453125" customWidth="1"/>
-    <col min="4" max="5" width="10.453125" customWidth="1"/>
-    <col min="8" max="8" width="10.54296875" customWidth="1"/>
+    <col min="1" max="1" width="18.5" customWidth="1"/>
+    <col min="3" max="3" width="9.5" customWidth="1"/>
+    <col min="4" max="5" width="10.5" customWidth="1"/>
+    <col min="8" max="8" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4204,7 +5364,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>60</v>
       </c>
@@ -4268,16 +5428,16 @@
       <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="19.7265625" customWidth="1"/>
-    <col min="2" max="2" width="13.26953125" customWidth="1"/>
-    <col min="3" max="3" width="17.7265625" customWidth="1"/>
-    <col min="4" max="5" width="16.453125" customWidth="1"/>
-    <col min="12" max="12" width="22.7265625" customWidth="1"/>
+    <col min="1" max="1" width="19.6640625" customWidth="1"/>
+    <col min="2" max="2" width="13.33203125" customWidth="1"/>
+    <col min="3" max="3" width="17.6640625" customWidth="1"/>
+    <col min="4" max="5" width="16.5" customWidth="1"/>
+    <col min="12" max="12" width="22.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4324,7 +5484,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>62</v>
       </c>
@@ -4371,7 +5531,7 @@
       </c>
       <c r="O2" s="2"/>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>62</v>
       </c>
@@ -4418,7 +5578,7 @@
       </c>
       <c r="O3" s="2"/>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>62</v>
       </c>
@@ -4481,15 +5641,15 @@
       <selection activeCell="A2" sqref="A2:O3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="29.26953125" customWidth="1"/>
+    <col min="1" max="1" width="29.33203125" customWidth="1"/>
     <col min="3" max="3" width="17" customWidth="1"/>
-    <col min="4" max="5" width="17.7265625" customWidth="1"/>
-    <col min="8" max="8" width="10.54296875" customWidth="1"/>
+    <col min="4" max="5" width="17.6640625" customWidth="1"/>
+    <col min="8" max="8" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4536,7 +5696,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>64</v>
       </c>
@@ -4581,7 +5741,7 @@
       </c>
       <c r="O2" s="2"/>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3" s="12" t="s">
         <v>64</v>
       </c>
@@ -4642,16 +5802,16 @@
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="34.54296875" customWidth="1"/>
-    <col min="3" max="3" width="16.453125" customWidth="1"/>
-    <col min="4" max="5" width="15.54296875" customWidth="1"/>
+    <col min="1" max="1" width="34.5" customWidth="1"/>
+    <col min="3" max="3" width="16.5" customWidth="1"/>
+    <col min="4" max="5" width="15.5" customWidth="1"/>
     <col min="6" max="6" width="14" customWidth="1"/>
-    <col min="12" max="12" width="17.7265625" customWidth="1"/>
+    <col min="12" max="12" width="17.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4698,7 +5858,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>67</v>
       </c>
@@ -4744,7 +5904,7 @@
       </c>
       <c r="O2" s="2"/>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>67</v>
       </c>
@@ -4808,14 +5968,14 @@
       <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="28" customWidth="1"/>
-    <col min="3" max="5" width="9.26953125" customWidth="1"/>
-    <col min="15" max="15" width="13.7265625" customWidth="1"/>
+    <col min="3" max="5" width="9.33203125" customWidth="1"/>
+    <col min="15" max="15" width="13.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4862,7 +6022,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>70</v>
       </c>
@@ -4920,62 +6080,62 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:M3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="I22" sqref="I22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>129</v>
+      </c>
+      <c r="B1" t="s">
         <v>130</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>131</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>132</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>133</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>134</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>135</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>136</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>137</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>138</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>139</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>140</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>141</v>
       </c>
-      <c r="M1" t="s">
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
+      <c r="B2" t="s">
         <v>143</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>144</v>
-      </c>
-      <c r="C2" t="s">
-        <v>145</v>
       </c>
       <c r="D2">
         <v>0.33018832999999997</v>
@@ -5005,18 +6165,18 @@
         <v>5.2346000000000001E-4</v>
       </c>
       <c r="M2" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
         <v>146</v>
       </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
+      <c r="B3" t="s">
+        <v>143</v>
+      </c>
+      <c r="C3" t="s">
         <v>147</v>
-      </c>
-      <c r="B3" t="s">
-        <v>144</v>
-      </c>
-      <c r="C3" t="s">
-        <v>148</v>
       </c>
       <c r="D3">
         <v>0.17149273000000001</v>
@@ -5046,7 +6206,7 @@
         <v>6.3139000000000001E-4</v>
       </c>
       <c r="M3" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
   </sheetData>
@@ -5062,15 +6222,15 @@
       <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="29.7265625" customWidth="1"/>
-    <col min="4" max="4" width="17.26953125" customWidth="1"/>
+    <col min="1" max="1" width="29.6640625" customWidth="1"/>
+    <col min="4" max="4" width="17.33203125" customWidth="1"/>
     <col min="5" max="6" width="24" customWidth="1"/>
-    <col min="16" max="16" width="33.26953125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="33.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -5078,7 +6238,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>3</v>
@@ -5120,7 +6280,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>72</v>
       </c>
@@ -5167,10 +6327,10 @@
         <v>5</v>
       </c>
       <c r="P2" s="2" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.35">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>74</v>
       </c>
@@ -5222,7 +6382,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:16" s="12" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:16" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>74</v>
       </c>
@@ -5272,10 +6432,10 @@
         <v>25</v>
       </c>
     </row>
-    <row r="23" spans="11:11" x14ac:dyDescent="0.35">
+    <row r="23" spans="11:11" x14ac:dyDescent="0.2">
       <c r="K23" s="13"/>
     </row>
-    <row r="25" spans="11:11" x14ac:dyDescent="0.35">
+    <row r="25" spans="11:11" x14ac:dyDescent="0.2">
       <c r="K25" s="13"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
temporarily revert changes to VCC
Reverting changes to vapour compression chillers script and database for the unit-tests to pass.
1. reverting change to the CONVERSION.xls database (old) that held parameters relating to the faulty part-load efficiency model.
2. reverting changes to the old VCC-class description that fetched these parameters from the old database.
</commit_message>
<xml_diff>
--- a/cea/databases/CH/components/CONVERSION.xlsx
+++ b/cea/databases/CH/components/CONVERSION.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mathiasniffeler/Documents/GitHub/CityEnergyAnalyst/cea/databases/CH/components/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mathiasniffeler/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9460BB3D-DA27-394A-80EA-3B4AEDFC16A1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{328E75CE-5E35-F34B-8CD4-F5CE4381CBA1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="10740" tabRatio="993" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="9300" windowWidth="38400" windowHeight="10740" tabRatio="993" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PV" sheetId="1" r:id="rId1"/>
@@ -20,14 +20,15 @@
     <sheet name="Furnace" sheetId="5" r:id="rId5"/>
     <sheet name="FC" sheetId="6" r:id="rId6"/>
     <sheet name="CCGT" sheetId="7" r:id="rId7"/>
-    <sheet name="Chiller" sheetId="8" r:id="rId8"/>
-    <sheet name="Absorption_chiller" sheetId="9" r:id="rId9"/>
-    <sheet name="CT" sheetId="10" r:id="rId10"/>
-    <sheet name="HEX" sheetId="11" r:id="rId11"/>
-    <sheet name="BH" sheetId="12" r:id="rId12"/>
-    <sheet name="HP" sheetId="13" r:id="rId13"/>
-    <sheet name="Pump" sheetId="15" r:id="rId14"/>
-    <sheet name="TES" sheetId="14" r:id="rId15"/>
+    <sheet name="Chiller_configuration" sheetId="16" r:id="rId8"/>
+    <sheet name="Chiller" sheetId="8" r:id="rId9"/>
+    <sheet name="Absorption_chiller" sheetId="9" r:id="rId10"/>
+    <sheet name="CT" sheetId="10" r:id="rId11"/>
+    <sheet name="HEX" sheetId="11" r:id="rId12"/>
+    <sheet name="BH" sheetId="12" r:id="rId13"/>
+    <sheet name="HP" sheetId="13" r:id="rId14"/>
+    <sheet name="Pump" sheetId="15" r:id="rId15"/>
+    <sheet name="TES" sheetId="14" r:id="rId16"/>
   </sheets>
   <definedNames>
     <definedName name="__xlfn_AGGREGATE">#N/A</definedName>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="539" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="560" uniqueCount="171">
   <si>
     <t>Description</t>
   </si>
@@ -425,6 +426,63 @@
   </si>
   <si>
     <t xml:space="preserve">Fit based on RESCUE WP 2.4. Figure 18 </t>
+  </si>
+  <si>
+    <t>CODE</t>
+  </si>
+  <si>
+    <t>SOURCE</t>
+  </si>
+  <si>
+    <t>COMPRESSOR</t>
+  </si>
+  <si>
+    <t>plf_a</t>
+  </si>
+  <si>
+    <t>plf_b</t>
+  </si>
+  <si>
+    <t>plf_c</t>
+  </si>
+  <si>
+    <t>q_a</t>
+  </si>
+  <si>
+    <t>q_b</t>
+  </si>
+  <si>
+    <t>q_c</t>
+  </si>
+  <si>
+    <t>q_d</t>
+  </si>
+  <si>
+    <t>q_e</t>
+  </si>
+  <si>
+    <t>q_f</t>
+  </si>
+  <si>
+    <t>REFERENCE</t>
+  </si>
+  <si>
+    <t>CH_T0</t>
+  </si>
+  <si>
+    <t>WATER</t>
+  </si>
+  <si>
+    <t>SCREW</t>
+  </si>
+  <si>
+    <t>https://comnet.org/index.php/382-chillers</t>
+  </si>
+  <si>
+    <t>CH_T1</t>
+  </si>
+  <si>
+    <t>CENTRIFUGAL</t>
   </si>
   <si>
     <t>G_VALUE</t>
@@ -1975,6 +2033,588 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
+  <dimension ref="A1:Z7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J29" sqref="J29"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="27.6640625" customWidth="1"/>
+    <col min="5" max="5" width="9.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="2" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="D2" s="2">
+        <v>0</v>
+      </c>
+      <c r="E2" s="2">
+        <v>51150</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="H2" s="2">
+        <v>0</v>
+      </c>
+      <c r="I2" s="2">
+        <v>0.4395</v>
+      </c>
+      <c r="J2" s="2">
+        <v>1</v>
+      </c>
+      <c r="K2" s="2">
+        <v>0</v>
+      </c>
+      <c r="L2" s="2">
+        <v>0</v>
+      </c>
+      <c r="M2" s="2">
+        <v>25</v>
+      </c>
+      <c r="N2" s="2">
+        <v>5</v>
+      </c>
+      <c r="O2" s="2">
+        <v>5</v>
+      </c>
+      <c r="P2" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q2" s="2">
+        <v>0.42</v>
+      </c>
+      <c r="R2" s="2">
+        <v>0.9</v>
+      </c>
+      <c r="S2" s="2">
+        <v>0.53</v>
+      </c>
+      <c r="T2" s="2">
+        <v>-2.5</v>
+      </c>
+      <c r="U2" s="2">
+        <v>-2.5</v>
+      </c>
+      <c r="V2" s="2">
+        <v>1.8</v>
+      </c>
+      <c r="W2" s="2">
+        <v>-2.1</v>
+      </c>
+      <c r="X2" s="2">
+        <v>1.5</v>
+      </c>
+      <c r="Y2" s="2">
+        <v>0.72199999999999998</v>
+      </c>
+      <c r="Z2" s="2">
+        <v>0.33300000000000002</v>
+      </c>
+    </row>
+    <row r="3" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="D3" s="2">
+        <v>51150</v>
+      </c>
+      <c r="E3" s="5">
+        <v>1176000</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="H3" s="2">
+        <v>0</v>
+      </c>
+      <c r="I3" s="2">
+        <v>0.4395</v>
+      </c>
+      <c r="J3" s="2">
+        <v>1</v>
+      </c>
+      <c r="K3" s="2">
+        <v>0</v>
+      </c>
+      <c r="L3" s="2">
+        <v>0</v>
+      </c>
+      <c r="M3" s="2">
+        <v>25</v>
+      </c>
+      <c r="N3" s="2">
+        <v>5</v>
+      </c>
+      <c r="O3" s="2">
+        <v>5</v>
+      </c>
+      <c r="P3" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q3" s="2">
+        <v>68.12</v>
+      </c>
+      <c r="R3" s="2">
+        <v>-3281.1</v>
+      </c>
+      <c r="S3" s="2">
+        <v>88.05</v>
+      </c>
+      <c r="T3" s="2">
+        <v>-4216.1000000000004</v>
+      </c>
+      <c r="U3" s="2">
+        <v>-1.45</v>
+      </c>
+      <c r="V3" s="2">
+        <v>1.75</v>
+      </c>
+      <c r="W3" s="2">
+        <v>-1.45</v>
+      </c>
+      <c r="X3" s="2">
+        <v>1.75</v>
+      </c>
+      <c r="Y3" s="2">
+        <v>81</v>
+      </c>
+      <c r="Z3" s="2">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="4" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="D4" s="2">
+        <v>0</v>
+      </c>
+      <c r="E4" s="2">
+        <v>58150</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="H4" s="2">
+        <v>0</v>
+      </c>
+      <c r="I4" s="2">
+        <v>0.52969999999999995</v>
+      </c>
+      <c r="J4" s="2">
+        <v>1</v>
+      </c>
+      <c r="K4" s="2">
+        <v>0</v>
+      </c>
+      <c r="L4" s="2">
+        <v>0</v>
+      </c>
+      <c r="M4" s="2">
+        <v>25</v>
+      </c>
+      <c r="N4" s="2">
+        <v>5</v>
+      </c>
+      <c r="O4" s="2">
+        <v>5</v>
+      </c>
+      <c r="P4" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q4" s="2">
+        <v>0.42</v>
+      </c>
+      <c r="R4" s="2">
+        <v>0.9</v>
+      </c>
+      <c r="S4" s="2">
+        <v>0.53</v>
+      </c>
+      <c r="T4" s="2">
+        <v>-2.5</v>
+      </c>
+      <c r="U4" s="2">
+        <v>-2.5</v>
+      </c>
+      <c r="V4" s="2">
+        <v>1.8</v>
+      </c>
+      <c r="W4" s="2">
+        <v>-2.1</v>
+      </c>
+      <c r="X4" s="2">
+        <v>1.5</v>
+      </c>
+      <c r="Y4" s="2">
+        <v>0.72199999999999998</v>
+      </c>
+      <c r="Z4" s="2">
+        <v>0.33300000000000002</v>
+      </c>
+    </row>
+    <row r="5" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="D5" s="2">
+        <v>58150</v>
+      </c>
+      <c r="E5" s="5">
+        <v>1337450</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="H5" s="2">
+        <v>0</v>
+      </c>
+      <c r="I5" s="2">
+        <v>0.52969999999999995</v>
+      </c>
+      <c r="J5" s="2">
+        <v>1</v>
+      </c>
+      <c r="K5" s="2">
+        <v>0</v>
+      </c>
+      <c r="L5" s="2">
+        <v>0</v>
+      </c>
+      <c r="M5" s="2">
+        <v>25</v>
+      </c>
+      <c r="N5" s="2">
+        <v>5</v>
+      </c>
+      <c r="O5" s="2">
+        <v>5</v>
+      </c>
+      <c r="P5" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q5" s="2">
+        <v>18.100000000000001</v>
+      </c>
+      <c r="R5" s="2">
+        <v>-1350.5</v>
+      </c>
+      <c r="S5" s="2">
+        <v>12.54</v>
+      </c>
+      <c r="T5" s="2">
+        <v>-917.3</v>
+      </c>
+      <c r="U5" s="2">
+        <v>-2.46</v>
+      </c>
+      <c r="V5" s="2">
+        <v>4.38</v>
+      </c>
+      <c r="W5" s="2">
+        <v>-2.46</v>
+      </c>
+      <c r="X5" s="2">
+        <v>4.38</v>
+      </c>
+      <c r="Y5" s="2">
+        <v>68</v>
+      </c>
+      <c r="Z5" s="2">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="D6" s="5">
+        <v>1337450</v>
+      </c>
+      <c r="E6" s="5">
+        <v>10000000000</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="H6" s="2">
+        <v>0</v>
+      </c>
+      <c r="I6" s="2">
+        <v>0.52969999999999995</v>
+      </c>
+      <c r="J6" s="2">
+        <v>1</v>
+      </c>
+      <c r="K6" s="2">
+        <v>0</v>
+      </c>
+      <c r="L6" s="2">
+        <v>0</v>
+      </c>
+      <c r="M6" s="2">
+        <v>25</v>
+      </c>
+      <c r="N6" s="2">
+        <v>5</v>
+      </c>
+      <c r="O6" s="2">
+        <v>5</v>
+      </c>
+      <c r="P6" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q6" s="2">
+        <v>18.100000000000001</v>
+      </c>
+      <c r="R6" s="2">
+        <v>-1350.5</v>
+      </c>
+      <c r="S6" s="2">
+        <v>12.54</v>
+      </c>
+      <c r="T6" s="2">
+        <v>-917.3</v>
+      </c>
+      <c r="U6" s="2">
+        <v>-2.46</v>
+      </c>
+      <c r="V6" s="2">
+        <v>4.38</v>
+      </c>
+      <c r="W6" s="2">
+        <v>-2.46</v>
+      </c>
+      <c r="X6" s="2">
+        <v>4.38</v>
+      </c>
+      <c r="Y6" s="2">
+        <v>68</v>
+      </c>
+      <c r="Z6" s="2">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="D7" s="2">
+        <v>116300</v>
+      </c>
+      <c r="E7" s="5">
+        <v>1628200</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="H7" s="2">
+        <v>0</v>
+      </c>
+      <c r="I7" s="2">
+        <v>0.64239999999999997</v>
+      </c>
+      <c r="J7" s="2">
+        <v>1</v>
+      </c>
+      <c r="K7" s="2">
+        <v>0</v>
+      </c>
+      <c r="L7" s="2">
+        <v>0</v>
+      </c>
+      <c r="M7" s="2">
+        <v>25</v>
+      </c>
+      <c r="N7" s="2">
+        <v>5</v>
+      </c>
+      <c r="O7" s="2">
+        <v>5</v>
+      </c>
+      <c r="P7" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q7" s="2">
+        <v>14.6</v>
+      </c>
+      <c r="R7" s="2">
+        <v>-1171.7</v>
+      </c>
+      <c r="S7" s="2">
+        <v>7.05</v>
+      </c>
+      <c r="T7" s="2">
+        <v>-504.2</v>
+      </c>
+      <c r="U7" s="2">
+        <v>-2.14</v>
+      </c>
+      <c r="V7" s="2">
+        <v>3.29</v>
+      </c>
+      <c r="W7" s="2">
+        <v>-2.14</v>
+      </c>
+      <c r="X7" s="2">
+        <v>3.29</v>
+      </c>
+      <c r="Y7" s="2">
+        <v>62</v>
+      </c>
+      <c r="Z7" s="2">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555551" footer="0.51180555555555551"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <headerFooter alignWithMargins="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:O3"/>
   <sheetViews>
@@ -2139,7 +2779,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:T5"/>
   <sheetViews>
@@ -2473,7 +3113,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="A1:O2"/>
   <sheetViews>
@@ -2591,7 +3231,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <dimension ref="A1:O3"/>
   <sheetViews>
@@ -2757,7 +3397,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
   <dimension ref="A1:O5"/>
   <sheetViews>
@@ -3021,7 +3661,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
   <dimension ref="A1:Z8"/>
   <sheetViews>
@@ -3714,7 +4354,7 @@
         <v>23</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>130</v>
+        <v>149</v>
       </c>
       <c r="O1" s="1" t="s">
         <v>24</v>
@@ -3723,31 +4363,31 @@
         <v>25</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>131</v>
+        <v>150</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>132</v>
+        <v>151</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>133</v>
+        <v>152</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>134</v>
+        <v>153</v>
       </c>
       <c r="U1" s="1" t="s">
-        <v>135</v>
+        <v>154</v>
       </c>
       <c r="V1" s="1" t="s">
-        <v>136</v>
+        <v>155</v>
       </c>
       <c r="W1" s="1" t="s">
-        <v>137</v>
+        <v>156</v>
       </c>
       <c r="X1" s="1" t="s">
-        <v>138</v>
+        <v>157</v>
       </c>
       <c r="Y1" s="1" t="s">
-        <v>139</v>
+        <v>158</v>
       </c>
       <c r="Z1" s="1" t="s">
         <v>26</v>
@@ -3761,7 +4401,7 @@
         <v>113</v>
       </c>
       <c r="C2" s="14" t="s">
-        <v>140</v>
+        <v>159</v>
       </c>
       <c r="D2" s="2">
         <v>100</v>
@@ -3843,7 +4483,7 @@
         <v>113</v>
       </c>
       <c r="C3" s="14" t="s">
-        <v>140</v>
+        <v>159</v>
       </c>
       <c r="D3" s="2">
         <v>12000</v>
@@ -3919,13 +4559,13 @@
     </row>
     <row r="4" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>141</v>
+        <v>160</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>116</v>
       </c>
       <c r="C4" s="14" t="s">
-        <v>142</v>
+        <v>161</v>
       </c>
       <c r="D4" s="14">
         <v>0</v>
@@ -3934,7 +4574,7 @@
         <v>10000000000</v>
       </c>
       <c r="F4" s="14" t="s">
-        <v>143</v>
+        <v>162</v>
       </c>
       <c r="G4" s="14" t="s">
         <v>31</v>
@@ -3999,13 +4639,13 @@
     </row>
     <row r="5" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>144</v>
+        <v>163</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>145</v>
+        <v>164</v>
       </c>
       <c r="C5" s="14" t="s">
-        <v>142</v>
+        <v>161</v>
       </c>
       <c r="D5" s="14">
         <v>0</v>
@@ -4014,7 +4654,7 @@
         <v>10000000000</v>
       </c>
       <c r="F5" s="14" t="s">
-        <v>143</v>
+        <v>162</v>
       </c>
       <c r="G5" s="14" t="s">
         <v>31</v>
@@ -4079,13 +4719,13 @@
     </row>
     <row r="6" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>146</v>
+        <v>165</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>147</v>
+        <v>166</v>
       </c>
       <c r="C6" s="14" t="s">
-        <v>142</v>
+        <v>161</v>
       </c>
       <c r="D6" s="14">
         <v>0</v>
@@ -4094,7 +4734,7 @@
         <v>10000000000</v>
       </c>
       <c r="F6" s="14" t="s">
-        <v>143</v>
+        <v>162</v>
       </c>
       <c r="G6" s="14" t="s">
         <v>31</v>
@@ -4159,13 +4799,13 @@
     </row>
     <row r="7" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>148</v>
+        <v>167</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>149</v>
+        <v>168</v>
       </c>
       <c r="C7" s="14" t="s">
-        <v>142</v>
+        <v>161</v>
       </c>
       <c r="D7" s="14">
         <v>0</v>
@@ -4174,7 +4814,7 @@
         <v>10000000000</v>
       </c>
       <c r="F7" s="14" t="s">
-        <v>143</v>
+        <v>162</v>
       </c>
       <c r="G7" s="14" t="s">
         <v>31</v>
@@ -4239,13 +4879,13 @@
     </row>
     <row r="8" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>150</v>
+        <v>169</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>151</v>
+        <v>170</v>
       </c>
       <c r="C8" s="14" t="s">
-        <v>142</v>
+        <v>161</v>
       </c>
       <c r="D8" s="14">
         <v>0</v>
@@ -4254,7 +4894,7 @@
         <v>10000000000</v>
       </c>
       <c r="F8" s="14" t="s">
-        <v>143</v>
+        <v>162</v>
       </c>
       <c r="G8" s="14" t="s">
         <v>31</v>
@@ -5325,7 +5965,7 @@
   <dimension ref="A1:O2"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:O2"/>
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -5437,6 +6077,144 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+  <dimension ref="A1:M3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I22" sqref="I22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>129</v>
+      </c>
+      <c r="B1" t="s">
+        <v>130</v>
+      </c>
+      <c r="C1" t="s">
+        <v>131</v>
+      </c>
+      <c r="D1" t="s">
+        <v>132</v>
+      </c>
+      <c r="E1" t="s">
+        <v>133</v>
+      </c>
+      <c r="F1" t="s">
+        <v>134</v>
+      </c>
+      <c r="G1" t="s">
+        <v>135</v>
+      </c>
+      <c r="H1" t="s">
+        <v>136</v>
+      </c>
+      <c r="I1" t="s">
+        <v>137</v>
+      </c>
+      <c r="J1" t="s">
+        <v>138</v>
+      </c>
+      <c r="K1" t="s">
+        <v>139</v>
+      </c>
+      <c r="L1" t="s">
+        <v>140</v>
+      </c>
+      <c r="M1" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>142</v>
+      </c>
+      <c r="B2" t="s">
+        <v>143</v>
+      </c>
+      <c r="C2" t="s">
+        <v>144</v>
+      </c>
+      <c r="D2">
+        <v>0.33018832999999997</v>
+      </c>
+      <c r="E2">
+        <v>0.23554290999999999</v>
+      </c>
+      <c r="F2">
+        <v>0.46070828000000003</v>
+      </c>
+      <c r="G2">
+        <v>0.33269598</v>
+      </c>
+      <c r="H2">
+        <v>7.2911599999999997E-3</v>
+      </c>
+      <c r="I2">
+        <v>-4.9938000000000001E-4</v>
+      </c>
+      <c r="J2">
+        <v>1.598983E-2</v>
+      </c>
+      <c r="K2">
+        <v>-2.8254000000000002E-4</v>
+      </c>
+      <c r="L2">
+        <v>5.2346000000000001E-4</v>
+      </c>
+      <c r="M2" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>146</v>
+      </c>
+      <c r="B3" t="s">
+        <v>143</v>
+      </c>
+      <c r="C3" t="s">
+        <v>147</v>
+      </c>
+      <c r="D3">
+        <v>0.17149273000000001</v>
+      </c>
+      <c r="E3">
+        <v>0.58820207999999996</v>
+      </c>
+      <c r="F3">
+        <v>0.23737257</v>
+      </c>
+      <c r="G3">
+        <v>-0.29861976000000001</v>
+      </c>
+      <c r="H3">
+        <v>2.9960759999999999E-2</v>
+      </c>
+      <c r="I3">
+        <v>-8.0124999999999999E-4</v>
+      </c>
+      <c r="J3">
+        <v>1.7362679999999998E-2</v>
+      </c>
+      <c r="K3">
+        <v>-3.2605999999999998E-4</v>
+      </c>
+      <c r="L3">
+        <v>6.3139000000000001E-4</v>
+      </c>
+      <c r="M3" t="s">
+        <v>145</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:P25"/>
   <sheetViews>
@@ -5460,7 +6238,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>129</v>
+        <v>148</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>3</v>
@@ -5659,588 +6437,6 @@
     </row>
     <row r="25" spans="11:11" x14ac:dyDescent="0.2">
       <c r="K25" s="13"/>
-    </row>
-  </sheetData>
-  <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555551" footer="0.51180555555555551"/>
-  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
-  <headerFooter alignWithMargins="0"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
-  <dimension ref="A1:Z7"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J29" sqref="J29"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="27.6640625" customWidth="1"/>
-    <col min="5" max="5" width="9.6640625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="U1" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="V1" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="W1" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="X1" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="Y1" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="Z1" s="1" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="D2" s="2">
-        <v>0</v>
-      </c>
-      <c r="E2" s="2">
-        <v>51150</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="H2" s="2">
-        <v>0</v>
-      </c>
-      <c r="I2" s="2">
-        <v>0.4395</v>
-      </c>
-      <c r="J2" s="2">
-        <v>1</v>
-      </c>
-      <c r="K2" s="2">
-        <v>0</v>
-      </c>
-      <c r="L2" s="2">
-        <v>0</v>
-      </c>
-      <c r="M2" s="2">
-        <v>25</v>
-      </c>
-      <c r="N2" s="2">
-        <v>5</v>
-      </c>
-      <c r="O2" s="2">
-        <v>5</v>
-      </c>
-      <c r="P2" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="Q2" s="2">
-        <v>0.42</v>
-      </c>
-      <c r="R2" s="2">
-        <v>0.9</v>
-      </c>
-      <c r="S2" s="2">
-        <v>0.53</v>
-      </c>
-      <c r="T2" s="2">
-        <v>-2.5</v>
-      </c>
-      <c r="U2" s="2">
-        <v>-2.5</v>
-      </c>
-      <c r="V2" s="2">
-        <v>1.8</v>
-      </c>
-      <c r="W2" s="2">
-        <v>-2.1</v>
-      </c>
-      <c r="X2" s="2">
-        <v>1.5</v>
-      </c>
-      <c r="Y2" s="2">
-        <v>0.72199999999999998</v>
-      </c>
-      <c r="Z2" s="2">
-        <v>0.33300000000000002</v>
-      </c>
-    </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="D3" s="2">
-        <v>51150</v>
-      </c>
-      <c r="E3" s="5">
-        <v>1176000</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="H3" s="2">
-        <v>0</v>
-      </c>
-      <c r="I3" s="2">
-        <v>0.4395</v>
-      </c>
-      <c r="J3" s="2">
-        <v>1</v>
-      </c>
-      <c r="K3" s="2">
-        <v>0</v>
-      </c>
-      <c r="L3" s="2">
-        <v>0</v>
-      </c>
-      <c r="M3" s="2">
-        <v>25</v>
-      </c>
-      <c r="N3" s="2">
-        <v>5</v>
-      </c>
-      <c r="O3" s="2">
-        <v>5</v>
-      </c>
-      <c r="P3" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="Q3" s="2">
-        <v>68.12</v>
-      </c>
-      <c r="R3" s="2">
-        <v>-3281.1</v>
-      </c>
-      <c r="S3" s="2">
-        <v>88.05</v>
-      </c>
-      <c r="T3" s="2">
-        <v>-4216.1000000000004</v>
-      </c>
-      <c r="U3" s="2">
-        <v>-1.45</v>
-      </c>
-      <c r="V3" s="2">
-        <v>1.75</v>
-      </c>
-      <c r="W3" s="2">
-        <v>-1.45</v>
-      </c>
-      <c r="X3" s="2">
-        <v>1.75</v>
-      </c>
-      <c r="Y3" s="2">
-        <v>81</v>
-      </c>
-      <c r="Z3" s="2">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="D4" s="2">
-        <v>0</v>
-      </c>
-      <c r="E4" s="2">
-        <v>58150</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="H4" s="2">
-        <v>0</v>
-      </c>
-      <c r="I4" s="2">
-        <v>0.52969999999999995</v>
-      </c>
-      <c r="J4" s="2">
-        <v>1</v>
-      </c>
-      <c r="K4" s="2">
-        <v>0</v>
-      </c>
-      <c r="L4" s="2">
-        <v>0</v>
-      </c>
-      <c r="M4" s="2">
-        <v>25</v>
-      </c>
-      <c r="N4" s="2">
-        <v>5</v>
-      </c>
-      <c r="O4" s="2">
-        <v>5</v>
-      </c>
-      <c r="P4" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="Q4" s="2">
-        <v>0.42</v>
-      </c>
-      <c r="R4" s="2">
-        <v>0.9</v>
-      </c>
-      <c r="S4" s="2">
-        <v>0.53</v>
-      </c>
-      <c r="T4" s="2">
-        <v>-2.5</v>
-      </c>
-      <c r="U4" s="2">
-        <v>-2.5</v>
-      </c>
-      <c r="V4" s="2">
-        <v>1.8</v>
-      </c>
-      <c r="W4" s="2">
-        <v>-2.1</v>
-      </c>
-      <c r="X4" s="2">
-        <v>1.5</v>
-      </c>
-      <c r="Y4" s="2">
-        <v>0.72199999999999998</v>
-      </c>
-      <c r="Z4" s="2">
-        <v>0.33300000000000002</v>
-      </c>
-    </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A5" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="D5" s="2">
-        <v>58150</v>
-      </c>
-      <c r="E5" s="5">
-        <v>1337450</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="H5" s="2">
-        <v>0</v>
-      </c>
-      <c r="I5" s="2">
-        <v>0.52969999999999995</v>
-      </c>
-      <c r="J5" s="2">
-        <v>1</v>
-      </c>
-      <c r="K5" s="2">
-        <v>0</v>
-      </c>
-      <c r="L5" s="2">
-        <v>0</v>
-      </c>
-      <c r="M5" s="2">
-        <v>25</v>
-      </c>
-      <c r="N5" s="2">
-        <v>5</v>
-      </c>
-      <c r="O5" s="2">
-        <v>5</v>
-      </c>
-      <c r="P5" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="Q5" s="2">
-        <v>18.100000000000001</v>
-      </c>
-      <c r="R5" s="2">
-        <v>-1350.5</v>
-      </c>
-      <c r="S5" s="2">
-        <v>12.54</v>
-      </c>
-      <c r="T5" s="2">
-        <v>-917.3</v>
-      </c>
-      <c r="U5" s="2">
-        <v>-2.46</v>
-      </c>
-      <c r="V5" s="2">
-        <v>4.38</v>
-      </c>
-      <c r="W5" s="2">
-        <v>-2.46</v>
-      </c>
-      <c r="X5" s="2">
-        <v>4.38</v>
-      </c>
-      <c r="Y5" s="2">
-        <v>68</v>
-      </c>
-      <c r="Z5" s="2">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A6" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="D6" s="5">
-        <v>1337450</v>
-      </c>
-      <c r="E6" s="5">
-        <v>10000000000</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="G6" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="H6" s="2">
-        <v>0</v>
-      </c>
-      <c r="I6" s="2">
-        <v>0.52969999999999995</v>
-      </c>
-      <c r="J6" s="2">
-        <v>1</v>
-      </c>
-      <c r="K6" s="2">
-        <v>0</v>
-      </c>
-      <c r="L6" s="2">
-        <v>0</v>
-      </c>
-      <c r="M6" s="2">
-        <v>25</v>
-      </c>
-      <c r="N6" s="2">
-        <v>5</v>
-      </c>
-      <c r="O6" s="2">
-        <v>5</v>
-      </c>
-      <c r="P6" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="Q6" s="2">
-        <v>18.100000000000001</v>
-      </c>
-      <c r="R6" s="2">
-        <v>-1350.5</v>
-      </c>
-      <c r="S6" s="2">
-        <v>12.54</v>
-      </c>
-      <c r="T6" s="2">
-        <v>-917.3</v>
-      </c>
-      <c r="U6" s="2">
-        <v>-2.46</v>
-      </c>
-      <c r="V6" s="2">
-        <v>4.38</v>
-      </c>
-      <c r="W6" s="2">
-        <v>-2.46</v>
-      </c>
-      <c r="X6" s="2">
-        <v>4.38</v>
-      </c>
-      <c r="Y6" s="2">
-        <v>68</v>
-      </c>
-      <c r="Z6" s="2">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A7" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="D7" s="2">
-        <v>116300</v>
-      </c>
-      <c r="E7" s="5">
-        <v>1628200</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="G7" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="H7" s="2">
-        <v>0</v>
-      </c>
-      <c r="I7" s="2">
-        <v>0.64239999999999997</v>
-      </c>
-      <c r="J7" s="2">
-        <v>1</v>
-      </c>
-      <c r="K7" s="2">
-        <v>0</v>
-      </c>
-      <c r="L7" s="2">
-        <v>0</v>
-      </c>
-      <c r="M7" s="2">
-        <v>25</v>
-      </c>
-      <c r="N7" s="2">
-        <v>5</v>
-      </c>
-      <c r="O7" s="2">
-        <v>5</v>
-      </c>
-      <c r="P7" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="Q7" s="2">
-        <v>14.6</v>
-      </c>
-      <c r="R7" s="2">
-        <v>-1171.7</v>
-      </c>
-      <c r="S7" s="2">
-        <v>7.05</v>
-      </c>
-      <c r="T7" s="2">
-        <v>-504.2</v>
-      </c>
-      <c r="U7" s="2">
-        <v>-2.14</v>
-      </c>
-      <c r="V7" s="2">
-        <v>3.29</v>
-      </c>
-      <c r="W7" s="2">
-        <v>-2.14</v>
-      </c>
-      <c r="X7" s="2">
-        <v>3.29</v>
-      </c>
-      <c r="Y7" s="2">
-        <v>62</v>
-      </c>
-      <c r="Z7" s="2">
-        <v>10</v>
-      </c>
     </row>
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>

</xml_diff>

<commit_message>
added back the District heat exchanger
</commit_message>
<xml_diff>
--- a/cea/databases/CH/components/CONVERSION.xlsx
+++ b/cea/databases/CH/components/CONVERSION.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zshi/Documents/GitHub/CityEnergyAnalyst/cea/databases/CH/components/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8910E4A9-CC62-9943-8E8B-989CE5EBAFCC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91D07EFF-DE6B-9848-8DF0-6D31BA1A5014}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="940" yWindow="500" windowWidth="30240" windowHeight="19640" tabRatio="993" firstSheet="2" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1000" yWindow="500" windowWidth="30240" windowHeight="19640" tabRatio="993" firstSheet="2" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PHOTOVOLTAIC_PANELS" sheetId="1" r:id="rId1"/>
@@ -51,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="908" uniqueCount="237">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="914" uniqueCount="242">
   <si>
     <t>Description</t>
   </si>
@@ -762,6 +762,21 @@
   </si>
   <si>
     <t xml:space="preserve"> Assumptions</t>
+  </si>
+  <si>
+    <t>District substation heat exchanger</t>
+  </si>
+  <si>
+    <t>HEX2</t>
+  </si>
+  <si>
+    <t>m^2</t>
+  </si>
+  <si>
+    <t>Values under 1 and above 50 are assumptions, as no datasheet values are available in this area. a_p to e_p denote the pressure drop in Pa</t>
+  </si>
+  <si>
+    <t>-</t>
   </si>
 </sst>
 </file>
@@ -982,7 +997,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1102,18 +1117,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2433,7 +2436,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3AFF6F14-A874-CB45-A2C1-8C31AFCB2875}">
   <dimension ref="A1:O3"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="112" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView zoomScale="112" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="J22" sqref="J22"/>
     </sheetView>
   </sheetViews>
@@ -7337,7 +7340,7 @@
       <c r="A8" s="16" t="s">
         <v>183</v>
       </c>
-      <c r="B8" s="43" t="s">
+      <c r="B8" s="11" t="s">
         <v>231</v>
       </c>
       <c r="C8" s="11" t="s">
@@ -7408,7 +7411,7 @@
       <c r="A9" s="16" t="s">
         <v>183</v>
       </c>
-      <c r="B9" s="43" t="s">
+      <c r="B9" s="11" t="s">
         <v>231</v>
       </c>
       <c r="C9" s="11" t="s">
@@ -7479,7 +7482,7 @@
       <c r="A10" s="16" t="s">
         <v>184</v>
       </c>
-      <c r="B10" s="43" t="s">
+      <c r="B10" s="11" t="s">
         <v>230</v>
       </c>
       <c r="C10" s="11" t="s">
@@ -7550,7 +7553,7 @@
       <c r="A11" s="16" t="s">
         <v>186</v>
       </c>
-      <c r="B11" s="43" t="s">
+      <c r="B11" s="11" t="s">
         <v>63</v>
       </c>
       <c r="C11" s="11" t="s">
@@ -7633,8 +7636,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:U5"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:XFD5"/>
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -7915,7 +7918,58 @@
       </c>
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="C5" s="9"/>
+      <c r="A5" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>238</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>241</v>
+      </c>
+      <c r="D5" s="2">
+        <v>0</v>
+      </c>
+      <c r="E5" s="5">
+        <v>500</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>239</v>
+      </c>
+      <c r="G5" s="2"/>
+      <c r="H5" s="2"/>
+      <c r="I5" s="2"/>
+      <c r="J5" s="2"/>
+      <c r="K5" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="L5" s="2">
+        <v>3381</v>
+      </c>
+      <c r="M5" s="2">
+        <v>229.8</v>
+      </c>
+      <c r="N5" s="2">
+        <v>0</v>
+      </c>
+      <c r="O5" s="2">
+        <v>0</v>
+      </c>
+      <c r="P5" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q5" s="2">
+        <v>20</v>
+      </c>
+      <c r="R5" s="2">
+        <v>5</v>
+      </c>
+      <c r="S5" s="2">
+        <v>5</v>
+      </c>
+      <c r="T5" s="2" t="s">
+        <v>240</v>
+      </c>
     </row>
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
@@ -8019,10 +8073,10 @@
       <c r="A2" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="B2" s="44" t="s">
+      <c r="B2" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="C2" s="45">
+      <c r="C2" s="12">
         <v>0.47</v>
       </c>
       <c r="D2" s="2" t="s">
@@ -8087,10 +8141,10 @@
       <c r="A3" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="B3" s="46" t="s">
+      <c r="B3" s="14" t="s">
         <v>65</v>
       </c>
-      <c r="C3" s="43">
+      <c r="C3" s="11">
         <v>0.4</v>
       </c>
       <c r="D3" s="19" t="s">
@@ -8157,10 +8211,10 @@
       <c r="A4" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="B4" s="46" t="s">
+      <c r="B4" s="14" t="s">
         <v>65</v>
       </c>
-      <c r="C4" s="43">
+      <c r="C4" s="11">
         <v>0.4</v>
       </c>
       <c r="D4" s="19" t="s">
@@ -8227,10 +8281,10 @@
       <c r="A5" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="B5" s="46" t="s">
+      <c r="B5" s="14" t="s">
         <v>65</v>
       </c>
-      <c r="C5" s="43">
+      <c r="C5" s="11">
         <v>0.4</v>
       </c>
       <c r="D5" s="19" t="s">
@@ -8297,10 +8351,10 @@
       <c r="A6" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="B6" s="46" t="s">
+      <c r="B6" s="14" t="s">
         <v>65</v>
       </c>
-      <c r="C6" s="43">
+      <c r="C6" s="11">
         <v>0.4</v>
       </c>
       <c r="D6" s="19" t="s">
@@ -8367,10 +8421,10 @@
       <c r="A7" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="B7" s="46" t="s">
+      <c r="B7" s="14" t="s">
         <v>65</v>
       </c>
-      <c r="C7" s="43">
+      <c r="C7" s="11">
         <v>0.4</v>
       </c>
       <c r="D7" s="19" t="s">

</xml_diff>

<commit_message>
Updated massflowrates in ACH database
The mass flow rates of absorption chillers were underdimensioned, which led to extreme temperatures in some cases. These changes should fix that issue.
</commit_message>
<xml_diff>
--- a/cea/databases/CH/components/CONVERSION.xlsx
+++ b/cea/databases/CH/components/CONVERSION.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zshi/Documents/GitHub/CityEnergyAnalyst/cea/databases/CH/components/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nimathia\Documents\GitHub\CityEnergyAnalyst\CityEnergyAnalyst\cea\databases\CH\components\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91D07EFF-DE6B-9848-8DF0-6D31BA1A5014}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A852B0A-DB51-452C-88BC-5CE2FC2B7756}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1000" yWindow="500" windowWidth="30240" windowHeight="19640" tabRatio="993" firstSheet="2" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="22620" windowHeight="13500" tabRatio="993" firstSheet="2" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PHOTOVOLTAIC_PANELS" sheetId="1" r:id="rId1"/>
@@ -51,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="914" uniqueCount="242">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="914" uniqueCount="243">
   <si>
     <t>Description</t>
   </si>
@@ -777,6 +777,9 @@
   </si>
   <si>
     <t>-</t>
+  </si>
+  <si>
+    <t>ASHRAE 90.1/2019 - minimum efficiency rating at full load; https://www.esmagazine.com/articles/82307-basics-for-absorption-chillers - capacity-specific mass-flow rates</t>
   </si>
 </sst>
 </file>
@@ -853,7 +856,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -989,6 +992,15 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="59"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -997,7 +1009,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1044,9 +1056,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1117,13 +1126,17 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
     <cellStyle name="Normal 2 2" xfId="2" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
     <cellStyle name="Normal 3" xfId="3" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
-    <cellStyle name="Per cent" xfId="4" builtinId="5"/>
+    <cellStyle name="Percent" xfId="4" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1563,112 +1576,112 @@
       <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="38.6640625" customWidth="1"/>
-    <col min="4" max="4" width="15.6640625" customWidth="1"/>
+    <col min="1" max="1" width="38.6328125" customWidth="1"/>
+    <col min="4" max="4" width="15.6328125" customWidth="1"/>
     <col min="5" max="6" width="12" customWidth="1"/>
-    <col min="7" max="7" width="14.5" customWidth="1"/>
-    <col min="8" max="8" width="9.33203125" customWidth="1"/>
-    <col min="9" max="9" width="8.5" customWidth="1"/>
-    <col min="10" max="10" width="8.6640625" customWidth="1"/>
-    <col min="12" max="12" width="16.5" customWidth="1"/>
-    <col min="13" max="13" width="18.5" customWidth="1"/>
-    <col min="14" max="14" width="16.33203125" customWidth="1"/>
-    <col min="15" max="15" width="14.6640625" customWidth="1"/>
-    <col min="16" max="17" width="12.5" customWidth="1"/>
-    <col min="19" max="19" width="10.5" customWidth="1"/>
-    <col min="20" max="20" width="13.6640625" customWidth="1"/>
-    <col min="21" max="23" width="10.5" customWidth="1"/>
-    <col min="24" max="24" width="14.6640625" customWidth="1"/>
-    <col min="25" max="25" width="12.6640625" customWidth="1"/>
-    <col min="27" max="27" width="13.33203125" customWidth="1"/>
+    <col min="7" max="7" width="14.453125" customWidth="1"/>
+    <col min="8" max="8" width="9.36328125" customWidth="1"/>
+    <col min="9" max="9" width="8.453125" customWidth="1"/>
+    <col min="10" max="10" width="8.6328125" customWidth="1"/>
+    <col min="12" max="12" width="16.453125" customWidth="1"/>
+    <col min="13" max="13" width="18.453125" customWidth="1"/>
+    <col min="14" max="14" width="16.36328125" customWidth="1"/>
+    <col min="15" max="15" width="14.6328125" customWidth="1"/>
+    <col min="16" max="17" width="12.453125" customWidth="1"/>
+    <col min="19" max="19" width="10.453125" customWidth="1"/>
+    <col min="20" max="20" width="13.6328125" customWidth="1"/>
+    <col min="21" max="23" width="10.453125" customWidth="1"/>
+    <col min="24" max="24" width="14.6328125" customWidth="1"/>
+    <col min="25" max="25" width="12.6328125" customWidth="1"/>
+    <col min="27" max="27" width="13.36328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A1" s="36" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="36" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="36" t="s">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.35">
+      <c r="A1" s="35" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="35" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="35" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="36" t="s">
+      <c r="D1" s="35" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="36" t="s">
+      <c r="E1" s="35" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="36" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="36" t="s">
+      <c r="F1" s="35" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="35" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="36" t="s">
+      <c r="H1" s="35" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="36" t="s">
+      <c r="I1" s="35" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="36" t="s">
+      <c r="J1" s="35" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="36" t="s">
+      <c r="K1" s="35" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="36" t="s">
+      <c r="L1" s="35" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="36" t="s">
+      <c r="M1" s="35" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="36" t="s">
+      <c r="N1" s="35" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="36" t="s">
+      <c r="O1" s="35" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="36" t="s">
+      <c r="P1" s="35" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="36" t="s">
+      <c r="Q1" s="35" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="36" t="s">
+      <c r="R1" s="35" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="36" t="s">
+      <c r="S1" s="35" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="36" t="s">
+      <c r="T1" s="35" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="36" t="s">
+      <c r="U1" s="35" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="36" t="s">
+      <c r="V1" s="35" t="s">
         <v>21</v>
       </c>
-      <c r="W1" s="36" t="s">
+      <c r="W1" s="35" t="s">
         <v>22</v>
       </c>
-      <c r="X1" s="36" t="s">
+      <c r="X1" s="35" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" s="36" t="s">
+      <c r="Y1" s="35" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" s="36" t="s">
+      <c r="Z1" s="35" t="s">
         <v>25</v>
       </c>
-      <c r="AA1" s="36" t="s">
+      <c r="AA1" s="35" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>27</v>
       </c>
@@ -1752,7 +1765,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>27</v>
       </c>
@@ -1836,7 +1849,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>27</v>
       </c>
@@ -1920,7 +1933,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="5" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>33</v>
       </c>
@@ -2004,7 +2017,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>33</v>
       </c>
@@ -2088,7 +2101,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>33</v>
       </c>
@@ -2172,7 +2185,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="8" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>35</v>
       </c>
@@ -2256,7 +2269,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="9" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>35</v>
       </c>
@@ -2340,7 +2353,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="10" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>35</v>
       </c>
@@ -2440,16 +2453,16 @@
       <selection activeCell="J22" sqref="J22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="34.5" customWidth="1"/>
-    <col min="3" max="3" width="16.5" customWidth="1"/>
-    <col min="4" max="5" width="15.5" customWidth="1"/>
+    <col min="1" max="1" width="34.453125" customWidth="1"/>
+    <col min="3" max="3" width="16.453125" customWidth="1"/>
+    <col min="4" max="5" width="15.453125" customWidth="1"/>
     <col min="6" max="6" width="14" customWidth="1"/>
-    <col min="12" max="12" width="17.6640625" customWidth="1"/>
+    <col min="12" max="12" width="17.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2496,7 +2509,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>235</v>
       </c>
@@ -2542,7 +2555,7 @@
       </c>
       <c r="O2" s="2"/>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>235</v>
       </c>
@@ -2606,86 +2619,86 @@
       <selection activeCell="U25" sqref="U25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="45.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.5" customWidth="1"/>
-    <col min="4" max="5" width="15.6640625" customWidth="1"/>
-    <col min="6" max="6" width="11.1640625" customWidth="1"/>
-    <col min="7" max="7" width="16.5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.33203125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="17.5" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="33.33203125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="93.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="45.453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.453125" customWidth="1"/>
+    <col min="4" max="5" width="15.6328125" customWidth="1"/>
+    <col min="6" max="6" width="11.1796875" customWidth="1"/>
+    <col min="7" max="7" width="16.453125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.6328125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.36328125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="17.453125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="33.36328125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="93.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A1" s="36" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="36" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="36" t="s">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A1" s="35" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="35" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="35" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="36" t="s">
+      <c r="D1" s="35" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="36" t="s">
+      <c r="E1" s="35" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="36" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="36" t="s">
+      <c r="F1" s="35" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="35" t="s">
         <v>153</v>
       </c>
-      <c r="H1" s="36" t="s">
+      <c r="H1" s="35" t="s">
         <v>131</v>
       </c>
-      <c r="I1" s="36" t="s">
+      <c r="I1" s="35" t="s">
         <v>144</v>
       </c>
-      <c r="J1" s="36" t="s">
+      <c r="J1" s="35" t="s">
         <v>145</v>
       </c>
-      <c r="K1" s="36" t="s">
+      <c r="K1" s="35" t="s">
         <v>17</v>
       </c>
-      <c r="L1" s="36" t="s">
+      <c r="L1" s="35" t="s">
         <v>18</v>
       </c>
-      <c r="M1" s="36" t="s">
+      <c r="M1" s="35" t="s">
         <v>19</v>
       </c>
-      <c r="N1" s="36" t="s">
+      <c r="N1" s="35" t="s">
         <v>20</v>
       </c>
-      <c r="O1" s="36" t="s">
+      <c r="O1" s="35" t="s">
         <v>21</v>
       </c>
-      <c r="P1" s="36" t="s">
+      <c r="P1" s="35" t="s">
         <v>22</v>
       </c>
-      <c r="Q1" s="36" t="s">
+      <c r="Q1" s="35" t="s">
         <v>23</v>
       </c>
-      <c r="R1" s="36" t="s">
+      <c r="R1" s="35" t="s">
         <v>24</v>
       </c>
-      <c r="S1" s="36" t="s">
+      <c r="S1" s="35" t="s">
         <v>25</v>
       </c>
-      <c r="T1" s="36" t="s">
+      <c r="T1" s="35" t="s">
         <v>26</v>
       </c>
-      <c r="U1" s="36" t="s">
+      <c r="U1" s="35" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>147</v>
       </c>
@@ -2750,7 +2763,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>150</v>
       </c>
@@ -2815,10 +2828,10 @@
         <v>146</v>
       </c>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.35">
       <c r="O9" s="10"/>
     </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.35">
       <c r="O11" s="10"/>
     </row>
   </sheetData>
@@ -2834,97 +2847,97 @@
       <selection activeCell="AB25" sqref="AB25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="29" customWidth="1"/>
     <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="15.1640625" customWidth="1"/>
-    <col min="6" max="6" width="6.83203125" customWidth="1"/>
-    <col min="7" max="7" width="19.5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.5" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.83203125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.83203125" customWidth="1"/>
+    <col min="4" max="5" width="15.1796875" customWidth="1"/>
+    <col min="6" max="6" width="6.81640625" customWidth="1"/>
+    <col min="7" max="7" width="19.453125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.6328125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.453125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.81640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.81640625" customWidth="1"/>
     <col min="12" max="12" width="16" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="11.33203125" customWidth="1"/>
-    <col min="16" max="16" width="12.5" customWidth="1"/>
+    <col min="14" max="14" width="11.36328125" customWidth="1"/>
+    <col min="16" max="16" width="12.453125" customWidth="1"/>
     <col min="17" max="17" width="12" customWidth="1"/>
     <col min="22" max="22" width="10" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="32.5" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="32.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A1" s="36" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="36" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="36" t="s">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A1" s="35" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="35" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="35" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="36" t="s">
+      <c r="D1" s="35" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="36" t="s">
+      <c r="E1" s="35" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="37" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="40" t="s">
+      <c r="F1" s="36" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="39" t="s">
         <v>207</v>
       </c>
-      <c r="H1" s="40" t="s">
+      <c r="H1" s="39" t="s">
         <v>131</v>
       </c>
-      <c r="I1" s="40" t="s">
+      <c r="I1" s="39" t="s">
         <v>129</v>
       </c>
-      <c r="J1" s="40" t="s">
+      <c r="J1" s="39" t="s">
         <v>130</v>
       </c>
-      <c r="K1" s="40" t="s">
+      <c r="K1" s="39" t="s">
         <v>203</v>
       </c>
-      <c r="L1" s="40" t="s">
+      <c r="L1" s="39" t="s">
         <v>204</v>
       </c>
-      <c r="M1" s="38" t="s">
+      <c r="M1" s="37" t="s">
         <v>17</v>
       </c>
-      <c r="N1" s="36" t="s">
+      <c r="N1" s="35" t="s">
         <v>18</v>
       </c>
-      <c r="O1" s="36" t="s">
+      <c r="O1" s="35" t="s">
         <v>19</v>
       </c>
-      <c r="P1" s="36" t="s">
+      <c r="P1" s="35" t="s">
         <v>20</v>
       </c>
-      <c r="Q1" s="36" t="s">
+      <c r="Q1" s="35" t="s">
         <v>21</v>
       </c>
-      <c r="R1" s="36" t="s">
+      <c r="R1" s="35" t="s">
         <v>22</v>
       </c>
-      <c r="S1" s="36" t="s">
+      <c r="S1" s="35" t="s">
         <v>23</v>
       </c>
-      <c r="T1" s="36" t="s">
+      <c r="T1" s="35" t="s">
         <v>24</v>
       </c>
-      <c r="U1" s="36" t="s">
+      <c r="U1" s="35" t="s">
         <v>25</v>
       </c>
-      <c r="V1" s="37" t="s">
+      <c r="V1" s="36" t="s">
         <v>26</v>
       </c>
-      <c r="W1" s="40" t="s">
+      <c r="W1" s="39" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>200</v>
       </c>
@@ -2961,7 +2974,7 @@
       <c r="L2" s="11" t="s">
         <v>206</v>
       </c>
-      <c r="M2" s="19" t="s">
+      <c r="M2" s="18" t="s">
         <v>31</v>
       </c>
       <c r="N2" s="2">
@@ -2990,11 +3003,11 @@
         <v>5</v>
       </c>
       <c r="V2" s="14"/>
-      <c r="W2" s="27" t="s">
+      <c r="W2" s="26" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>200</v>
       </c>
@@ -3031,7 +3044,7 @@
       <c r="L3" s="11" t="s">
         <v>206</v>
       </c>
-      <c r="M3" s="19" t="s">
+      <c r="M3" s="18" t="s">
         <v>31</v>
       </c>
       <c r="N3" s="2">
@@ -3060,11 +3073,11 @@
         <v>5</v>
       </c>
       <c r="V3" s="14"/>
-      <c r="W3" s="27" t="s">
+      <c r="W3" s="26" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>199</v>
       </c>
@@ -3101,7 +3114,7 @@
       <c r="L4" s="11" t="s">
         <v>206</v>
       </c>
-      <c r="M4" s="19" t="s">
+      <c r="M4" s="18" t="s">
         <v>31</v>
       </c>
       <c r="N4" s="2">
@@ -3131,11 +3144,11 @@
         <v>6</v>
       </c>
       <c r="V4" s="14"/>
-      <c r="W4" s="27" t="s">
+      <c r="W4" s="26" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>199</v>
       </c>
@@ -3172,7 +3185,7 @@
       <c r="L5" s="11" t="s">
         <v>206</v>
       </c>
-      <c r="M5" s="19" t="s">
+      <c r="M5" s="18" t="s">
         <v>31</v>
       </c>
       <c r="N5" s="2">
@@ -3202,11 +3215,11 @@
         <v>6</v>
       </c>
       <c r="V5" s="14"/>
-      <c r="W5" s="27" t="s">
+      <c r="W5" s="26" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>199</v>
       </c>
@@ -3243,7 +3256,7 @@
       <c r="L6" s="11" t="s">
         <v>206</v>
       </c>
-      <c r="M6" s="19" t="s">
+      <c r="M6" s="18" t="s">
         <v>31</v>
       </c>
       <c r="N6" s="2">
@@ -3273,11 +3286,11 @@
         <v>6</v>
       </c>
       <c r="V6" s="14"/>
-      <c r="W6" s="27" t="s">
+      <c r="W6" s="26" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>199</v>
       </c>
@@ -3314,7 +3327,7 @@
       <c r="L7" s="11" t="s">
         <v>206</v>
       </c>
-      <c r="M7" s="19" t="s">
+      <c r="M7" s="18" t="s">
         <v>31</v>
       </c>
       <c r="N7" s="2">
@@ -3344,11 +3357,11 @@
         <v>6</v>
       </c>
       <c r="V7" s="14"/>
-      <c r="W7" s="27" t="s">
+      <c r="W7" s="26" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>197</v>
       </c>
@@ -3385,7 +3398,7 @@
       <c r="L8" s="11" t="s">
         <v>193</v>
       </c>
-      <c r="M8" s="19" t="s">
+      <c r="M8" s="18" t="s">
         <v>31</v>
       </c>
       <c r="N8" s="2">
@@ -3416,11 +3429,11 @@
       <c r="V8" s="14" t="s">
         <v>201</v>
       </c>
-      <c r="W8" s="27" t="s">
+      <c r="W8" s="26" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>197</v>
       </c>
@@ -3457,7 +3470,7 @@
       <c r="L9" s="11" t="s">
         <v>193</v>
       </c>
-      <c r="M9" s="19" t="s">
+      <c r="M9" s="18" t="s">
         <v>31</v>
       </c>
       <c r="N9" s="2">
@@ -3488,11 +3501,11 @@
       <c r="V9" s="14" t="s">
         <v>201</v>
       </c>
-      <c r="W9" s="27" t="s">
+      <c r="W9" s="26" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>197</v>
       </c>
@@ -3529,7 +3542,7 @@
       <c r="L10" s="11" t="s">
         <v>193</v>
       </c>
-      <c r="M10" s="19" t="s">
+      <c r="M10" s="18" t="s">
         <v>31</v>
       </c>
       <c r="N10" s="2">
@@ -3560,11 +3573,11 @@
       <c r="V10" s="14" t="s">
         <v>201</v>
       </c>
-      <c r="W10" s="27" t="s">
+      <c r="W10" s="26" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
         <v>197</v>
       </c>
@@ -3601,7 +3614,7 @@
       <c r="L11" s="11" t="s">
         <v>193</v>
       </c>
-      <c r="M11" s="19" t="s">
+      <c r="M11" s="18" t="s">
         <v>31</v>
       </c>
       <c r="N11" s="2">
@@ -3632,7 +3645,7 @@
       <c r="V11" s="14" t="s">
         <v>201</v>
       </c>
-      <c r="W11" s="27" t="s">
+      <c r="W11" s="26" t="s">
         <v>202</v>
       </c>
     </row>
@@ -3652,731 +3665,731 @@
       <selection activeCell="AB23" sqref="AB23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="43.33203125" customWidth="1"/>
-    <col min="2" max="2" width="12.6640625" customWidth="1"/>
-    <col min="3" max="3" width="19.6640625" customWidth="1"/>
-    <col min="4" max="5" width="19.33203125" customWidth="1"/>
+    <col min="1" max="1" width="43.36328125" customWidth="1"/>
+    <col min="2" max="2" width="12.6328125" customWidth="1"/>
+    <col min="3" max="3" width="19.6328125" customWidth="1"/>
+    <col min="4" max="5" width="19.36328125" customWidth="1"/>
     <col min="14" max="14" width="10" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="17.36328125" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="10" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="18.1796875" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="7" customWidth="1"/>
-    <col min="26" max="26" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="257" max="257" width="43.33203125" customWidth="1"/>
-    <col min="258" max="258" width="12.6640625" customWidth="1"/>
-    <col min="259" max="259" width="19.6640625" customWidth="1"/>
-    <col min="260" max="261" width="19.33203125" customWidth="1"/>
+    <col min="26" max="26" width="17.36328125" bestFit="1" customWidth="1"/>
+    <col min="257" max="257" width="43.36328125" customWidth="1"/>
+    <col min="258" max="258" width="12.6328125" customWidth="1"/>
+    <col min="259" max="259" width="19.6328125" customWidth="1"/>
+    <col min="260" max="261" width="19.36328125" customWidth="1"/>
     <col min="270" max="270" width="10" bestFit="1" customWidth="1"/>
-    <col min="271" max="271" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="271" max="271" width="17.36328125" bestFit="1" customWidth="1"/>
     <col min="274" max="274" width="10" bestFit="1" customWidth="1"/>
-    <col min="278" max="278" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="278" max="278" width="18.1796875" bestFit="1" customWidth="1"/>
     <col min="280" max="280" width="7" customWidth="1"/>
-    <col min="282" max="282" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="513" max="513" width="43.33203125" customWidth="1"/>
-    <col min="514" max="514" width="12.6640625" customWidth="1"/>
-    <col min="515" max="515" width="19.6640625" customWidth="1"/>
-    <col min="516" max="517" width="19.33203125" customWidth="1"/>
+    <col min="282" max="282" width="17.36328125" bestFit="1" customWidth="1"/>
+    <col min="513" max="513" width="43.36328125" customWidth="1"/>
+    <col min="514" max="514" width="12.6328125" customWidth="1"/>
+    <col min="515" max="515" width="19.6328125" customWidth="1"/>
+    <col min="516" max="517" width="19.36328125" customWidth="1"/>
     <col min="526" max="526" width="10" bestFit="1" customWidth="1"/>
-    <col min="527" max="527" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="527" max="527" width="17.36328125" bestFit="1" customWidth="1"/>
     <col min="530" max="530" width="10" bestFit="1" customWidth="1"/>
-    <col min="534" max="534" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="534" max="534" width="18.1796875" bestFit="1" customWidth="1"/>
     <col min="536" max="536" width="7" customWidth="1"/>
-    <col min="538" max="538" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="769" max="769" width="43.33203125" customWidth="1"/>
-    <col min="770" max="770" width="12.6640625" customWidth="1"/>
-    <col min="771" max="771" width="19.6640625" customWidth="1"/>
-    <col min="772" max="773" width="19.33203125" customWidth="1"/>
+    <col min="538" max="538" width="17.36328125" bestFit="1" customWidth="1"/>
+    <col min="769" max="769" width="43.36328125" customWidth="1"/>
+    <col min="770" max="770" width="12.6328125" customWidth="1"/>
+    <col min="771" max="771" width="19.6328125" customWidth="1"/>
+    <col min="772" max="773" width="19.36328125" customWidth="1"/>
     <col min="782" max="782" width="10" bestFit="1" customWidth="1"/>
-    <col min="783" max="783" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="783" max="783" width="17.36328125" bestFit="1" customWidth="1"/>
     <col min="786" max="786" width="10" bestFit="1" customWidth="1"/>
-    <col min="790" max="790" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="790" max="790" width="18.1796875" bestFit="1" customWidth="1"/>
     <col min="792" max="792" width="7" customWidth="1"/>
-    <col min="794" max="794" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="1025" max="1025" width="43.33203125" customWidth="1"/>
-    <col min="1026" max="1026" width="12.6640625" customWidth="1"/>
-    <col min="1027" max="1027" width="19.6640625" customWidth="1"/>
-    <col min="1028" max="1029" width="19.33203125" customWidth="1"/>
+    <col min="794" max="794" width="17.36328125" bestFit="1" customWidth="1"/>
+    <col min="1025" max="1025" width="43.36328125" customWidth="1"/>
+    <col min="1026" max="1026" width="12.6328125" customWidth="1"/>
+    <col min="1027" max="1027" width="19.6328125" customWidth="1"/>
+    <col min="1028" max="1029" width="19.36328125" customWidth="1"/>
     <col min="1038" max="1038" width="10" bestFit="1" customWidth="1"/>
-    <col min="1039" max="1039" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="1039" max="1039" width="17.36328125" bestFit="1" customWidth="1"/>
     <col min="1042" max="1042" width="10" bestFit="1" customWidth="1"/>
-    <col min="1046" max="1046" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="1046" max="1046" width="18.1796875" bestFit="1" customWidth="1"/>
     <col min="1048" max="1048" width="7" customWidth="1"/>
-    <col min="1050" max="1050" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="1281" max="1281" width="43.33203125" customWidth="1"/>
-    <col min="1282" max="1282" width="12.6640625" customWidth="1"/>
-    <col min="1283" max="1283" width="19.6640625" customWidth="1"/>
-    <col min="1284" max="1285" width="19.33203125" customWidth="1"/>
+    <col min="1050" max="1050" width="17.36328125" bestFit="1" customWidth="1"/>
+    <col min="1281" max="1281" width="43.36328125" customWidth="1"/>
+    <col min="1282" max="1282" width="12.6328125" customWidth="1"/>
+    <col min="1283" max="1283" width="19.6328125" customWidth="1"/>
+    <col min="1284" max="1285" width="19.36328125" customWidth="1"/>
     <col min="1294" max="1294" width="10" bestFit="1" customWidth="1"/>
-    <col min="1295" max="1295" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="1295" max="1295" width="17.36328125" bestFit="1" customWidth="1"/>
     <col min="1298" max="1298" width="10" bestFit="1" customWidth="1"/>
-    <col min="1302" max="1302" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="1302" max="1302" width="18.1796875" bestFit="1" customWidth="1"/>
     <col min="1304" max="1304" width="7" customWidth="1"/>
-    <col min="1306" max="1306" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="1537" max="1537" width="43.33203125" customWidth="1"/>
-    <col min="1538" max="1538" width="12.6640625" customWidth="1"/>
-    <col min="1539" max="1539" width="19.6640625" customWidth="1"/>
-    <col min="1540" max="1541" width="19.33203125" customWidth="1"/>
+    <col min="1306" max="1306" width="17.36328125" bestFit="1" customWidth="1"/>
+    <col min="1537" max="1537" width="43.36328125" customWidth="1"/>
+    <col min="1538" max="1538" width="12.6328125" customWidth="1"/>
+    <col min="1539" max="1539" width="19.6328125" customWidth="1"/>
+    <col min="1540" max="1541" width="19.36328125" customWidth="1"/>
     <col min="1550" max="1550" width="10" bestFit="1" customWidth="1"/>
-    <col min="1551" max="1551" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="1551" max="1551" width="17.36328125" bestFit="1" customWidth="1"/>
     <col min="1554" max="1554" width="10" bestFit="1" customWidth="1"/>
-    <col min="1558" max="1558" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="1558" max="1558" width="18.1796875" bestFit="1" customWidth="1"/>
     <col min="1560" max="1560" width="7" customWidth="1"/>
-    <col min="1562" max="1562" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="1793" max="1793" width="43.33203125" customWidth="1"/>
-    <col min="1794" max="1794" width="12.6640625" customWidth="1"/>
-    <col min="1795" max="1795" width="19.6640625" customWidth="1"/>
-    <col min="1796" max="1797" width="19.33203125" customWidth="1"/>
+    <col min="1562" max="1562" width="17.36328125" bestFit="1" customWidth="1"/>
+    <col min="1793" max="1793" width="43.36328125" customWidth="1"/>
+    <col min="1794" max="1794" width="12.6328125" customWidth="1"/>
+    <col min="1795" max="1795" width="19.6328125" customWidth="1"/>
+    <col min="1796" max="1797" width="19.36328125" customWidth="1"/>
     <col min="1806" max="1806" width="10" bestFit="1" customWidth="1"/>
-    <col min="1807" max="1807" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="1807" max="1807" width="17.36328125" bestFit="1" customWidth="1"/>
     <col min="1810" max="1810" width="10" bestFit="1" customWidth="1"/>
-    <col min="1814" max="1814" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="1814" max="1814" width="18.1796875" bestFit="1" customWidth="1"/>
     <col min="1816" max="1816" width="7" customWidth="1"/>
-    <col min="1818" max="1818" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="2049" max="2049" width="43.33203125" customWidth="1"/>
-    <col min="2050" max="2050" width="12.6640625" customWidth="1"/>
-    <col min="2051" max="2051" width="19.6640625" customWidth="1"/>
-    <col min="2052" max="2053" width="19.33203125" customWidth="1"/>
+    <col min="1818" max="1818" width="17.36328125" bestFit="1" customWidth="1"/>
+    <col min="2049" max="2049" width="43.36328125" customWidth="1"/>
+    <col min="2050" max="2050" width="12.6328125" customWidth="1"/>
+    <col min="2051" max="2051" width="19.6328125" customWidth="1"/>
+    <col min="2052" max="2053" width="19.36328125" customWidth="1"/>
     <col min="2062" max="2062" width="10" bestFit="1" customWidth="1"/>
-    <col min="2063" max="2063" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="2063" max="2063" width="17.36328125" bestFit="1" customWidth="1"/>
     <col min="2066" max="2066" width="10" bestFit="1" customWidth="1"/>
-    <col min="2070" max="2070" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="2070" max="2070" width="18.1796875" bestFit="1" customWidth="1"/>
     <col min="2072" max="2072" width="7" customWidth="1"/>
-    <col min="2074" max="2074" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="2305" max="2305" width="43.33203125" customWidth="1"/>
-    <col min="2306" max="2306" width="12.6640625" customWidth="1"/>
-    <col min="2307" max="2307" width="19.6640625" customWidth="1"/>
-    <col min="2308" max="2309" width="19.33203125" customWidth="1"/>
+    <col min="2074" max="2074" width="17.36328125" bestFit="1" customWidth="1"/>
+    <col min="2305" max="2305" width="43.36328125" customWidth="1"/>
+    <col min="2306" max="2306" width="12.6328125" customWidth="1"/>
+    <col min="2307" max="2307" width="19.6328125" customWidth="1"/>
+    <col min="2308" max="2309" width="19.36328125" customWidth="1"/>
     <col min="2318" max="2318" width="10" bestFit="1" customWidth="1"/>
-    <col min="2319" max="2319" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="2319" max="2319" width="17.36328125" bestFit="1" customWidth="1"/>
     <col min="2322" max="2322" width="10" bestFit="1" customWidth="1"/>
-    <col min="2326" max="2326" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="2326" max="2326" width="18.1796875" bestFit="1" customWidth="1"/>
     <col min="2328" max="2328" width="7" customWidth="1"/>
-    <col min="2330" max="2330" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="2561" max="2561" width="43.33203125" customWidth="1"/>
-    <col min="2562" max="2562" width="12.6640625" customWidth="1"/>
-    <col min="2563" max="2563" width="19.6640625" customWidth="1"/>
-    <col min="2564" max="2565" width="19.33203125" customWidth="1"/>
+    <col min="2330" max="2330" width="17.36328125" bestFit="1" customWidth="1"/>
+    <col min="2561" max="2561" width="43.36328125" customWidth="1"/>
+    <col min="2562" max="2562" width="12.6328125" customWidth="1"/>
+    <col min="2563" max="2563" width="19.6328125" customWidth="1"/>
+    <col min="2564" max="2565" width="19.36328125" customWidth="1"/>
     <col min="2574" max="2574" width="10" bestFit="1" customWidth="1"/>
-    <col min="2575" max="2575" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="2575" max="2575" width="17.36328125" bestFit="1" customWidth="1"/>
     <col min="2578" max="2578" width="10" bestFit="1" customWidth="1"/>
-    <col min="2582" max="2582" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="2582" max="2582" width="18.1796875" bestFit="1" customWidth="1"/>
     <col min="2584" max="2584" width="7" customWidth="1"/>
-    <col min="2586" max="2586" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="2817" max="2817" width="43.33203125" customWidth="1"/>
-    <col min="2818" max="2818" width="12.6640625" customWidth="1"/>
-    <col min="2819" max="2819" width="19.6640625" customWidth="1"/>
-    <col min="2820" max="2821" width="19.33203125" customWidth="1"/>
+    <col min="2586" max="2586" width="17.36328125" bestFit="1" customWidth="1"/>
+    <col min="2817" max="2817" width="43.36328125" customWidth="1"/>
+    <col min="2818" max="2818" width="12.6328125" customWidth="1"/>
+    <col min="2819" max="2819" width="19.6328125" customWidth="1"/>
+    <col min="2820" max="2821" width="19.36328125" customWidth="1"/>
     <col min="2830" max="2830" width="10" bestFit="1" customWidth="1"/>
-    <col min="2831" max="2831" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="2831" max="2831" width="17.36328125" bestFit="1" customWidth="1"/>
     <col min="2834" max="2834" width="10" bestFit="1" customWidth="1"/>
-    <col min="2838" max="2838" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="2838" max="2838" width="18.1796875" bestFit="1" customWidth="1"/>
     <col min="2840" max="2840" width="7" customWidth="1"/>
-    <col min="2842" max="2842" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="3073" max="3073" width="43.33203125" customWidth="1"/>
-    <col min="3074" max="3074" width="12.6640625" customWidth="1"/>
-    <col min="3075" max="3075" width="19.6640625" customWidth="1"/>
-    <col min="3076" max="3077" width="19.33203125" customWidth="1"/>
+    <col min="2842" max="2842" width="17.36328125" bestFit="1" customWidth="1"/>
+    <col min="3073" max="3073" width="43.36328125" customWidth="1"/>
+    <col min="3074" max="3074" width="12.6328125" customWidth="1"/>
+    <col min="3075" max="3075" width="19.6328125" customWidth="1"/>
+    <col min="3076" max="3077" width="19.36328125" customWidth="1"/>
     <col min="3086" max="3086" width="10" bestFit="1" customWidth="1"/>
-    <col min="3087" max="3087" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="3087" max="3087" width="17.36328125" bestFit="1" customWidth="1"/>
     <col min="3090" max="3090" width="10" bestFit="1" customWidth="1"/>
-    <col min="3094" max="3094" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="3094" max="3094" width="18.1796875" bestFit="1" customWidth="1"/>
     <col min="3096" max="3096" width="7" customWidth="1"/>
-    <col min="3098" max="3098" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="3329" max="3329" width="43.33203125" customWidth="1"/>
-    <col min="3330" max="3330" width="12.6640625" customWidth="1"/>
-    <col min="3331" max="3331" width="19.6640625" customWidth="1"/>
-    <col min="3332" max="3333" width="19.33203125" customWidth="1"/>
+    <col min="3098" max="3098" width="17.36328125" bestFit="1" customWidth="1"/>
+    <col min="3329" max="3329" width="43.36328125" customWidth="1"/>
+    <col min="3330" max="3330" width="12.6328125" customWidth="1"/>
+    <col min="3331" max="3331" width="19.6328125" customWidth="1"/>
+    <col min="3332" max="3333" width="19.36328125" customWidth="1"/>
     <col min="3342" max="3342" width="10" bestFit="1" customWidth="1"/>
-    <col min="3343" max="3343" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="3343" max="3343" width="17.36328125" bestFit="1" customWidth="1"/>
     <col min="3346" max="3346" width="10" bestFit="1" customWidth="1"/>
-    <col min="3350" max="3350" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="3350" max="3350" width="18.1796875" bestFit="1" customWidth="1"/>
     <col min="3352" max="3352" width="7" customWidth="1"/>
-    <col min="3354" max="3354" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="3585" max="3585" width="43.33203125" customWidth="1"/>
-    <col min="3586" max="3586" width="12.6640625" customWidth="1"/>
-    <col min="3587" max="3587" width="19.6640625" customWidth="1"/>
-    <col min="3588" max="3589" width="19.33203125" customWidth="1"/>
+    <col min="3354" max="3354" width="17.36328125" bestFit="1" customWidth="1"/>
+    <col min="3585" max="3585" width="43.36328125" customWidth="1"/>
+    <col min="3586" max="3586" width="12.6328125" customWidth="1"/>
+    <col min="3587" max="3587" width="19.6328125" customWidth="1"/>
+    <col min="3588" max="3589" width="19.36328125" customWidth="1"/>
     <col min="3598" max="3598" width="10" bestFit="1" customWidth="1"/>
-    <col min="3599" max="3599" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="3599" max="3599" width="17.36328125" bestFit="1" customWidth="1"/>
     <col min="3602" max="3602" width="10" bestFit="1" customWidth="1"/>
-    <col min="3606" max="3606" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="3606" max="3606" width="18.1796875" bestFit="1" customWidth="1"/>
     <col min="3608" max="3608" width="7" customWidth="1"/>
-    <col min="3610" max="3610" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="3841" max="3841" width="43.33203125" customWidth="1"/>
-    <col min="3842" max="3842" width="12.6640625" customWidth="1"/>
-    <col min="3843" max="3843" width="19.6640625" customWidth="1"/>
-    <col min="3844" max="3845" width="19.33203125" customWidth="1"/>
+    <col min="3610" max="3610" width="17.36328125" bestFit="1" customWidth="1"/>
+    <col min="3841" max="3841" width="43.36328125" customWidth="1"/>
+    <col min="3842" max="3842" width="12.6328125" customWidth="1"/>
+    <col min="3843" max="3843" width="19.6328125" customWidth="1"/>
+    <col min="3844" max="3845" width="19.36328125" customWidth="1"/>
     <col min="3854" max="3854" width="10" bestFit="1" customWidth="1"/>
-    <col min="3855" max="3855" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="3855" max="3855" width="17.36328125" bestFit="1" customWidth="1"/>
     <col min="3858" max="3858" width="10" bestFit="1" customWidth="1"/>
-    <col min="3862" max="3862" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="3862" max="3862" width="18.1796875" bestFit="1" customWidth="1"/>
     <col min="3864" max="3864" width="7" customWidth="1"/>
-    <col min="3866" max="3866" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="4097" max="4097" width="43.33203125" customWidth="1"/>
-    <col min="4098" max="4098" width="12.6640625" customWidth="1"/>
-    <col min="4099" max="4099" width="19.6640625" customWidth="1"/>
-    <col min="4100" max="4101" width="19.33203125" customWidth="1"/>
+    <col min="3866" max="3866" width="17.36328125" bestFit="1" customWidth="1"/>
+    <col min="4097" max="4097" width="43.36328125" customWidth="1"/>
+    <col min="4098" max="4098" width="12.6328125" customWidth="1"/>
+    <col min="4099" max="4099" width="19.6328125" customWidth="1"/>
+    <col min="4100" max="4101" width="19.36328125" customWidth="1"/>
     <col min="4110" max="4110" width="10" bestFit="1" customWidth="1"/>
-    <col min="4111" max="4111" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="4111" max="4111" width="17.36328125" bestFit="1" customWidth="1"/>
     <col min="4114" max="4114" width="10" bestFit="1" customWidth="1"/>
-    <col min="4118" max="4118" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="4118" max="4118" width="18.1796875" bestFit="1" customWidth="1"/>
     <col min="4120" max="4120" width="7" customWidth="1"/>
-    <col min="4122" max="4122" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="4353" max="4353" width="43.33203125" customWidth="1"/>
-    <col min="4354" max="4354" width="12.6640625" customWidth="1"/>
-    <col min="4355" max="4355" width="19.6640625" customWidth="1"/>
-    <col min="4356" max="4357" width="19.33203125" customWidth="1"/>
+    <col min="4122" max="4122" width="17.36328125" bestFit="1" customWidth="1"/>
+    <col min="4353" max="4353" width="43.36328125" customWidth="1"/>
+    <col min="4354" max="4354" width="12.6328125" customWidth="1"/>
+    <col min="4355" max="4355" width="19.6328125" customWidth="1"/>
+    <col min="4356" max="4357" width="19.36328125" customWidth="1"/>
     <col min="4366" max="4366" width="10" bestFit="1" customWidth="1"/>
-    <col min="4367" max="4367" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="4367" max="4367" width="17.36328125" bestFit="1" customWidth="1"/>
     <col min="4370" max="4370" width="10" bestFit="1" customWidth="1"/>
-    <col min="4374" max="4374" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="4374" max="4374" width="18.1796875" bestFit="1" customWidth="1"/>
     <col min="4376" max="4376" width="7" customWidth="1"/>
-    <col min="4378" max="4378" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="4609" max="4609" width="43.33203125" customWidth="1"/>
-    <col min="4610" max="4610" width="12.6640625" customWidth="1"/>
-    <col min="4611" max="4611" width="19.6640625" customWidth="1"/>
-    <col min="4612" max="4613" width="19.33203125" customWidth="1"/>
+    <col min="4378" max="4378" width="17.36328125" bestFit="1" customWidth="1"/>
+    <col min="4609" max="4609" width="43.36328125" customWidth="1"/>
+    <col min="4610" max="4610" width="12.6328125" customWidth="1"/>
+    <col min="4611" max="4611" width="19.6328125" customWidth="1"/>
+    <col min="4612" max="4613" width="19.36328125" customWidth="1"/>
     <col min="4622" max="4622" width="10" bestFit="1" customWidth="1"/>
-    <col min="4623" max="4623" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="4623" max="4623" width="17.36328125" bestFit="1" customWidth="1"/>
     <col min="4626" max="4626" width="10" bestFit="1" customWidth="1"/>
-    <col min="4630" max="4630" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="4630" max="4630" width="18.1796875" bestFit="1" customWidth="1"/>
     <col min="4632" max="4632" width="7" customWidth="1"/>
-    <col min="4634" max="4634" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="4865" max="4865" width="43.33203125" customWidth="1"/>
-    <col min="4866" max="4866" width="12.6640625" customWidth="1"/>
-    <col min="4867" max="4867" width="19.6640625" customWidth="1"/>
-    <col min="4868" max="4869" width="19.33203125" customWidth="1"/>
+    <col min="4634" max="4634" width="17.36328125" bestFit="1" customWidth="1"/>
+    <col min="4865" max="4865" width="43.36328125" customWidth="1"/>
+    <col min="4866" max="4866" width="12.6328125" customWidth="1"/>
+    <col min="4867" max="4867" width="19.6328125" customWidth="1"/>
+    <col min="4868" max="4869" width="19.36328125" customWidth="1"/>
     <col min="4878" max="4878" width="10" bestFit="1" customWidth="1"/>
-    <col min="4879" max="4879" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="4879" max="4879" width="17.36328125" bestFit="1" customWidth="1"/>
     <col min="4882" max="4882" width="10" bestFit="1" customWidth="1"/>
-    <col min="4886" max="4886" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="4886" max="4886" width="18.1796875" bestFit="1" customWidth="1"/>
     <col min="4888" max="4888" width="7" customWidth="1"/>
-    <col min="4890" max="4890" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="5121" max="5121" width="43.33203125" customWidth="1"/>
-    <col min="5122" max="5122" width="12.6640625" customWidth="1"/>
-    <col min="5123" max="5123" width="19.6640625" customWidth="1"/>
-    <col min="5124" max="5125" width="19.33203125" customWidth="1"/>
+    <col min="4890" max="4890" width="17.36328125" bestFit="1" customWidth="1"/>
+    <col min="5121" max="5121" width="43.36328125" customWidth="1"/>
+    <col min="5122" max="5122" width="12.6328125" customWidth="1"/>
+    <col min="5123" max="5123" width="19.6328125" customWidth="1"/>
+    <col min="5124" max="5125" width="19.36328125" customWidth="1"/>
     <col min="5134" max="5134" width="10" bestFit="1" customWidth="1"/>
-    <col min="5135" max="5135" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="5135" max="5135" width="17.36328125" bestFit="1" customWidth="1"/>
     <col min="5138" max="5138" width="10" bestFit="1" customWidth="1"/>
-    <col min="5142" max="5142" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="5142" max="5142" width="18.1796875" bestFit="1" customWidth="1"/>
     <col min="5144" max="5144" width="7" customWidth="1"/>
-    <col min="5146" max="5146" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="5377" max="5377" width="43.33203125" customWidth="1"/>
-    <col min="5378" max="5378" width="12.6640625" customWidth="1"/>
-    <col min="5379" max="5379" width="19.6640625" customWidth="1"/>
-    <col min="5380" max="5381" width="19.33203125" customWidth="1"/>
+    <col min="5146" max="5146" width="17.36328125" bestFit="1" customWidth="1"/>
+    <col min="5377" max="5377" width="43.36328125" customWidth="1"/>
+    <col min="5378" max="5378" width="12.6328125" customWidth="1"/>
+    <col min="5379" max="5379" width="19.6328125" customWidth="1"/>
+    <col min="5380" max="5381" width="19.36328125" customWidth="1"/>
     <col min="5390" max="5390" width="10" bestFit="1" customWidth="1"/>
-    <col min="5391" max="5391" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="5391" max="5391" width="17.36328125" bestFit="1" customWidth="1"/>
     <col min="5394" max="5394" width="10" bestFit="1" customWidth="1"/>
-    <col min="5398" max="5398" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="5398" max="5398" width="18.1796875" bestFit="1" customWidth="1"/>
     <col min="5400" max="5400" width="7" customWidth="1"/>
-    <col min="5402" max="5402" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="5633" max="5633" width="43.33203125" customWidth="1"/>
-    <col min="5634" max="5634" width="12.6640625" customWidth="1"/>
-    <col min="5635" max="5635" width="19.6640625" customWidth="1"/>
-    <col min="5636" max="5637" width="19.33203125" customWidth="1"/>
+    <col min="5402" max="5402" width="17.36328125" bestFit="1" customWidth="1"/>
+    <col min="5633" max="5633" width="43.36328125" customWidth="1"/>
+    <col min="5634" max="5634" width="12.6328125" customWidth="1"/>
+    <col min="5635" max="5635" width="19.6328125" customWidth="1"/>
+    <col min="5636" max="5637" width="19.36328125" customWidth="1"/>
     <col min="5646" max="5646" width="10" bestFit="1" customWidth="1"/>
-    <col min="5647" max="5647" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="5647" max="5647" width="17.36328125" bestFit="1" customWidth="1"/>
     <col min="5650" max="5650" width="10" bestFit="1" customWidth="1"/>
-    <col min="5654" max="5654" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="5654" max="5654" width="18.1796875" bestFit="1" customWidth="1"/>
     <col min="5656" max="5656" width="7" customWidth="1"/>
-    <col min="5658" max="5658" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="5889" max="5889" width="43.33203125" customWidth="1"/>
-    <col min="5890" max="5890" width="12.6640625" customWidth="1"/>
-    <col min="5891" max="5891" width="19.6640625" customWidth="1"/>
-    <col min="5892" max="5893" width="19.33203125" customWidth="1"/>
+    <col min="5658" max="5658" width="17.36328125" bestFit="1" customWidth="1"/>
+    <col min="5889" max="5889" width="43.36328125" customWidth="1"/>
+    <col min="5890" max="5890" width="12.6328125" customWidth="1"/>
+    <col min="5891" max="5891" width="19.6328125" customWidth="1"/>
+    <col min="5892" max="5893" width="19.36328125" customWidth="1"/>
     <col min="5902" max="5902" width="10" bestFit="1" customWidth="1"/>
-    <col min="5903" max="5903" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="5903" max="5903" width="17.36328125" bestFit="1" customWidth="1"/>
     <col min="5906" max="5906" width="10" bestFit="1" customWidth="1"/>
-    <col min="5910" max="5910" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="5910" max="5910" width="18.1796875" bestFit="1" customWidth="1"/>
     <col min="5912" max="5912" width="7" customWidth="1"/>
-    <col min="5914" max="5914" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="6145" max="6145" width="43.33203125" customWidth="1"/>
-    <col min="6146" max="6146" width="12.6640625" customWidth="1"/>
-    <col min="6147" max="6147" width="19.6640625" customWidth="1"/>
-    <col min="6148" max="6149" width="19.33203125" customWidth="1"/>
+    <col min="5914" max="5914" width="17.36328125" bestFit="1" customWidth="1"/>
+    <col min="6145" max="6145" width="43.36328125" customWidth="1"/>
+    <col min="6146" max="6146" width="12.6328125" customWidth="1"/>
+    <col min="6147" max="6147" width="19.6328125" customWidth="1"/>
+    <col min="6148" max="6149" width="19.36328125" customWidth="1"/>
     <col min="6158" max="6158" width="10" bestFit="1" customWidth="1"/>
-    <col min="6159" max="6159" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="6159" max="6159" width="17.36328125" bestFit="1" customWidth="1"/>
     <col min="6162" max="6162" width="10" bestFit="1" customWidth="1"/>
-    <col min="6166" max="6166" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="6166" max="6166" width="18.1796875" bestFit="1" customWidth="1"/>
     <col min="6168" max="6168" width="7" customWidth="1"/>
-    <col min="6170" max="6170" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="6401" max="6401" width="43.33203125" customWidth="1"/>
-    <col min="6402" max="6402" width="12.6640625" customWidth="1"/>
-    <col min="6403" max="6403" width="19.6640625" customWidth="1"/>
-    <col min="6404" max="6405" width="19.33203125" customWidth="1"/>
+    <col min="6170" max="6170" width="17.36328125" bestFit="1" customWidth="1"/>
+    <col min="6401" max="6401" width="43.36328125" customWidth="1"/>
+    <col min="6402" max="6402" width="12.6328125" customWidth="1"/>
+    <col min="6403" max="6403" width="19.6328125" customWidth="1"/>
+    <col min="6404" max="6405" width="19.36328125" customWidth="1"/>
     <col min="6414" max="6414" width="10" bestFit="1" customWidth="1"/>
-    <col min="6415" max="6415" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="6415" max="6415" width="17.36328125" bestFit="1" customWidth="1"/>
     <col min="6418" max="6418" width="10" bestFit="1" customWidth="1"/>
-    <col min="6422" max="6422" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="6422" max="6422" width="18.1796875" bestFit="1" customWidth="1"/>
     <col min="6424" max="6424" width="7" customWidth="1"/>
-    <col min="6426" max="6426" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="6657" max="6657" width="43.33203125" customWidth="1"/>
-    <col min="6658" max="6658" width="12.6640625" customWidth="1"/>
-    <col min="6659" max="6659" width="19.6640625" customWidth="1"/>
-    <col min="6660" max="6661" width="19.33203125" customWidth="1"/>
+    <col min="6426" max="6426" width="17.36328125" bestFit="1" customWidth="1"/>
+    <col min="6657" max="6657" width="43.36328125" customWidth="1"/>
+    <col min="6658" max="6658" width="12.6328125" customWidth="1"/>
+    <col min="6659" max="6659" width="19.6328125" customWidth="1"/>
+    <col min="6660" max="6661" width="19.36328125" customWidth="1"/>
     <col min="6670" max="6670" width="10" bestFit="1" customWidth="1"/>
-    <col min="6671" max="6671" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="6671" max="6671" width="17.36328125" bestFit="1" customWidth="1"/>
     <col min="6674" max="6674" width="10" bestFit="1" customWidth="1"/>
-    <col min="6678" max="6678" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="6678" max="6678" width="18.1796875" bestFit="1" customWidth="1"/>
     <col min="6680" max="6680" width="7" customWidth="1"/>
-    <col min="6682" max="6682" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="6913" max="6913" width="43.33203125" customWidth="1"/>
-    <col min="6914" max="6914" width="12.6640625" customWidth="1"/>
-    <col min="6915" max="6915" width="19.6640625" customWidth="1"/>
-    <col min="6916" max="6917" width="19.33203125" customWidth="1"/>
+    <col min="6682" max="6682" width="17.36328125" bestFit="1" customWidth="1"/>
+    <col min="6913" max="6913" width="43.36328125" customWidth="1"/>
+    <col min="6914" max="6914" width="12.6328125" customWidth="1"/>
+    <col min="6915" max="6915" width="19.6328125" customWidth="1"/>
+    <col min="6916" max="6917" width="19.36328125" customWidth="1"/>
     <col min="6926" max="6926" width="10" bestFit="1" customWidth="1"/>
-    <col min="6927" max="6927" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="6927" max="6927" width="17.36328125" bestFit="1" customWidth="1"/>
     <col min="6930" max="6930" width="10" bestFit="1" customWidth="1"/>
-    <col min="6934" max="6934" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="6934" max="6934" width="18.1796875" bestFit="1" customWidth="1"/>
     <col min="6936" max="6936" width="7" customWidth="1"/>
-    <col min="6938" max="6938" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="7169" max="7169" width="43.33203125" customWidth="1"/>
-    <col min="7170" max="7170" width="12.6640625" customWidth="1"/>
-    <col min="7171" max="7171" width="19.6640625" customWidth="1"/>
-    <col min="7172" max="7173" width="19.33203125" customWidth="1"/>
+    <col min="6938" max="6938" width="17.36328125" bestFit="1" customWidth="1"/>
+    <col min="7169" max="7169" width="43.36328125" customWidth="1"/>
+    <col min="7170" max="7170" width="12.6328125" customWidth="1"/>
+    <col min="7171" max="7171" width="19.6328125" customWidth="1"/>
+    <col min="7172" max="7173" width="19.36328125" customWidth="1"/>
     <col min="7182" max="7182" width="10" bestFit="1" customWidth="1"/>
-    <col min="7183" max="7183" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="7183" max="7183" width="17.36328125" bestFit="1" customWidth="1"/>
     <col min="7186" max="7186" width="10" bestFit="1" customWidth="1"/>
-    <col min="7190" max="7190" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="7190" max="7190" width="18.1796875" bestFit="1" customWidth="1"/>
     <col min="7192" max="7192" width="7" customWidth="1"/>
-    <col min="7194" max="7194" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="7425" max="7425" width="43.33203125" customWidth="1"/>
-    <col min="7426" max="7426" width="12.6640625" customWidth="1"/>
-    <col min="7427" max="7427" width="19.6640625" customWidth="1"/>
-    <col min="7428" max="7429" width="19.33203125" customWidth="1"/>
+    <col min="7194" max="7194" width="17.36328125" bestFit="1" customWidth="1"/>
+    <col min="7425" max="7425" width="43.36328125" customWidth="1"/>
+    <col min="7426" max="7426" width="12.6328125" customWidth="1"/>
+    <col min="7427" max="7427" width="19.6328125" customWidth="1"/>
+    <col min="7428" max="7429" width="19.36328125" customWidth="1"/>
     <col min="7438" max="7438" width="10" bestFit="1" customWidth="1"/>
-    <col min="7439" max="7439" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="7439" max="7439" width="17.36328125" bestFit="1" customWidth="1"/>
     <col min="7442" max="7442" width="10" bestFit="1" customWidth="1"/>
-    <col min="7446" max="7446" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="7446" max="7446" width="18.1796875" bestFit="1" customWidth="1"/>
     <col min="7448" max="7448" width="7" customWidth="1"/>
-    <col min="7450" max="7450" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="7681" max="7681" width="43.33203125" customWidth="1"/>
-    <col min="7682" max="7682" width="12.6640625" customWidth="1"/>
-    <col min="7683" max="7683" width="19.6640625" customWidth="1"/>
-    <col min="7684" max="7685" width="19.33203125" customWidth="1"/>
+    <col min="7450" max="7450" width="17.36328125" bestFit="1" customWidth="1"/>
+    <col min="7681" max="7681" width="43.36328125" customWidth="1"/>
+    <col min="7682" max="7682" width="12.6328125" customWidth="1"/>
+    <col min="7683" max="7683" width="19.6328125" customWidth="1"/>
+    <col min="7684" max="7685" width="19.36328125" customWidth="1"/>
     <col min="7694" max="7694" width="10" bestFit="1" customWidth="1"/>
-    <col min="7695" max="7695" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="7695" max="7695" width="17.36328125" bestFit="1" customWidth="1"/>
     <col min="7698" max="7698" width="10" bestFit="1" customWidth="1"/>
-    <col min="7702" max="7702" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="7702" max="7702" width="18.1796875" bestFit="1" customWidth="1"/>
     <col min="7704" max="7704" width="7" customWidth="1"/>
-    <col min="7706" max="7706" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="7937" max="7937" width="43.33203125" customWidth="1"/>
-    <col min="7938" max="7938" width="12.6640625" customWidth="1"/>
-    <col min="7939" max="7939" width="19.6640625" customWidth="1"/>
-    <col min="7940" max="7941" width="19.33203125" customWidth="1"/>
+    <col min="7706" max="7706" width="17.36328125" bestFit="1" customWidth="1"/>
+    <col min="7937" max="7937" width="43.36328125" customWidth="1"/>
+    <col min="7938" max="7938" width="12.6328125" customWidth="1"/>
+    <col min="7939" max="7939" width="19.6328125" customWidth="1"/>
+    <col min="7940" max="7941" width="19.36328125" customWidth="1"/>
     <col min="7950" max="7950" width="10" bestFit="1" customWidth="1"/>
-    <col min="7951" max="7951" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="7951" max="7951" width="17.36328125" bestFit="1" customWidth="1"/>
     <col min="7954" max="7954" width="10" bestFit="1" customWidth="1"/>
-    <col min="7958" max="7958" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="7958" max="7958" width="18.1796875" bestFit="1" customWidth="1"/>
     <col min="7960" max="7960" width="7" customWidth="1"/>
-    <col min="7962" max="7962" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="8193" max="8193" width="43.33203125" customWidth="1"/>
-    <col min="8194" max="8194" width="12.6640625" customWidth="1"/>
-    <col min="8195" max="8195" width="19.6640625" customWidth="1"/>
-    <col min="8196" max="8197" width="19.33203125" customWidth="1"/>
+    <col min="7962" max="7962" width="17.36328125" bestFit="1" customWidth="1"/>
+    <col min="8193" max="8193" width="43.36328125" customWidth="1"/>
+    <col min="8194" max="8194" width="12.6328125" customWidth="1"/>
+    <col min="8195" max="8195" width="19.6328125" customWidth="1"/>
+    <col min="8196" max="8197" width="19.36328125" customWidth="1"/>
     <col min="8206" max="8206" width="10" bestFit="1" customWidth="1"/>
-    <col min="8207" max="8207" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="8207" max="8207" width="17.36328125" bestFit="1" customWidth="1"/>
     <col min="8210" max="8210" width="10" bestFit="1" customWidth="1"/>
-    <col min="8214" max="8214" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="8214" max="8214" width="18.1796875" bestFit="1" customWidth="1"/>
     <col min="8216" max="8216" width="7" customWidth="1"/>
-    <col min="8218" max="8218" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="8449" max="8449" width="43.33203125" customWidth="1"/>
-    <col min="8450" max="8450" width="12.6640625" customWidth="1"/>
-    <col min="8451" max="8451" width="19.6640625" customWidth="1"/>
-    <col min="8452" max="8453" width="19.33203125" customWidth="1"/>
+    <col min="8218" max="8218" width="17.36328125" bestFit="1" customWidth="1"/>
+    <col min="8449" max="8449" width="43.36328125" customWidth="1"/>
+    <col min="8450" max="8450" width="12.6328125" customWidth="1"/>
+    <col min="8451" max="8451" width="19.6328125" customWidth="1"/>
+    <col min="8452" max="8453" width="19.36328125" customWidth="1"/>
     <col min="8462" max="8462" width="10" bestFit="1" customWidth="1"/>
-    <col min="8463" max="8463" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="8463" max="8463" width="17.36328125" bestFit="1" customWidth="1"/>
     <col min="8466" max="8466" width="10" bestFit="1" customWidth="1"/>
-    <col min="8470" max="8470" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="8470" max="8470" width="18.1796875" bestFit="1" customWidth="1"/>
     <col min="8472" max="8472" width="7" customWidth="1"/>
-    <col min="8474" max="8474" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="8705" max="8705" width="43.33203125" customWidth="1"/>
-    <col min="8706" max="8706" width="12.6640625" customWidth="1"/>
-    <col min="8707" max="8707" width="19.6640625" customWidth="1"/>
-    <col min="8708" max="8709" width="19.33203125" customWidth="1"/>
+    <col min="8474" max="8474" width="17.36328125" bestFit="1" customWidth="1"/>
+    <col min="8705" max="8705" width="43.36328125" customWidth="1"/>
+    <col min="8706" max="8706" width="12.6328125" customWidth="1"/>
+    <col min="8707" max="8707" width="19.6328125" customWidth="1"/>
+    <col min="8708" max="8709" width="19.36328125" customWidth="1"/>
     <col min="8718" max="8718" width="10" bestFit="1" customWidth="1"/>
-    <col min="8719" max="8719" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="8719" max="8719" width="17.36328125" bestFit="1" customWidth="1"/>
     <col min="8722" max="8722" width="10" bestFit="1" customWidth="1"/>
-    <col min="8726" max="8726" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="8726" max="8726" width="18.1796875" bestFit="1" customWidth="1"/>
     <col min="8728" max="8728" width="7" customWidth="1"/>
-    <col min="8730" max="8730" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="8961" max="8961" width="43.33203125" customWidth="1"/>
-    <col min="8962" max="8962" width="12.6640625" customWidth="1"/>
-    <col min="8963" max="8963" width="19.6640625" customWidth="1"/>
-    <col min="8964" max="8965" width="19.33203125" customWidth="1"/>
+    <col min="8730" max="8730" width="17.36328125" bestFit="1" customWidth="1"/>
+    <col min="8961" max="8961" width="43.36328125" customWidth="1"/>
+    <col min="8962" max="8962" width="12.6328125" customWidth="1"/>
+    <col min="8963" max="8963" width="19.6328125" customWidth="1"/>
+    <col min="8964" max="8965" width="19.36328125" customWidth="1"/>
     <col min="8974" max="8974" width="10" bestFit="1" customWidth="1"/>
-    <col min="8975" max="8975" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="8975" max="8975" width="17.36328125" bestFit="1" customWidth="1"/>
     <col min="8978" max="8978" width="10" bestFit="1" customWidth="1"/>
-    <col min="8982" max="8982" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="8982" max="8982" width="18.1796875" bestFit="1" customWidth="1"/>
     <col min="8984" max="8984" width="7" customWidth="1"/>
-    <col min="8986" max="8986" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="9217" max="9217" width="43.33203125" customWidth="1"/>
-    <col min="9218" max="9218" width="12.6640625" customWidth="1"/>
-    <col min="9219" max="9219" width="19.6640625" customWidth="1"/>
-    <col min="9220" max="9221" width="19.33203125" customWidth="1"/>
+    <col min="8986" max="8986" width="17.36328125" bestFit="1" customWidth="1"/>
+    <col min="9217" max="9217" width="43.36328125" customWidth="1"/>
+    <col min="9218" max="9218" width="12.6328125" customWidth="1"/>
+    <col min="9219" max="9219" width="19.6328125" customWidth="1"/>
+    <col min="9220" max="9221" width="19.36328125" customWidth="1"/>
     <col min="9230" max="9230" width="10" bestFit="1" customWidth="1"/>
-    <col min="9231" max="9231" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="9231" max="9231" width="17.36328125" bestFit="1" customWidth="1"/>
     <col min="9234" max="9234" width="10" bestFit="1" customWidth="1"/>
-    <col min="9238" max="9238" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="9238" max="9238" width="18.1796875" bestFit="1" customWidth="1"/>
     <col min="9240" max="9240" width="7" customWidth="1"/>
-    <col min="9242" max="9242" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="9473" max="9473" width="43.33203125" customWidth="1"/>
-    <col min="9474" max="9474" width="12.6640625" customWidth="1"/>
-    <col min="9475" max="9475" width="19.6640625" customWidth="1"/>
-    <col min="9476" max="9477" width="19.33203125" customWidth="1"/>
+    <col min="9242" max="9242" width="17.36328125" bestFit="1" customWidth="1"/>
+    <col min="9473" max="9473" width="43.36328125" customWidth="1"/>
+    <col min="9474" max="9474" width="12.6328125" customWidth="1"/>
+    <col min="9475" max="9475" width="19.6328125" customWidth="1"/>
+    <col min="9476" max="9477" width="19.36328125" customWidth="1"/>
     <col min="9486" max="9486" width="10" bestFit="1" customWidth="1"/>
-    <col min="9487" max="9487" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="9487" max="9487" width="17.36328125" bestFit="1" customWidth="1"/>
     <col min="9490" max="9490" width="10" bestFit="1" customWidth="1"/>
-    <col min="9494" max="9494" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="9494" max="9494" width="18.1796875" bestFit="1" customWidth="1"/>
     <col min="9496" max="9496" width="7" customWidth="1"/>
-    <col min="9498" max="9498" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="9729" max="9729" width="43.33203125" customWidth="1"/>
-    <col min="9730" max="9730" width="12.6640625" customWidth="1"/>
-    <col min="9731" max="9731" width="19.6640625" customWidth="1"/>
-    <col min="9732" max="9733" width="19.33203125" customWidth="1"/>
+    <col min="9498" max="9498" width="17.36328125" bestFit="1" customWidth="1"/>
+    <col min="9729" max="9729" width="43.36328125" customWidth="1"/>
+    <col min="9730" max="9730" width="12.6328125" customWidth="1"/>
+    <col min="9731" max="9731" width="19.6328125" customWidth="1"/>
+    <col min="9732" max="9733" width="19.36328125" customWidth="1"/>
     <col min="9742" max="9742" width="10" bestFit="1" customWidth="1"/>
-    <col min="9743" max="9743" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="9743" max="9743" width="17.36328125" bestFit="1" customWidth="1"/>
     <col min="9746" max="9746" width="10" bestFit="1" customWidth="1"/>
-    <col min="9750" max="9750" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="9750" max="9750" width="18.1796875" bestFit="1" customWidth="1"/>
     <col min="9752" max="9752" width="7" customWidth="1"/>
-    <col min="9754" max="9754" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="9985" max="9985" width="43.33203125" customWidth="1"/>
-    <col min="9986" max="9986" width="12.6640625" customWidth="1"/>
-    <col min="9987" max="9987" width="19.6640625" customWidth="1"/>
-    <col min="9988" max="9989" width="19.33203125" customWidth="1"/>
+    <col min="9754" max="9754" width="17.36328125" bestFit="1" customWidth="1"/>
+    <col min="9985" max="9985" width="43.36328125" customWidth="1"/>
+    <col min="9986" max="9986" width="12.6328125" customWidth="1"/>
+    <col min="9987" max="9987" width="19.6328125" customWidth="1"/>
+    <col min="9988" max="9989" width="19.36328125" customWidth="1"/>
     <col min="9998" max="9998" width="10" bestFit="1" customWidth="1"/>
-    <col min="9999" max="9999" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="9999" max="9999" width="17.36328125" bestFit="1" customWidth="1"/>
     <col min="10002" max="10002" width="10" bestFit="1" customWidth="1"/>
-    <col min="10006" max="10006" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="10006" max="10006" width="18.1796875" bestFit="1" customWidth="1"/>
     <col min="10008" max="10008" width="7" customWidth="1"/>
-    <col min="10010" max="10010" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="10241" max="10241" width="43.33203125" customWidth="1"/>
-    <col min="10242" max="10242" width="12.6640625" customWidth="1"/>
-    <col min="10243" max="10243" width="19.6640625" customWidth="1"/>
-    <col min="10244" max="10245" width="19.33203125" customWidth="1"/>
+    <col min="10010" max="10010" width="17.36328125" bestFit="1" customWidth="1"/>
+    <col min="10241" max="10241" width="43.36328125" customWidth="1"/>
+    <col min="10242" max="10242" width="12.6328125" customWidth="1"/>
+    <col min="10243" max="10243" width="19.6328125" customWidth="1"/>
+    <col min="10244" max="10245" width="19.36328125" customWidth="1"/>
     <col min="10254" max="10254" width="10" bestFit="1" customWidth="1"/>
-    <col min="10255" max="10255" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="10255" max="10255" width="17.36328125" bestFit="1" customWidth="1"/>
     <col min="10258" max="10258" width="10" bestFit="1" customWidth="1"/>
-    <col min="10262" max="10262" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="10262" max="10262" width="18.1796875" bestFit="1" customWidth="1"/>
     <col min="10264" max="10264" width="7" customWidth="1"/>
-    <col min="10266" max="10266" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="10497" max="10497" width="43.33203125" customWidth="1"/>
-    <col min="10498" max="10498" width="12.6640625" customWidth="1"/>
-    <col min="10499" max="10499" width="19.6640625" customWidth="1"/>
-    <col min="10500" max="10501" width="19.33203125" customWidth="1"/>
+    <col min="10266" max="10266" width="17.36328125" bestFit="1" customWidth="1"/>
+    <col min="10497" max="10497" width="43.36328125" customWidth="1"/>
+    <col min="10498" max="10498" width="12.6328125" customWidth="1"/>
+    <col min="10499" max="10499" width="19.6328125" customWidth="1"/>
+    <col min="10500" max="10501" width="19.36328125" customWidth="1"/>
     <col min="10510" max="10510" width="10" bestFit="1" customWidth="1"/>
-    <col min="10511" max="10511" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="10511" max="10511" width="17.36328125" bestFit="1" customWidth="1"/>
     <col min="10514" max="10514" width="10" bestFit="1" customWidth="1"/>
-    <col min="10518" max="10518" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="10518" max="10518" width="18.1796875" bestFit="1" customWidth="1"/>
     <col min="10520" max="10520" width="7" customWidth="1"/>
-    <col min="10522" max="10522" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="10753" max="10753" width="43.33203125" customWidth="1"/>
-    <col min="10754" max="10754" width="12.6640625" customWidth="1"/>
-    <col min="10755" max="10755" width="19.6640625" customWidth="1"/>
-    <col min="10756" max="10757" width="19.33203125" customWidth="1"/>
+    <col min="10522" max="10522" width="17.36328125" bestFit="1" customWidth="1"/>
+    <col min="10753" max="10753" width="43.36328125" customWidth="1"/>
+    <col min="10754" max="10754" width="12.6328125" customWidth="1"/>
+    <col min="10755" max="10755" width="19.6328125" customWidth="1"/>
+    <col min="10756" max="10757" width="19.36328125" customWidth="1"/>
     <col min="10766" max="10766" width="10" bestFit="1" customWidth="1"/>
-    <col min="10767" max="10767" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="10767" max="10767" width="17.36328125" bestFit="1" customWidth="1"/>
     <col min="10770" max="10770" width="10" bestFit="1" customWidth="1"/>
-    <col min="10774" max="10774" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="10774" max="10774" width="18.1796875" bestFit="1" customWidth="1"/>
     <col min="10776" max="10776" width="7" customWidth="1"/>
-    <col min="10778" max="10778" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="11009" max="11009" width="43.33203125" customWidth="1"/>
-    <col min="11010" max="11010" width="12.6640625" customWidth="1"/>
-    <col min="11011" max="11011" width="19.6640625" customWidth="1"/>
-    <col min="11012" max="11013" width="19.33203125" customWidth="1"/>
+    <col min="10778" max="10778" width="17.36328125" bestFit="1" customWidth="1"/>
+    <col min="11009" max="11009" width="43.36328125" customWidth="1"/>
+    <col min="11010" max="11010" width="12.6328125" customWidth="1"/>
+    <col min="11011" max="11011" width="19.6328125" customWidth="1"/>
+    <col min="11012" max="11013" width="19.36328125" customWidth="1"/>
     <col min="11022" max="11022" width="10" bestFit="1" customWidth="1"/>
-    <col min="11023" max="11023" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="11023" max="11023" width="17.36328125" bestFit="1" customWidth="1"/>
     <col min="11026" max="11026" width="10" bestFit="1" customWidth="1"/>
-    <col min="11030" max="11030" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="11030" max="11030" width="18.1796875" bestFit="1" customWidth="1"/>
     <col min="11032" max="11032" width="7" customWidth="1"/>
-    <col min="11034" max="11034" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="11265" max="11265" width="43.33203125" customWidth="1"/>
-    <col min="11266" max="11266" width="12.6640625" customWidth="1"/>
-    <col min="11267" max="11267" width="19.6640625" customWidth="1"/>
-    <col min="11268" max="11269" width="19.33203125" customWidth="1"/>
+    <col min="11034" max="11034" width="17.36328125" bestFit="1" customWidth="1"/>
+    <col min="11265" max="11265" width="43.36328125" customWidth="1"/>
+    <col min="11266" max="11266" width="12.6328125" customWidth="1"/>
+    <col min="11267" max="11267" width="19.6328125" customWidth="1"/>
+    <col min="11268" max="11269" width="19.36328125" customWidth="1"/>
     <col min="11278" max="11278" width="10" bestFit="1" customWidth="1"/>
-    <col min="11279" max="11279" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="11279" max="11279" width="17.36328125" bestFit="1" customWidth="1"/>
     <col min="11282" max="11282" width="10" bestFit="1" customWidth="1"/>
-    <col min="11286" max="11286" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="11286" max="11286" width="18.1796875" bestFit="1" customWidth="1"/>
     <col min="11288" max="11288" width="7" customWidth="1"/>
-    <col min="11290" max="11290" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="11521" max="11521" width="43.33203125" customWidth="1"/>
-    <col min="11522" max="11522" width="12.6640625" customWidth="1"/>
-    <col min="11523" max="11523" width="19.6640625" customWidth="1"/>
-    <col min="11524" max="11525" width="19.33203125" customWidth="1"/>
+    <col min="11290" max="11290" width="17.36328125" bestFit="1" customWidth="1"/>
+    <col min="11521" max="11521" width="43.36328125" customWidth="1"/>
+    <col min="11522" max="11522" width="12.6328125" customWidth="1"/>
+    <col min="11523" max="11523" width="19.6328125" customWidth="1"/>
+    <col min="11524" max="11525" width="19.36328125" customWidth="1"/>
     <col min="11534" max="11534" width="10" bestFit="1" customWidth="1"/>
-    <col min="11535" max="11535" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="11535" max="11535" width="17.36328125" bestFit="1" customWidth="1"/>
     <col min="11538" max="11538" width="10" bestFit="1" customWidth="1"/>
-    <col min="11542" max="11542" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="11542" max="11542" width="18.1796875" bestFit="1" customWidth="1"/>
     <col min="11544" max="11544" width="7" customWidth="1"/>
-    <col min="11546" max="11546" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="11777" max="11777" width="43.33203125" customWidth="1"/>
-    <col min="11778" max="11778" width="12.6640625" customWidth="1"/>
-    <col min="11779" max="11779" width="19.6640625" customWidth="1"/>
-    <col min="11780" max="11781" width="19.33203125" customWidth="1"/>
+    <col min="11546" max="11546" width="17.36328125" bestFit="1" customWidth="1"/>
+    <col min="11777" max="11777" width="43.36328125" customWidth="1"/>
+    <col min="11778" max="11778" width="12.6328125" customWidth="1"/>
+    <col min="11779" max="11779" width="19.6328125" customWidth="1"/>
+    <col min="11780" max="11781" width="19.36328125" customWidth="1"/>
     <col min="11790" max="11790" width="10" bestFit="1" customWidth="1"/>
-    <col min="11791" max="11791" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="11791" max="11791" width="17.36328125" bestFit="1" customWidth="1"/>
     <col min="11794" max="11794" width="10" bestFit="1" customWidth="1"/>
-    <col min="11798" max="11798" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="11798" max="11798" width="18.1796875" bestFit="1" customWidth="1"/>
     <col min="11800" max="11800" width="7" customWidth="1"/>
-    <col min="11802" max="11802" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="12033" max="12033" width="43.33203125" customWidth="1"/>
-    <col min="12034" max="12034" width="12.6640625" customWidth="1"/>
-    <col min="12035" max="12035" width="19.6640625" customWidth="1"/>
-    <col min="12036" max="12037" width="19.33203125" customWidth="1"/>
+    <col min="11802" max="11802" width="17.36328125" bestFit="1" customWidth="1"/>
+    <col min="12033" max="12033" width="43.36328125" customWidth="1"/>
+    <col min="12034" max="12034" width="12.6328125" customWidth="1"/>
+    <col min="12035" max="12035" width="19.6328125" customWidth="1"/>
+    <col min="12036" max="12037" width="19.36328125" customWidth="1"/>
     <col min="12046" max="12046" width="10" bestFit="1" customWidth="1"/>
-    <col min="12047" max="12047" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="12047" max="12047" width="17.36328125" bestFit="1" customWidth="1"/>
     <col min="12050" max="12050" width="10" bestFit="1" customWidth="1"/>
-    <col min="12054" max="12054" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="12054" max="12054" width="18.1796875" bestFit="1" customWidth="1"/>
     <col min="12056" max="12056" width="7" customWidth="1"/>
-    <col min="12058" max="12058" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="12289" max="12289" width="43.33203125" customWidth="1"/>
-    <col min="12290" max="12290" width="12.6640625" customWidth="1"/>
-    <col min="12291" max="12291" width="19.6640625" customWidth="1"/>
-    <col min="12292" max="12293" width="19.33203125" customWidth="1"/>
+    <col min="12058" max="12058" width="17.36328125" bestFit="1" customWidth="1"/>
+    <col min="12289" max="12289" width="43.36328125" customWidth="1"/>
+    <col min="12290" max="12290" width="12.6328125" customWidth="1"/>
+    <col min="12291" max="12291" width="19.6328125" customWidth="1"/>
+    <col min="12292" max="12293" width="19.36328125" customWidth="1"/>
     <col min="12302" max="12302" width="10" bestFit="1" customWidth="1"/>
-    <col min="12303" max="12303" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="12303" max="12303" width="17.36328125" bestFit="1" customWidth="1"/>
     <col min="12306" max="12306" width="10" bestFit="1" customWidth="1"/>
-    <col min="12310" max="12310" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="12310" max="12310" width="18.1796875" bestFit="1" customWidth="1"/>
     <col min="12312" max="12312" width="7" customWidth="1"/>
-    <col min="12314" max="12314" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="12545" max="12545" width="43.33203125" customWidth="1"/>
-    <col min="12546" max="12546" width="12.6640625" customWidth="1"/>
-    <col min="12547" max="12547" width="19.6640625" customWidth="1"/>
-    <col min="12548" max="12549" width="19.33203125" customWidth="1"/>
+    <col min="12314" max="12314" width="17.36328125" bestFit="1" customWidth="1"/>
+    <col min="12545" max="12545" width="43.36328125" customWidth="1"/>
+    <col min="12546" max="12546" width="12.6328125" customWidth="1"/>
+    <col min="12547" max="12547" width="19.6328125" customWidth="1"/>
+    <col min="12548" max="12549" width="19.36328125" customWidth="1"/>
     <col min="12558" max="12558" width="10" bestFit="1" customWidth="1"/>
-    <col min="12559" max="12559" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="12559" max="12559" width="17.36328125" bestFit="1" customWidth="1"/>
     <col min="12562" max="12562" width="10" bestFit="1" customWidth="1"/>
-    <col min="12566" max="12566" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="12566" max="12566" width="18.1796875" bestFit="1" customWidth="1"/>
     <col min="12568" max="12568" width="7" customWidth="1"/>
-    <col min="12570" max="12570" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="12801" max="12801" width="43.33203125" customWidth="1"/>
-    <col min="12802" max="12802" width="12.6640625" customWidth="1"/>
-    <col min="12803" max="12803" width="19.6640625" customWidth="1"/>
-    <col min="12804" max="12805" width="19.33203125" customWidth="1"/>
+    <col min="12570" max="12570" width="17.36328125" bestFit="1" customWidth="1"/>
+    <col min="12801" max="12801" width="43.36328125" customWidth="1"/>
+    <col min="12802" max="12802" width="12.6328125" customWidth="1"/>
+    <col min="12803" max="12803" width="19.6328125" customWidth="1"/>
+    <col min="12804" max="12805" width="19.36328125" customWidth="1"/>
     <col min="12814" max="12814" width="10" bestFit="1" customWidth="1"/>
-    <col min="12815" max="12815" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="12815" max="12815" width="17.36328125" bestFit="1" customWidth="1"/>
     <col min="12818" max="12818" width="10" bestFit="1" customWidth="1"/>
-    <col min="12822" max="12822" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="12822" max="12822" width="18.1796875" bestFit="1" customWidth="1"/>
     <col min="12824" max="12824" width="7" customWidth="1"/>
-    <col min="12826" max="12826" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="13057" max="13057" width="43.33203125" customWidth="1"/>
-    <col min="13058" max="13058" width="12.6640625" customWidth="1"/>
-    <col min="13059" max="13059" width="19.6640625" customWidth="1"/>
-    <col min="13060" max="13061" width="19.33203125" customWidth="1"/>
+    <col min="12826" max="12826" width="17.36328125" bestFit="1" customWidth="1"/>
+    <col min="13057" max="13057" width="43.36328125" customWidth="1"/>
+    <col min="13058" max="13058" width="12.6328125" customWidth="1"/>
+    <col min="13059" max="13059" width="19.6328125" customWidth="1"/>
+    <col min="13060" max="13061" width="19.36328125" customWidth="1"/>
     <col min="13070" max="13070" width="10" bestFit="1" customWidth="1"/>
-    <col min="13071" max="13071" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="13071" max="13071" width="17.36328125" bestFit="1" customWidth="1"/>
     <col min="13074" max="13074" width="10" bestFit="1" customWidth="1"/>
-    <col min="13078" max="13078" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="13078" max="13078" width="18.1796875" bestFit="1" customWidth="1"/>
     <col min="13080" max="13080" width="7" customWidth="1"/>
-    <col min="13082" max="13082" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="13313" max="13313" width="43.33203125" customWidth="1"/>
-    <col min="13314" max="13314" width="12.6640625" customWidth="1"/>
-    <col min="13315" max="13315" width="19.6640625" customWidth="1"/>
-    <col min="13316" max="13317" width="19.33203125" customWidth="1"/>
+    <col min="13082" max="13082" width="17.36328125" bestFit="1" customWidth="1"/>
+    <col min="13313" max="13313" width="43.36328125" customWidth="1"/>
+    <col min="13314" max="13314" width="12.6328125" customWidth="1"/>
+    <col min="13315" max="13315" width="19.6328125" customWidth="1"/>
+    <col min="13316" max="13317" width="19.36328125" customWidth="1"/>
     <col min="13326" max="13326" width="10" bestFit="1" customWidth="1"/>
-    <col min="13327" max="13327" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="13327" max="13327" width="17.36328125" bestFit="1" customWidth="1"/>
     <col min="13330" max="13330" width="10" bestFit="1" customWidth="1"/>
-    <col min="13334" max="13334" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="13334" max="13334" width="18.1796875" bestFit="1" customWidth="1"/>
     <col min="13336" max="13336" width="7" customWidth="1"/>
-    <col min="13338" max="13338" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="13569" max="13569" width="43.33203125" customWidth="1"/>
-    <col min="13570" max="13570" width="12.6640625" customWidth="1"/>
-    <col min="13571" max="13571" width="19.6640625" customWidth="1"/>
-    <col min="13572" max="13573" width="19.33203125" customWidth="1"/>
+    <col min="13338" max="13338" width="17.36328125" bestFit="1" customWidth="1"/>
+    <col min="13569" max="13569" width="43.36328125" customWidth="1"/>
+    <col min="13570" max="13570" width="12.6328125" customWidth="1"/>
+    <col min="13571" max="13571" width="19.6328125" customWidth="1"/>
+    <col min="13572" max="13573" width="19.36328125" customWidth="1"/>
     <col min="13582" max="13582" width="10" bestFit="1" customWidth="1"/>
-    <col min="13583" max="13583" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="13583" max="13583" width="17.36328125" bestFit="1" customWidth="1"/>
     <col min="13586" max="13586" width="10" bestFit="1" customWidth="1"/>
-    <col min="13590" max="13590" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="13590" max="13590" width="18.1796875" bestFit="1" customWidth="1"/>
     <col min="13592" max="13592" width="7" customWidth="1"/>
-    <col min="13594" max="13594" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="13825" max="13825" width="43.33203125" customWidth="1"/>
-    <col min="13826" max="13826" width="12.6640625" customWidth="1"/>
-    <col min="13827" max="13827" width="19.6640625" customWidth="1"/>
-    <col min="13828" max="13829" width="19.33203125" customWidth="1"/>
+    <col min="13594" max="13594" width="17.36328125" bestFit="1" customWidth="1"/>
+    <col min="13825" max="13825" width="43.36328125" customWidth="1"/>
+    <col min="13826" max="13826" width="12.6328125" customWidth="1"/>
+    <col min="13827" max="13827" width="19.6328125" customWidth="1"/>
+    <col min="13828" max="13829" width="19.36328125" customWidth="1"/>
     <col min="13838" max="13838" width="10" bestFit="1" customWidth="1"/>
-    <col min="13839" max="13839" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="13839" max="13839" width="17.36328125" bestFit="1" customWidth="1"/>
     <col min="13842" max="13842" width="10" bestFit="1" customWidth="1"/>
-    <col min="13846" max="13846" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="13846" max="13846" width="18.1796875" bestFit="1" customWidth="1"/>
     <col min="13848" max="13848" width="7" customWidth="1"/>
-    <col min="13850" max="13850" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="14081" max="14081" width="43.33203125" customWidth="1"/>
-    <col min="14082" max="14082" width="12.6640625" customWidth="1"/>
-    <col min="14083" max="14083" width="19.6640625" customWidth="1"/>
-    <col min="14084" max="14085" width="19.33203125" customWidth="1"/>
+    <col min="13850" max="13850" width="17.36328125" bestFit="1" customWidth="1"/>
+    <col min="14081" max="14081" width="43.36328125" customWidth="1"/>
+    <col min="14082" max="14082" width="12.6328125" customWidth="1"/>
+    <col min="14083" max="14083" width="19.6328125" customWidth="1"/>
+    <col min="14084" max="14085" width="19.36328125" customWidth="1"/>
     <col min="14094" max="14094" width="10" bestFit="1" customWidth="1"/>
-    <col min="14095" max="14095" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="14095" max="14095" width="17.36328125" bestFit="1" customWidth="1"/>
     <col min="14098" max="14098" width="10" bestFit="1" customWidth="1"/>
-    <col min="14102" max="14102" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="14102" max="14102" width="18.1796875" bestFit="1" customWidth="1"/>
     <col min="14104" max="14104" width="7" customWidth="1"/>
-    <col min="14106" max="14106" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="14337" max="14337" width="43.33203125" customWidth="1"/>
-    <col min="14338" max="14338" width="12.6640625" customWidth="1"/>
-    <col min="14339" max="14339" width="19.6640625" customWidth="1"/>
-    <col min="14340" max="14341" width="19.33203125" customWidth="1"/>
+    <col min="14106" max="14106" width="17.36328125" bestFit="1" customWidth="1"/>
+    <col min="14337" max="14337" width="43.36328125" customWidth="1"/>
+    <col min="14338" max="14338" width="12.6328125" customWidth="1"/>
+    <col min="14339" max="14339" width="19.6328125" customWidth="1"/>
+    <col min="14340" max="14341" width="19.36328125" customWidth="1"/>
     <col min="14350" max="14350" width="10" bestFit="1" customWidth="1"/>
-    <col min="14351" max="14351" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="14351" max="14351" width="17.36328125" bestFit="1" customWidth="1"/>
     <col min="14354" max="14354" width="10" bestFit="1" customWidth="1"/>
-    <col min="14358" max="14358" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="14358" max="14358" width="18.1796875" bestFit="1" customWidth="1"/>
     <col min="14360" max="14360" width="7" customWidth="1"/>
-    <col min="14362" max="14362" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="14593" max="14593" width="43.33203125" customWidth="1"/>
-    <col min="14594" max="14594" width="12.6640625" customWidth="1"/>
-    <col min="14595" max="14595" width="19.6640625" customWidth="1"/>
-    <col min="14596" max="14597" width="19.33203125" customWidth="1"/>
+    <col min="14362" max="14362" width="17.36328125" bestFit="1" customWidth="1"/>
+    <col min="14593" max="14593" width="43.36328125" customWidth="1"/>
+    <col min="14594" max="14594" width="12.6328125" customWidth="1"/>
+    <col min="14595" max="14595" width="19.6328125" customWidth="1"/>
+    <col min="14596" max="14597" width="19.36328125" customWidth="1"/>
     <col min="14606" max="14606" width="10" bestFit="1" customWidth="1"/>
-    <col min="14607" max="14607" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="14607" max="14607" width="17.36328125" bestFit="1" customWidth="1"/>
     <col min="14610" max="14610" width="10" bestFit="1" customWidth="1"/>
-    <col min="14614" max="14614" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="14614" max="14614" width="18.1796875" bestFit="1" customWidth="1"/>
     <col min="14616" max="14616" width="7" customWidth="1"/>
-    <col min="14618" max="14618" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="14849" max="14849" width="43.33203125" customWidth="1"/>
-    <col min="14850" max="14850" width="12.6640625" customWidth="1"/>
-    <col min="14851" max="14851" width="19.6640625" customWidth="1"/>
-    <col min="14852" max="14853" width="19.33203125" customWidth="1"/>
+    <col min="14618" max="14618" width="17.36328125" bestFit="1" customWidth="1"/>
+    <col min="14849" max="14849" width="43.36328125" customWidth="1"/>
+    <col min="14850" max="14850" width="12.6328125" customWidth="1"/>
+    <col min="14851" max="14851" width="19.6328125" customWidth="1"/>
+    <col min="14852" max="14853" width="19.36328125" customWidth="1"/>
     <col min="14862" max="14862" width="10" bestFit="1" customWidth="1"/>
-    <col min="14863" max="14863" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="14863" max="14863" width="17.36328125" bestFit="1" customWidth="1"/>
     <col min="14866" max="14866" width="10" bestFit="1" customWidth="1"/>
-    <col min="14870" max="14870" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="14870" max="14870" width="18.1796875" bestFit="1" customWidth="1"/>
     <col min="14872" max="14872" width="7" customWidth="1"/>
-    <col min="14874" max="14874" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="15105" max="15105" width="43.33203125" customWidth="1"/>
-    <col min="15106" max="15106" width="12.6640625" customWidth="1"/>
-    <col min="15107" max="15107" width="19.6640625" customWidth="1"/>
-    <col min="15108" max="15109" width="19.33203125" customWidth="1"/>
+    <col min="14874" max="14874" width="17.36328125" bestFit="1" customWidth="1"/>
+    <col min="15105" max="15105" width="43.36328125" customWidth="1"/>
+    <col min="15106" max="15106" width="12.6328125" customWidth="1"/>
+    <col min="15107" max="15107" width="19.6328125" customWidth="1"/>
+    <col min="15108" max="15109" width="19.36328125" customWidth="1"/>
     <col min="15118" max="15118" width="10" bestFit="1" customWidth="1"/>
-    <col min="15119" max="15119" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="15119" max="15119" width="17.36328125" bestFit="1" customWidth="1"/>
     <col min="15122" max="15122" width="10" bestFit="1" customWidth="1"/>
-    <col min="15126" max="15126" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="15126" max="15126" width="18.1796875" bestFit="1" customWidth="1"/>
     <col min="15128" max="15128" width="7" customWidth="1"/>
-    <col min="15130" max="15130" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="15361" max="15361" width="43.33203125" customWidth="1"/>
-    <col min="15362" max="15362" width="12.6640625" customWidth="1"/>
-    <col min="15363" max="15363" width="19.6640625" customWidth="1"/>
-    <col min="15364" max="15365" width="19.33203125" customWidth="1"/>
+    <col min="15130" max="15130" width="17.36328125" bestFit="1" customWidth="1"/>
+    <col min="15361" max="15361" width="43.36328125" customWidth="1"/>
+    <col min="15362" max="15362" width="12.6328125" customWidth="1"/>
+    <col min="15363" max="15363" width="19.6328125" customWidth="1"/>
+    <col min="15364" max="15365" width="19.36328125" customWidth="1"/>
     <col min="15374" max="15374" width="10" bestFit="1" customWidth="1"/>
-    <col min="15375" max="15375" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="15375" max="15375" width="17.36328125" bestFit="1" customWidth="1"/>
     <col min="15378" max="15378" width="10" bestFit="1" customWidth="1"/>
-    <col min="15382" max="15382" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="15382" max="15382" width="18.1796875" bestFit="1" customWidth="1"/>
     <col min="15384" max="15384" width="7" customWidth="1"/>
-    <col min="15386" max="15386" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="15617" max="15617" width="43.33203125" customWidth="1"/>
-    <col min="15618" max="15618" width="12.6640625" customWidth="1"/>
-    <col min="15619" max="15619" width="19.6640625" customWidth="1"/>
-    <col min="15620" max="15621" width="19.33203125" customWidth="1"/>
+    <col min="15386" max="15386" width="17.36328125" bestFit="1" customWidth="1"/>
+    <col min="15617" max="15617" width="43.36328125" customWidth="1"/>
+    <col min="15618" max="15618" width="12.6328125" customWidth="1"/>
+    <col min="15619" max="15619" width="19.6328125" customWidth="1"/>
+    <col min="15620" max="15621" width="19.36328125" customWidth="1"/>
     <col min="15630" max="15630" width="10" bestFit="1" customWidth="1"/>
-    <col min="15631" max="15631" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="15631" max="15631" width="17.36328125" bestFit="1" customWidth="1"/>
     <col min="15634" max="15634" width="10" bestFit="1" customWidth="1"/>
-    <col min="15638" max="15638" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="15638" max="15638" width="18.1796875" bestFit="1" customWidth="1"/>
     <col min="15640" max="15640" width="7" customWidth="1"/>
-    <col min="15642" max="15642" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="15873" max="15873" width="43.33203125" customWidth="1"/>
-    <col min="15874" max="15874" width="12.6640625" customWidth="1"/>
-    <col min="15875" max="15875" width="19.6640625" customWidth="1"/>
-    <col min="15876" max="15877" width="19.33203125" customWidth="1"/>
+    <col min="15642" max="15642" width="17.36328125" bestFit="1" customWidth="1"/>
+    <col min="15873" max="15873" width="43.36328125" customWidth="1"/>
+    <col min="15874" max="15874" width="12.6328125" customWidth="1"/>
+    <col min="15875" max="15875" width="19.6328125" customWidth="1"/>
+    <col min="15876" max="15877" width="19.36328125" customWidth="1"/>
     <col min="15886" max="15886" width="10" bestFit="1" customWidth="1"/>
-    <col min="15887" max="15887" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="15887" max="15887" width="17.36328125" bestFit="1" customWidth="1"/>
     <col min="15890" max="15890" width="10" bestFit="1" customWidth="1"/>
-    <col min="15894" max="15894" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="15894" max="15894" width="18.1796875" bestFit="1" customWidth="1"/>
     <col min="15896" max="15896" width="7" customWidth="1"/>
-    <col min="15898" max="15898" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="16129" max="16129" width="43.33203125" customWidth="1"/>
-    <col min="16130" max="16130" width="12.6640625" customWidth="1"/>
-    <col min="16131" max="16131" width="19.6640625" customWidth="1"/>
-    <col min="16132" max="16133" width="19.33203125" customWidth="1"/>
+    <col min="15898" max="15898" width="17.36328125" bestFit="1" customWidth="1"/>
+    <col min="16129" max="16129" width="43.36328125" customWidth="1"/>
+    <col min="16130" max="16130" width="12.6328125" customWidth="1"/>
+    <col min="16131" max="16131" width="19.6328125" customWidth="1"/>
+    <col min="16132" max="16133" width="19.36328125" customWidth="1"/>
     <col min="16142" max="16142" width="10" bestFit="1" customWidth="1"/>
-    <col min="16143" max="16143" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="16143" max="16143" width="17.36328125" bestFit="1" customWidth="1"/>
     <col min="16146" max="16146" width="10" bestFit="1" customWidth="1"/>
-    <col min="16150" max="16150" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="16150" max="16150" width="18.1796875" bestFit="1" customWidth="1"/>
     <col min="16152" max="16152" width="7" customWidth="1"/>
-    <col min="16154" max="16154" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="16154" max="16154" width="17.36328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A1" s="36" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="37" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="38" t="s">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="A1" s="35" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="36" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="37" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="36" t="s">
+      <c r="D1" s="35" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="36" t="s">
+      <c r="E1" s="35" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="36" t="s">
+      <c r="F1" s="35" t="s">
         <v>91</v>
       </c>
-      <c r="G1" s="36" t="s">
+      <c r="G1" s="35" t="s">
         <v>17</v>
       </c>
-      <c r="H1" s="36" t="s">
+      <c r="H1" s="35" t="s">
         <v>18</v>
       </c>
-      <c r="I1" s="36" t="s">
+      <c r="I1" s="35" t="s">
         <v>19</v>
       </c>
-      <c r="J1" s="36" t="s">
+      <c r="J1" s="35" t="s">
         <v>20</v>
       </c>
-      <c r="K1" s="36" t="s">
+      <c r="K1" s="35" t="s">
         <v>21</v>
       </c>
-      <c r="L1" s="36" t="s">
+      <c r="L1" s="35" t="s">
         <v>22</v>
       </c>
-      <c r="M1" s="36" t="s">
+      <c r="M1" s="35" t="s">
         <v>23</v>
       </c>
-      <c r="N1" s="36" t="s">
+      <c r="N1" s="35" t="s">
         <v>100</v>
       </c>
-      <c r="O1" s="36" t="s">
+      <c r="O1" s="35" t="s">
         <v>24</v>
       </c>
-      <c r="P1" s="36" t="s">
+      <c r="P1" s="35" t="s">
         <v>25</v>
       </c>
-      <c r="Q1" s="36" t="s">
+      <c r="Q1" s="35" t="s">
         <v>101</v>
       </c>
-      <c r="R1" s="36" t="s">
+      <c r="R1" s="35" t="s">
         <v>102</v>
       </c>
-      <c r="S1" s="36" t="s">
+      <c r="S1" s="35" t="s">
         <v>103</v>
       </c>
-      <c r="T1" s="36" t="s">
+      <c r="T1" s="35" t="s">
         <v>104</v>
       </c>
-      <c r="U1" s="36" t="s">
+      <c r="U1" s="35" t="s">
         <v>105</v>
       </c>
-      <c r="V1" s="36" t="s">
+      <c r="V1" s="35" t="s">
         <v>106</v>
       </c>
-      <c r="W1" s="36" t="s">
+      <c r="W1" s="35" t="s">
         <v>107</v>
       </c>
-      <c r="X1" s="36" t="s">
+      <c r="X1" s="35" t="s">
         <v>108</v>
       </c>
-      <c r="Y1" s="36" t="s">
+      <c r="Y1" s="35" t="s">
         <v>109</v>
       </c>
-      <c r="Z1" s="36" t="s">
+      <c r="Z1" s="35" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>92</v>
       </c>
@@ -4458,7 +4471,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>92</v>
       </c>
@@ -4540,7 +4553,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>111</v>
       </c>
@@ -4620,7 +4633,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>114</v>
       </c>
@@ -4700,7 +4713,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>116</v>
       </c>
@@ -4780,7 +4793,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>118</v>
       </c>
@@ -4860,7 +4873,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>120</v>
       </c>
@@ -4956,94 +4969,94 @@
       <selection activeCell="U27" sqref="U27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="28.6640625" customWidth="1"/>
-    <col min="2" max="2" width="16.5" customWidth="1"/>
+    <col min="1" max="1" width="28.6328125" customWidth="1"/>
+    <col min="2" max="2" width="16.453125" customWidth="1"/>
     <col min="3" max="3" width="30" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.6640625" customWidth="1"/>
+    <col min="4" max="4" width="16.6328125" customWidth="1"/>
     <col min="5" max="5" width="23" customWidth="1"/>
     <col min="6" max="6" width="9" customWidth="1"/>
     <col min="7" max="10" width="17" customWidth="1"/>
-    <col min="11" max="11" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="18.36328125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="20" bestFit="1" customWidth="1"/>
-    <col min="13" max="21" width="8.83203125"/>
+    <col min="13" max="21" width="8.81640625"/>
     <col min="22" max="22" width="10" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="16.33203125" customWidth="1"/>
+    <col min="23" max="23" width="16.36328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A1" s="36" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="36" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="36" t="s">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A1" s="35" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="35" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="35" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="36" t="s">
+      <c r="D1" s="35" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="36" t="s">
+      <c r="E1" s="35" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="36" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="36" t="s">
+      <c r="F1" s="35" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="35" t="s">
         <v>224</v>
       </c>
-      <c r="H1" s="36" t="s">
+      <c r="H1" s="35" t="s">
         <v>221</v>
       </c>
-      <c r="I1" s="36" t="s">
+      <c r="I1" s="35" t="s">
         <v>223</v>
       </c>
-      <c r="J1" s="36" t="s">
+      <c r="J1" s="35" t="s">
         <v>222</v>
       </c>
-      <c r="K1" s="36" t="s">
+      <c r="K1" s="35" t="s">
         <v>225</v>
       </c>
-      <c r="L1" s="36" t="s">
+      <c r="L1" s="35" t="s">
         <v>226</v>
       </c>
-      <c r="M1" s="36" t="s">
+      <c r="M1" s="35" t="s">
         <v>17</v>
       </c>
-      <c r="N1" s="36" t="s">
+      <c r="N1" s="35" t="s">
         <v>18</v>
       </c>
-      <c r="O1" s="36" t="s">
+      <c r="O1" s="35" t="s">
         <v>19</v>
       </c>
-      <c r="P1" s="36" t="s">
+      <c r="P1" s="35" t="s">
         <v>20</v>
       </c>
-      <c r="Q1" s="36" t="s">
+      <c r="Q1" s="35" t="s">
         <v>21</v>
       </c>
-      <c r="R1" s="36" t="s">
+      <c r="R1" s="35" t="s">
         <v>22</v>
       </c>
-      <c r="S1" s="36" t="s">
+      <c r="S1" s="35" t="s">
         <v>23</v>
       </c>
-      <c r="T1" s="36" t="s">
+      <c r="T1" s="35" t="s">
         <v>24</v>
       </c>
-      <c r="U1" s="36" t="s">
+      <c r="U1" s="35" t="s">
         <v>25</v>
       </c>
-      <c r="V1" s="37" t="s">
+      <c r="V1" s="36" t="s">
         <v>26</v>
       </c>
-      <c r="W1" s="40" t="s">
+      <c r="W1" s="39" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>217</v>
       </c>
@@ -5112,11 +5125,11 @@
       <c r="V2" s="14" t="s">
         <v>201</v>
       </c>
-      <c r="W2" s="27" t="s">
+      <c r="W2" s="26" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>218</v>
       </c>
@@ -5184,11 +5197,11 @@
       <c r="V3" s="14" t="s">
         <v>201</v>
       </c>
-      <c r="W3" s="27" t="s">
+      <c r="W3" s="26" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>219</v>
       </c>
@@ -5257,13 +5270,13 @@
       <c r="V4" s="14" t="s">
         <v>201</v>
       </c>
-      <c r="W4" s="27" t="s">
+      <c r="W4" s="26" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A7" s="42"/>
-      <c r="U7" s="42"/>
+    <row r="7" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A7" s="41"/>
+      <c r="U7" s="41"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5279,64 +5292,64 @@
       <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="17.5" customWidth="1"/>
+    <col min="1" max="1" width="17.453125" customWidth="1"/>
     <col min="3" max="3" width="18" customWidth="1"/>
-    <col min="4" max="5" width="21.6640625" customWidth="1"/>
-    <col min="8" max="8" width="11.6640625" customWidth="1"/>
+    <col min="4" max="5" width="21.6328125" customWidth="1"/>
+    <col min="8" max="8" width="11.6328125" customWidth="1"/>
     <col min="10" max="10" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A1" s="36" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="36" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="36" t="s">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A1" s="35" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="35" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="35" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="36" t="s">
+      <c r="D1" s="35" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="36" t="s">
-        <v>5</v>
-      </c>
-      <c r="F1" s="36" t="s">
+      <c r="E1" s="35" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" s="35" t="s">
         <v>17</v>
       </c>
-      <c r="G1" s="36" t="s">
+      <c r="G1" s="35" t="s">
         <v>18</v>
       </c>
-      <c r="H1" s="36" t="s">
+      <c r="H1" s="35" t="s">
         <v>19</v>
       </c>
-      <c r="I1" s="36" t="s">
+      <c r="I1" s="35" t="s">
         <v>20</v>
       </c>
-      <c r="J1" s="36" t="s">
+      <c r="J1" s="35" t="s">
         <v>21</v>
       </c>
-      <c r="K1" s="36" t="s">
+      <c r="K1" s="35" t="s">
         <v>22</v>
       </c>
-      <c r="L1" s="36" t="s">
+      <c r="L1" s="35" t="s">
         <v>23</v>
       </c>
-      <c r="M1" s="36" t="s">
+      <c r="M1" s="35" t="s">
         <v>24</v>
       </c>
-      <c r="N1" s="36" t="s">
+      <c r="N1" s="35" t="s">
         <v>25</v>
       </c>
-      <c r="O1" s="36" t="s">
+      <c r="O1" s="35" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A2" s="36" t="s">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A2" s="35" t="s">
         <v>97</v>
       </c>
       <c r="B2" s="2" t="s">
@@ -5383,7 +5396,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>97</v>
       </c>
@@ -5431,7 +5444,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>97</v>
       </c>
@@ -5479,7 +5492,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>97</v>
       </c>
@@ -5543,16 +5556,16 @@
       <selection activeCell="AH22" sqref="AH22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="23" customWidth="1"/>
-    <col min="2" max="2" width="15.33203125" customWidth="1"/>
-    <col min="3" max="3" width="16.6640625" customWidth="1"/>
+    <col min="2" max="2" width="15.36328125" customWidth="1"/>
+    <col min="3" max="3" width="16.6328125" customWidth="1"/>
     <col min="4" max="4" width="13" customWidth="1"/>
-    <col min="15" max="15" width="29.6640625" customWidth="1"/>
+    <col min="15" max="15" width="29.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -5599,7 +5612,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>87</v>
       </c>
@@ -5661,121 +5674,121 @@
       <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="16.6640625" customWidth="1"/>
+    <col min="1" max="1" width="16.6328125" customWidth="1"/>
     <col min="4" max="4" width="15" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.33203125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.36328125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.36328125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.1796875" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="9" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="14.33203125" customWidth="1"/>
-    <col min="22" max="22" width="12.6640625" customWidth="1"/>
-    <col min="23" max="23" width="10.5" customWidth="1"/>
+    <col min="21" max="21" width="14.36328125" customWidth="1"/>
+    <col min="22" max="22" width="12.6328125" customWidth="1"/>
+    <col min="23" max="23" width="10.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:33" x14ac:dyDescent="0.2">
-      <c r="A1" s="36" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="36" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="36" t="s">
+    <row r="1" spans="1:33" x14ac:dyDescent="0.35">
+      <c r="A1" s="35" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="35" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="35" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="36" t="s">
+      <c r="D1" s="35" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="36" t="s">
+      <c r="E1" s="35" t="s">
         <v>37</v>
       </c>
-      <c r="F1" s="36" t="s">
+      <c r="F1" s="35" t="s">
         <v>38</v>
       </c>
-      <c r="G1" s="36" t="s">
+      <c r="G1" s="35" t="s">
         <v>39</v>
       </c>
-      <c r="H1" s="36" t="s">
+      <c r="H1" s="35" t="s">
         <v>40</v>
       </c>
-      <c r="I1" s="36" t="s">
+      <c r="I1" s="35" t="s">
         <v>41</v>
       </c>
-      <c r="J1" s="36" t="s">
+      <c r="J1" s="35" t="s">
         <v>42</v>
       </c>
-      <c r="K1" s="36" t="s">
+      <c r="K1" s="35" t="s">
         <v>43</v>
       </c>
-      <c r="L1" s="36" t="s">
+      <c r="L1" s="35" t="s">
         <v>44</v>
       </c>
-      <c r="M1" s="41" t="s">
+      <c r="M1" s="40" t="s">
         <v>45</v>
       </c>
-      <c r="N1" s="39" t="s">
+      <c r="N1" s="38" t="s">
         <v>46</v>
       </c>
-      <c r="O1" s="39" t="s">
+      <c r="O1" s="38" t="s">
         <v>47</v>
       </c>
-      <c r="P1" s="39" t="s">
+      <c r="P1" s="38" t="s">
         <v>48</v>
       </c>
-      <c r="Q1" s="39" t="s">
+      <c r="Q1" s="38" t="s">
         <v>49</v>
       </c>
-      <c r="R1" s="39" t="s">
+      <c r="R1" s="38" t="s">
         <v>50</v>
       </c>
-      <c r="S1" s="39" t="s">
+      <c r="S1" s="38" t="s">
         <v>51</v>
       </c>
-      <c r="T1" s="39" t="s">
+      <c r="T1" s="38" t="s">
         <v>52</v>
       </c>
-      <c r="U1" s="36" t="s">
+      <c r="U1" s="35" t="s">
         <v>3</v>
       </c>
-      <c r="V1" s="36" t="s">
+      <c r="V1" s="35" t="s">
         <v>4</v>
       </c>
-      <c r="W1" s="36" t="s">
-        <v>5</v>
-      </c>
-      <c r="X1" s="36" t="s">
+      <c r="W1" s="35" t="s">
+        <v>5</v>
+      </c>
+      <c r="X1" s="35" t="s">
         <v>17</v>
       </c>
-      <c r="Y1" s="36" t="s">
+      <c r="Y1" s="35" t="s">
         <v>18</v>
       </c>
-      <c r="Z1" s="36" t="s">
+      <c r="Z1" s="35" t="s">
         <v>19</v>
       </c>
-      <c r="AA1" s="36" t="s">
+      <c r="AA1" s="35" t="s">
         <v>20</v>
       </c>
-      <c r="AB1" s="36" t="s">
+      <c r="AB1" s="35" t="s">
         <v>21</v>
       </c>
-      <c r="AC1" s="36" t="s">
+      <c r="AC1" s="35" t="s">
         <v>22</v>
       </c>
-      <c r="AD1" s="36" t="s">
+      <c r="AD1" s="35" t="s">
         <v>23</v>
       </c>
-      <c r="AE1" s="36" t="s">
+      <c r="AE1" s="35" t="s">
         <v>24</v>
       </c>
-      <c r="AF1" s="36" t="s">
+      <c r="AF1" s="35" t="s">
         <v>25</v>
       </c>
-      <c r="AG1" s="36" t="s">
+      <c r="AG1" s="35" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>53</v>
       </c>
@@ -5880,7 +5893,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>57</v>
       </c>
@@ -6001,62 +6014,62 @@
       <selection activeCell="F54" sqref="F54"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="18.5" customWidth="1"/>
-    <col min="3" max="3" width="9.5" customWidth="1"/>
-    <col min="4" max="5" width="10.5" customWidth="1"/>
-    <col min="8" max="8" width="10.5" customWidth="1"/>
+    <col min="1" max="1" width="18.453125" customWidth="1"/>
+    <col min="3" max="3" width="9.453125" customWidth="1"/>
+    <col min="4" max="5" width="10.453125" customWidth="1"/>
+    <col min="8" max="8" width="10.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A1" s="36" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="36" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="36" t="s">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A1" s="35" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="35" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="35" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="36" t="s">
+      <c r="D1" s="35" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="36" t="s">
-        <v>5</v>
-      </c>
-      <c r="F1" s="36" t="s">
+      <c r="E1" s="35" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" s="35" t="s">
         <v>17</v>
       </c>
-      <c r="G1" s="36" t="s">
+      <c r="G1" s="35" t="s">
         <v>18</v>
       </c>
-      <c r="H1" s="36" t="s">
+      <c r="H1" s="35" t="s">
         <v>19</v>
       </c>
-      <c r="I1" s="36" t="s">
+      <c r="I1" s="35" t="s">
         <v>20</v>
       </c>
-      <c r="J1" s="36" t="s">
+      <c r="J1" s="35" t="s">
         <v>21</v>
       </c>
-      <c r="K1" s="36" t="s">
+      <c r="K1" s="35" t="s">
         <v>22</v>
       </c>
-      <c r="L1" s="36" t="s">
+      <c r="L1" s="35" t="s">
         <v>23</v>
       </c>
-      <c r="M1" s="36" t="s">
+      <c r="M1" s="35" t="s">
         <v>24</v>
       </c>
-      <c r="N1" s="36" t="s">
+      <c r="N1" s="35" t="s">
         <v>25</v>
       </c>
-      <c r="O1" s="36" t="s">
+      <c r="O1" s="35" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>60</v>
       </c>
@@ -6120,17 +6133,17 @@
       <selection activeCell="I27" sqref="I27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="24.83203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="4" width="13.33203125" customWidth="1"/>
-    <col min="5" max="5" width="17.6640625" customWidth="1"/>
-    <col min="6" max="11" width="16.5" customWidth="1"/>
-    <col min="18" max="18" width="22.6640625" customWidth="1"/>
+    <col min="1" max="1" width="24.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="4" width="13.36328125" customWidth="1"/>
+    <col min="5" max="5" width="17.6328125" customWidth="1"/>
+    <col min="6" max="11" width="16.453125" customWidth="1"/>
+    <col min="18" max="18" width="22.6328125" customWidth="1"/>
     <col min="22" max="22" width="75" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -6198,7 +6211,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>166</v>
       </c>
@@ -6220,7 +6233,7 @@
       <c r="G2" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="H2" s="22">
+      <c r="H2" s="21">
         <v>0.82</v>
       </c>
       <c r="I2" s="2">
@@ -6266,7 +6279,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>166</v>
       </c>
@@ -6288,7 +6301,7 @@
       <c r="G3" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="H3" s="22">
+      <c r="H3" s="21">
         <v>0.8</v>
       </c>
       <c r="I3" s="2">
@@ -6334,7 +6347,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>166</v>
       </c>
@@ -6356,7 +6369,7 @@
       <c r="G4" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="H4" s="22">
+      <c r="H4" s="21">
         <v>0.82</v>
       </c>
       <c r="I4" s="2">
@@ -6402,7 +6415,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>168</v>
       </c>
@@ -6424,7 +6437,7 @@
       <c r="G5" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="H5" s="22">
+      <c r="H5" s="21">
         <v>0.84</v>
       </c>
       <c r="I5" s="2">
@@ -6470,7 +6483,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>168</v>
       </c>
@@ -6492,7 +6505,7 @@
       <c r="G6" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="H6" s="22">
+      <c r="H6" s="21">
         <v>0.82</v>
       </c>
       <c r="I6" s="2">
@@ -6538,7 +6551,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>168</v>
       </c>
@@ -6560,7 +6573,7 @@
       <c r="G7" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="H7" s="22">
+      <c r="H7" s="21">
         <v>0.84</v>
       </c>
       <c r="I7" s="2">
@@ -6606,7 +6619,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>167</v>
       </c>
@@ -6628,7 +6641,7 @@
       <c r="G8" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="H8" s="22">
+      <c r="H8" s="21">
         <v>0.92</v>
       </c>
       <c r="I8" s="2">
@@ -6674,7 +6687,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>167</v>
       </c>
@@ -6696,7 +6709,7 @@
       <c r="G9" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="H9" s="22">
+      <c r="H9" s="21">
         <v>0.9</v>
       </c>
       <c r="I9" s="2">
@@ -6742,7 +6755,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>167</v>
       </c>
@@ -6764,7 +6777,7 @@
       <c r="G10" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="H10" s="22">
+      <c r="H10" s="21">
         <v>0.92</v>
       </c>
       <c r="I10" s="2">
@@ -6826,91 +6839,91 @@
       <selection activeCell="B8" sqref="B8:B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="38.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="38.6328125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="17" customWidth="1"/>
-    <col min="6" max="7" width="17.6640625" customWidth="1"/>
-    <col min="8" max="9" width="15.5" customWidth="1"/>
-    <col min="10" max="10" width="17.1640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="12" width="17.6640625" customWidth="1"/>
-    <col min="15" max="15" width="10.5" customWidth="1"/>
-    <col min="22" max="22" width="18.1640625" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="72.5" customWidth="1"/>
+    <col min="6" max="7" width="17.6328125" customWidth="1"/>
+    <col min="8" max="9" width="15.453125" customWidth="1"/>
+    <col min="10" max="10" width="17.1796875" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="17.6328125" customWidth="1"/>
+    <col min="15" max="15" width="10.453125" customWidth="1"/>
+    <col min="22" max="22" width="18.1796875" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="72.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A1" s="36" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="36" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="36" t="s">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A1" s="35" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="35" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="35" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="36" t="s">
+      <c r="D1" s="35" t="s">
         <v>163</v>
       </c>
-      <c r="E1" s="36" t="s">
+      <c r="E1" s="35" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="36" t="s">
+      <c r="F1" s="35" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="36" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" s="39" t="s">
+      <c r="G1" s="35" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="38" t="s">
         <v>174</v>
       </c>
-      <c r="I1" s="39" t="s">
+      <c r="I1" s="38" t="s">
         <v>175</v>
       </c>
-      <c r="J1" s="39" t="s">
+      <c r="J1" s="38" t="s">
         <v>187</v>
       </c>
-      <c r="K1" s="39" t="s">
+      <c r="K1" s="38" t="s">
         <v>140</v>
       </c>
-      <c r="L1" s="36" t="s">
+      <c r="L1" s="35" t="s">
         <v>162</v>
       </c>
-      <c r="M1" s="36" t="s">
+      <c r="M1" s="35" t="s">
         <v>17</v>
       </c>
-      <c r="N1" s="36" t="s">
+      <c r="N1" s="35" t="s">
         <v>18</v>
       </c>
-      <c r="O1" s="36" t="s">
+      <c r="O1" s="35" t="s">
         <v>19</v>
       </c>
-      <c r="P1" s="36" t="s">
+      <c r="P1" s="35" t="s">
         <v>20</v>
       </c>
-      <c r="Q1" s="36" t="s">
+      <c r="Q1" s="35" t="s">
         <v>21</v>
       </c>
-      <c r="R1" s="36" t="s">
+      <c r="R1" s="35" t="s">
         <v>22</v>
       </c>
-      <c r="S1" s="36" t="s">
+      <c r="S1" s="35" t="s">
         <v>23</v>
       </c>
-      <c r="T1" s="36" t="s">
+      <c r="T1" s="35" t="s">
         <v>24</v>
       </c>
-      <c r="U1" s="36" t="s">
+      <c r="U1" s="35" t="s">
         <v>25</v>
       </c>
-      <c r="V1" s="36" t="s">
+      <c r="V1" s="35" t="s">
         <v>26</v>
       </c>
-      <c r="W1" s="36" t="s">
+      <c r="W1" s="35" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="2" spans="1:23" ht="32" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:23" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>179</v>
       </c>
@@ -6932,16 +6945,16 @@
       <c r="G2" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="H2" s="28">
+      <c r="H2" s="27">
         <v>0.4</v>
       </c>
-      <c r="I2" s="32">
+      <c r="I2" s="31">
         <v>0.47</v>
       </c>
-      <c r="J2" s="34">
+      <c r="J2" s="33">
         <v>380</v>
       </c>
-      <c r="K2" s="33">
+      <c r="K2" s="32">
         <v>100</v>
       </c>
       <c r="L2" s="12">
@@ -6977,39 +6990,39 @@
       <c r="V2" s="12" t="s">
         <v>173</v>
       </c>
-      <c r="W2" s="31" t="s">
+      <c r="W2" s="30" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="3" spans="1:23" ht="32" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:23" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A3" s="6" t="s">
         <v>179</v>
       </c>
-      <c r="B3" s="23" t="s">
+      <c r="B3" s="22" t="s">
         <v>169</v>
       </c>
-      <c r="C3" s="23" t="s">
+      <c r="C3" s="22" t="s">
         <v>170</v>
       </c>
-      <c r="D3" s="23" t="s">
+      <c r="D3" s="22" t="s">
         <v>164</v>
       </c>
       <c r="E3" s="17">
         <v>2600000</v>
       </c>
-      <c r="F3" s="24">
+      <c r="F3" s="23">
         <v>3500000</v>
       </c>
-      <c r="G3" s="23" t="s">
+      <c r="G3" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="H3" s="29">
+      <c r="H3" s="28">
         <v>0.43</v>
       </c>
-      <c r="I3" s="29">
+      <c r="I3" s="28">
         <v>0.44</v>
       </c>
-      <c r="J3" s="35">
+      <c r="J3" s="34">
         <v>380</v>
       </c>
       <c r="K3" s="12">
@@ -7048,11 +7061,11 @@
       <c r="V3" s="12" t="s">
         <v>173</v>
       </c>
-      <c r="W3" s="31" t="s">
+      <c r="W3" s="30" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="4" spans="1:23" ht="32" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:23" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A4" s="16" t="s">
         <v>179</v>
       </c>
@@ -7065,22 +7078,22 @@
       <c r="D4" s="11" t="s">
         <v>164</v>
       </c>
-      <c r="E4" s="24">
+      <c r="E4" s="23">
         <v>3500000</v>
       </c>
-      <c r="F4" s="25">
+      <c r="F4" s="24">
         <v>10000000</v>
       </c>
       <c r="G4" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="H4" s="30">
+      <c r="H4" s="29">
         <v>0.45500000000000002</v>
       </c>
-      <c r="I4" s="30">
+      <c r="I4" s="29">
         <v>0.43</v>
       </c>
-      <c r="J4" s="34">
+      <c r="J4" s="33">
         <v>380</v>
       </c>
       <c r="K4" s="11">
@@ -7119,11 +7132,11 @@
       <c r="V4" s="11" t="s">
         <v>173</v>
       </c>
-      <c r="W4" s="31" t="s">
+      <c r="W4" s="30" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="5" spans="1:23" ht="32" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:23" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A5" s="16" t="s">
         <v>178</v>
       </c>
@@ -7136,22 +7149,22 @@
       <c r="D5" s="11" t="s">
         <v>177</v>
       </c>
-      <c r="E5" s="25">
+      <c r="E5" s="24">
         <v>180000</v>
       </c>
-      <c r="F5" s="25">
+      <c r="F5" s="24">
         <v>280000</v>
       </c>
       <c r="G5" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="H5" s="30">
+      <c r="H5" s="29">
         <v>0.35</v>
       </c>
-      <c r="I5" s="30">
+      <c r="I5" s="29">
         <v>0.39</v>
       </c>
-      <c r="J5" s="34">
+      <c r="J5" s="33">
         <v>380</v>
       </c>
       <c r="K5" s="11">
@@ -7190,11 +7203,11 @@
       <c r="V5" s="11" t="s">
         <v>173</v>
       </c>
-      <c r="W5" s="31" t="s">
+      <c r="W5" s="30" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="6" spans="1:23" ht="32" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:23" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A6" s="16" t="s">
         <v>178</v>
       </c>
@@ -7207,22 +7220,22 @@
       <c r="D6" s="11" t="s">
         <v>177</v>
       </c>
-      <c r="E6" s="25">
+      <c r="E6" s="24">
         <v>280000</v>
       </c>
-      <c r="F6" s="25">
+      <c r="F6" s="24">
         <v>900000</v>
       </c>
       <c r="G6" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="H6" s="30">
+      <c r="H6" s="29">
         <v>0.39</v>
       </c>
-      <c r="I6" s="30">
+      <c r="I6" s="29">
         <v>0.4</v>
       </c>
-      <c r="J6" s="34">
+      <c r="J6" s="33">
         <v>380</v>
       </c>
       <c r="K6" s="11">
@@ -7261,11 +7274,11 @@
       <c r="V6" s="11" t="s">
         <v>173</v>
       </c>
-      <c r="W6" s="31" t="s">
+      <c r="W6" s="30" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="7" spans="1:23" ht="32" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:23" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A7" s="16" t="s">
         <v>178</v>
       </c>
@@ -7278,22 +7291,22 @@
       <c r="D7" s="11" t="s">
         <v>177</v>
       </c>
-      <c r="E7" s="25">
+      <c r="E7" s="24">
         <v>900000</v>
       </c>
-      <c r="F7" s="25">
+      <c r="F7" s="24">
         <v>2600000</v>
       </c>
       <c r="G7" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="H7" s="30">
+      <c r="H7" s="29">
         <v>0.42</v>
       </c>
-      <c r="I7" s="30">
+      <c r="I7" s="29">
         <v>0.41</v>
       </c>
-      <c r="J7" s="34">
+      <c r="J7" s="33">
         <v>380</v>
       </c>
       <c r="K7" s="11">
@@ -7332,11 +7345,11 @@
       <c r="V7" s="11" t="s">
         <v>173</v>
       </c>
-      <c r="W7" s="31" t="s">
+      <c r="W7" s="30" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A8" s="16" t="s">
         <v>183</v>
       </c>
@@ -7349,22 +7362,22 @@
       <c r="D8" s="11" t="s">
         <v>182</v>
       </c>
-      <c r="E8" s="25">
+      <c r="E8" s="24">
         <v>1000000</v>
       </c>
-      <c r="F8" s="25">
+      <c r="F8" s="24">
         <v>5000000</v>
       </c>
       <c r="G8" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="H8" s="30">
+      <c r="H8" s="29">
         <v>0.15</v>
       </c>
-      <c r="I8" s="30">
+      <c r="I8" s="29">
         <v>0.65</v>
       </c>
-      <c r="J8" s="34">
+      <c r="J8" s="33">
         <v>380</v>
       </c>
       <c r="K8" s="11">
@@ -7379,7 +7392,7 @@
       <c r="N8" s="11">
         <v>0</v>
       </c>
-      <c r="O8" s="26">
+      <c r="O8" s="25">
         <v>0.74299999999999999</v>
       </c>
       <c r="P8" s="11">
@@ -7403,11 +7416,11 @@
       <c r="V8" s="11" t="s">
         <v>84</v>
       </c>
-      <c r="W8" s="27" t="s">
+      <c r="W8" s="26" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A9" s="16" t="s">
         <v>183</v>
       </c>
@@ -7420,22 +7433,22 @@
       <c r="D9" s="11" t="s">
         <v>182</v>
       </c>
-      <c r="E9" s="25">
+      <c r="E9" s="24">
         <v>5000000</v>
       </c>
-      <c r="F9" s="25">
+      <c r="F9" s="24">
         <v>50000000</v>
       </c>
       <c r="G9" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="H9" s="30">
+      <c r="H9" s="29">
         <v>0.17</v>
       </c>
-      <c r="I9" s="30">
+      <c r="I9" s="29">
         <v>0.67</v>
       </c>
-      <c r="J9" s="34">
+      <c r="J9" s="33">
         <v>380</v>
       </c>
       <c r="K9" s="11">
@@ -7474,11 +7487,11 @@
       <c r="V9" s="11" t="s">
         <v>84</v>
       </c>
-      <c r="W9" s="27" t="s">
+      <c r="W9" s="26" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A10" s="16" t="s">
         <v>184</v>
       </c>
@@ -7491,22 +7504,22 @@
       <c r="D10" s="11" t="s">
         <v>182</v>
       </c>
-      <c r="E10" s="25">
+      <c r="E10" s="24">
         <v>1000000</v>
       </c>
-      <c r="F10" s="25">
+      <c r="F10" s="24">
         <v>50000000</v>
       </c>
       <c r="G10" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="H10" s="30">
+      <c r="H10" s="29">
         <v>0.18</v>
       </c>
-      <c r="I10" s="30">
+      <c r="I10" s="29">
         <v>0.8</v>
       </c>
-      <c r="J10" s="34">
+      <c r="J10" s="33">
         <v>380</v>
       </c>
       <c r="K10" s="11">
@@ -7521,7 +7534,7 @@
       <c r="N10" s="11">
         <v>0</v>
       </c>
-      <c r="O10" s="26">
+      <c r="O10" s="25">
         <v>0.74299999999999999</v>
       </c>
       <c r="P10" s="11">
@@ -7545,11 +7558,11 @@
       <c r="V10" s="11" t="s">
         <v>84</v>
       </c>
-      <c r="W10" s="27" t="s">
+      <c r="W10" s="26" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A11" s="16" t="s">
         <v>186</v>
       </c>
@@ -7562,22 +7575,22 @@
       <c r="D11" s="11" t="s">
         <v>164</v>
       </c>
-      <c r="E11" s="25">
+      <c r="E11" s="24">
         <v>30000000</v>
       </c>
-      <c r="F11" s="25">
+      <c r="F11" s="24">
         <v>150000000</v>
       </c>
       <c r="G11" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="H11" s="30">
+      <c r="H11" s="29">
         <v>0.62</v>
       </c>
-      <c r="I11" s="30">
+      <c r="I11" s="29">
         <v>0.28999999999999998</v>
       </c>
-      <c r="J11" s="34">
+      <c r="J11" s="33">
         <v>380</v>
       </c>
       <c r="K11" s="11">
@@ -7617,11 +7630,11 @@
       <c r="V11" s="11" t="s">
         <v>84</v>
       </c>
-      <c r="W11" s="27" t="s">
+      <c r="W11" s="26" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="13" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:23" x14ac:dyDescent="0.35">
       <c r="B13" s="9"/>
     </row>
   </sheetData>
@@ -7636,88 +7649,88 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:U5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView zoomScale="125" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="28.6640625" customWidth="1"/>
-    <col min="2" max="2" width="16.5" customWidth="1"/>
-    <col min="3" max="3" width="17.83203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.6640625" customWidth="1"/>
+    <col min="1" max="1" width="28.6328125" customWidth="1"/>
+    <col min="2" max="2" width="16.453125" customWidth="1"/>
+    <col min="3" max="3" width="17.81640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.6328125" customWidth="1"/>
     <col min="5" max="6" width="23" customWidth="1"/>
-    <col min="7" max="10" width="15.83203125" customWidth="1"/>
+    <col min="7" max="10" width="15.81640625" customWidth="1"/>
     <col min="20" max="20" width="10" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="111.6640625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="111.6328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A1" s="36" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="36" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="36" t="s">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A1" s="35" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="35" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="35" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="36" t="s">
+      <c r="D1" s="35" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="36" t="s">
+      <c r="E1" s="35" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="36" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="36" t="s">
+      <c r="F1" s="35" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="35" t="s">
         <v>194</v>
       </c>
-      <c r="H1" s="36" t="s">
+      <c r="H1" s="35" t="s">
         <v>190</v>
       </c>
-      <c r="I1" s="36" t="s">
+      <c r="I1" s="35" t="s">
         <v>191</v>
       </c>
-      <c r="J1" s="36" t="s">
+      <c r="J1" s="35" t="s">
         <v>192</v>
       </c>
-      <c r="K1" s="36" t="s">
+      <c r="K1" s="35" t="s">
         <v>17</v>
       </c>
-      <c r="L1" s="36" t="s">
+      <c r="L1" s="35" t="s">
         <v>18</v>
       </c>
-      <c r="M1" s="36" t="s">
+      <c r="M1" s="35" t="s">
         <v>19</v>
       </c>
-      <c r="N1" s="36" t="s">
+      <c r="N1" s="35" t="s">
         <v>20</v>
       </c>
-      <c r="O1" s="36" t="s">
+      <c r="O1" s="35" t="s">
         <v>21</v>
       </c>
-      <c r="P1" s="36" t="s">
+      <c r="P1" s="35" t="s">
         <v>22</v>
       </c>
-      <c r="Q1" s="36" t="s">
+      <c r="Q1" s="35" t="s">
         <v>23</v>
       </c>
-      <c r="R1" s="36" t="s">
+      <c r="R1" s="35" t="s">
         <v>24</v>
       </c>
-      <c r="S1" s="37" t="s">
+      <c r="S1" s="36" t="s">
         <v>25</v>
       </c>
-      <c r="T1" s="40" t="s">
+      <c r="T1" s="39" t="s">
         <v>26</v>
       </c>
-      <c r="U1" s="40" t="s">
+      <c r="U1" s="39" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>85</v>
       </c>
@@ -7780,11 +7793,11 @@
       <c r="T2" s="11" t="s">
         <v>84</v>
       </c>
-      <c r="U2" s="27" t="s">
+      <c r="U2" s="26" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>85</v>
       </c>
@@ -7846,11 +7859,11 @@
       <c r="T3" s="11" t="s">
         <v>84</v>
       </c>
-      <c r="U3" s="27" t="s">
+      <c r="U3" s="26" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>85</v>
       </c>
@@ -7860,10 +7873,10 @@
       <c r="C4" s="12" t="s">
         <v>189</v>
       </c>
-      <c r="D4" s="24">
+      <c r="D4" s="23">
         <v>100000</v>
       </c>
-      <c r="E4" s="24">
+      <c r="E4" s="23">
         <v>10000000000</v>
       </c>
       <c r="F4" s="12" t="s">
@@ -7913,11 +7926,11 @@
       <c r="T4" s="11" t="s">
         <v>84</v>
       </c>
-      <c r="U4" s="27" t="s">
+      <c r="U4" s="26" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>237</v>
       </c>
@@ -7987,89 +8000,89 @@
       <selection activeCell="B2" sqref="B2:C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="45.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.5" customWidth="1"/>
-    <col min="5" max="6" width="15.6640625" customWidth="1"/>
-    <col min="7" max="7" width="11.1640625" customWidth="1"/>
-    <col min="8" max="8" width="12.1640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.5" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.83203125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="33.33203125" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="45.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="45.453125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.453125" customWidth="1"/>
+    <col min="5" max="6" width="15.6328125" customWidth="1"/>
+    <col min="7" max="7" width="11.1796875" customWidth="1"/>
+    <col min="8" max="8" width="12.1796875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.6328125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.453125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.81640625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="33.36328125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="45.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A1" s="36" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="36" t="s">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="A1" s="35" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="35" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>232</v>
       </c>
-      <c r="D1" s="36" t="s">
+      <c r="D1" s="35" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="36" t="s">
+      <c r="E1" s="35" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="36" t="s">
+      <c r="F1" s="35" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="36" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" s="36" t="s">
+      <c r="G1" s="35" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="35" t="s">
         <v>122</v>
       </c>
-      <c r="I1" s="36" t="s">
+      <c r="I1" s="35" t="s">
         <v>131</v>
       </c>
-      <c r="J1" s="36" t="s">
+      <c r="J1" s="35" t="s">
         <v>130</v>
       </c>
-      <c r="K1" s="36" t="s">
+      <c r="K1" s="35" t="s">
         <v>129</v>
       </c>
-      <c r="L1" s="36" t="s">
+      <c r="L1" s="35" t="s">
         <v>17</v>
       </c>
-      <c r="M1" s="36" t="s">
+      <c r="M1" s="35" t="s">
         <v>18</v>
       </c>
-      <c r="N1" s="36" t="s">
+      <c r="N1" s="35" t="s">
         <v>19</v>
       </c>
-      <c r="O1" s="36" t="s">
+      <c r="O1" s="35" t="s">
         <v>20</v>
       </c>
-      <c r="P1" s="36" t="s">
+      <c r="P1" s="35" t="s">
         <v>21</v>
       </c>
-      <c r="Q1" s="36" t="s">
+      <c r="Q1" s="35" t="s">
         <v>22</v>
       </c>
-      <c r="R1" s="36" t="s">
+      <c r="R1" s="35" t="s">
         <v>23</v>
       </c>
-      <c r="S1" s="36" t="s">
+      <c r="S1" s="35" t="s">
         <v>24</v>
       </c>
-      <c r="T1" s="36" t="s">
+      <c r="T1" s="35" t="s">
         <v>25</v>
       </c>
-      <c r="U1" s="36" t="s">
+      <c r="U1" s="35" t="s">
         <v>26</v>
       </c>
-      <c r="V1" s="36" t="s">
+      <c r="V1" s="35" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>126</v>
       </c>
@@ -8137,7 +8150,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>125</v>
       </c>
@@ -8147,7 +8160,7 @@
       <c r="C3" s="11">
         <v>0.4</v>
       </c>
-      <c r="D3" s="19" t="s">
+      <c r="D3" s="18" t="s">
         <v>124</v>
       </c>
       <c r="E3" s="17">
@@ -8207,7 +8220,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="4" spans="1:22" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:22" s="9" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>125</v>
       </c>
@@ -8217,7 +8230,7 @@
       <c r="C4" s="11">
         <v>0.4</v>
       </c>
-      <c r="D4" s="19" t="s">
+      <c r="D4" s="18" t="s">
         <v>124</v>
       </c>
       <c r="E4" s="17">
@@ -8277,7 +8290,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="5" spans="1:22" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:22" s="9" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>125</v>
       </c>
@@ -8287,7 +8300,7 @@
       <c r="C5" s="11">
         <v>0.4</v>
       </c>
-      <c r="D5" s="19" t="s">
+      <c r="D5" s="18" t="s">
         <v>124</v>
       </c>
       <c r="E5" s="17">
@@ -8347,7 +8360,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="6" spans="1:22" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:22" s="9" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>125</v>
       </c>
@@ -8357,7 +8370,7 @@
       <c r="C6" s="11">
         <v>0.4</v>
       </c>
-      <c r="D6" s="19" t="s">
+      <c r="D6" s="18" t="s">
         <v>124</v>
       </c>
       <c r="E6" s="17">
@@ -8417,7 +8430,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="7" spans="1:22" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:22" s="9" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>125</v>
       </c>
@@ -8427,7 +8440,7 @@
       <c r="C7" s="11">
         <v>0.4</v>
       </c>
-      <c r="D7" s="19" t="s">
+      <c r="D7" s="18" t="s">
         <v>124</v>
       </c>
       <c r="E7" s="17">
@@ -8485,10 +8498,10 @@
         <v>128</v>
       </c>
     </row>
-    <row r="13" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:22" x14ac:dyDescent="0.35">
       <c r="P13" s="10"/>
     </row>
-    <row r="15" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:22" x14ac:dyDescent="0.35">
       <c r="P15" s="10"/>
     </row>
   </sheetData>
@@ -8503,24 +8516,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:AG7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="Y25" sqref="Y25"/>
+    <sheetView tabSelected="1" topLeftCell="R1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AE1" sqref="AE1:AG7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="29.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.1640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.1640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.1640625" customWidth="1"/>
-    <col min="9" max="9" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.6640625" customWidth="1"/>
-    <col min="11" max="12" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="45.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="29.453125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.1796875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.6328125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.1796875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.1796875" customWidth="1"/>
+    <col min="9" max="9" width="13.6328125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.6328125" customWidth="1"/>
+    <col min="11" max="12" width="12.36328125" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="45.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -8617,11 +8630,11 @@
       <c r="AF1" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="AG1" s="1" t="s">
+      <c r="AG1" s="6" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="2" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>133</v>
       </c>
@@ -8713,16 +8726,16 @@
         <v>1.5</v>
       </c>
       <c r="AE2" s="2">
-        <v>0.72199999999999998</v>
-      </c>
-      <c r="AF2" s="2">
-        <v>0.33300000000000002</v>
-      </c>
-      <c r="AG2" s="2" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="3" spans="1:33" x14ac:dyDescent="0.2">
+        <v>3.23</v>
+      </c>
+      <c r="AF2" s="14">
+        <v>2.14</v>
+      </c>
+      <c r="AG2" s="11" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="3" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>133</v>
       </c>
@@ -8816,14 +8829,14 @@
       <c r="AE3" s="2">
         <v>81</v>
       </c>
-      <c r="AF3" s="2">
+      <c r="AF3" s="14">
         <v>33</v>
       </c>
-      <c r="AG3" s="2" t="s">
+      <c r="AG3" s="11" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="4" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>134</v>
       </c>
@@ -8914,17 +8927,17 @@
       <c r="AD4" s="2">
         <v>1.5</v>
       </c>
-      <c r="AE4" s="2">
-        <v>0.72199999999999998</v>
-      </c>
-      <c r="AF4" s="2">
-        <v>0.33300000000000002</v>
-      </c>
-      <c r="AG4" s="2" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="5" spans="1:33" x14ac:dyDescent="0.2">
+      <c r="AE4" s="14">
+        <v>3.74</v>
+      </c>
+      <c r="AF4" s="43">
+        <v>2.5</v>
+      </c>
+      <c r="AG4" s="11" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="5" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>135</v>
       </c>
@@ -9018,14 +9031,14 @@
       <c r="AE5" s="2">
         <v>68</v>
       </c>
-      <c r="AF5" s="2">
+      <c r="AF5" s="14">
         <v>14</v>
       </c>
-      <c r="AG5" s="2" t="s">
+      <c r="AG5" s="11" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="6" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>135</v>
       </c>
@@ -9116,17 +9129,17 @@
       <c r="AD6" s="2">
         <v>4.38</v>
       </c>
-      <c r="AE6" s="2">
-        <v>68</v>
-      </c>
-      <c r="AF6" s="2">
-        <v>14</v>
-      </c>
-      <c r="AG6" s="2" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="7" spans="1:33" x14ac:dyDescent="0.2">
+      <c r="AE6" s="14">
+        <v>646</v>
+      </c>
+      <c r="AF6" s="43">
+        <v>431</v>
+      </c>
+      <c r="AG6" s="11" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="7" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>136</v>
       </c>
@@ -9220,10 +9233,10 @@
       <c r="AE7" s="2">
         <v>62</v>
       </c>
-      <c r="AF7" s="2">
+      <c r="AF7" s="14">
         <v>10</v>
       </c>
-      <c r="AG7" s="18"/>
+      <c r="AG7" s="42"/>
     </row>
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
@@ -9241,91 +9254,91 @@
       <selection activeCell="V23" sqref="V23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="26.5" customWidth="1"/>
-    <col min="3" max="3" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.5" customWidth="1"/>
-    <col min="5" max="5" width="20.83203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.1640625" customWidth="1"/>
-    <col min="7" max="7" width="12.1640625" customWidth="1"/>
-    <col min="8" max="8" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.1640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.5" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.453125" customWidth="1"/>
+    <col min="3" max="3" width="11.453125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.453125" customWidth="1"/>
+    <col min="5" max="5" width="20.81640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.1796875" customWidth="1"/>
+    <col min="7" max="7" width="12.1796875" customWidth="1"/>
+    <col min="8" max="8" width="13.6328125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.1796875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.453125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.81640625" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="29" customWidth="1"/>
     <col min="22" max="22" width="69" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A1" s="36" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="36" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="36" t="s">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="A1" s="35" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="35" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="35" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="36" t="s">
+      <c r="D1" s="35" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="36" t="s">
+      <c r="E1" s="35" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="36" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="36" t="s">
+      <c r="F1" s="35" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="35" t="s">
         <v>137</v>
       </c>
-      <c r="H1" s="36" t="s">
+      <c r="H1" s="35" t="s">
         <v>131</v>
       </c>
-      <c r="I1" s="36" t="s">
+      <c r="I1" s="35" t="s">
         <v>138</v>
       </c>
-      <c r="J1" s="36" t="s">
+      <c r="J1" s="35" t="s">
         <v>140</v>
       </c>
-      <c r="K1" s="36" t="s">
+      <c r="K1" s="35" t="s">
         <v>139</v>
       </c>
-      <c r="L1" s="36" t="s">
+      <c r="L1" s="35" t="s">
         <v>17</v>
       </c>
-      <c r="M1" s="36" t="s">
+      <c r="M1" s="35" t="s">
         <v>18</v>
       </c>
-      <c r="N1" s="36" t="s">
+      <c r="N1" s="35" t="s">
         <v>19</v>
       </c>
-      <c r="O1" s="36" t="s">
+      <c r="O1" s="35" t="s">
         <v>20</v>
       </c>
-      <c r="P1" s="36" t="s">
+      <c r="P1" s="35" t="s">
         <v>21</v>
       </c>
-      <c r="Q1" s="36" t="s">
+      <c r="Q1" s="35" t="s">
         <v>22</v>
       </c>
-      <c r="R1" s="36" t="s">
+      <c r="R1" s="35" t="s">
         <v>23</v>
       </c>
-      <c r="S1" s="36" t="s">
+      <c r="S1" s="35" t="s">
         <v>24</v>
       </c>
-      <c r="T1" s="36" t="s">
+      <c r="T1" s="35" t="s">
         <v>25</v>
       </c>
-      <c r="U1" s="37" t="s">
+      <c r="U1" s="36" t="s">
         <v>26</v>
       </c>
-      <c r="V1" s="40" t="s">
+      <c r="V1" s="39" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>82</v>
       </c>
@@ -9344,7 +9357,7 @@
       <c r="F2" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="G2" s="20">
+      <c r="G2" s="19">
         <v>1.26E-2</v>
       </c>
       <c r="H2" s="2">
@@ -9393,7 +9406,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>82</v>
       </c>
@@ -9412,7 +9425,7 @@
       <c r="F3" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="G3" s="20">
+      <c r="G3" s="19">
         <v>1.26E-2</v>
       </c>
       <c r="H3" s="12">
@@ -9461,7 +9474,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>82</v>
       </c>
@@ -9480,7 +9493,7 @@
       <c r="F4" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="G4" s="20">
+      <c r="G4" s="19">
         <v>3.15E-2</v>
       </c>
       <c r="H4" s="12">
@@ -9529,7 +9542,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>82</v>
       </c>
@@ -9548,7 +9561,7 @@
       <c r="F5" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="G5" s="20">
+      <c r="G5" s="19">
         <v>3.15E-2</v>
       </c>
       <c r="H5" s="11">
@@ -9566,7 +9579,7 @@
       <c r="L5" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="M5" s="19">
+      <c r="M5" s="18">
         <v>1457.3</v>
       </c>
       <c r="N5" s="2">
@@ -9597,7 +9610,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:22" x14ac:dyDescent="0.35">
       <c r="G6" s="9"/>
       <c r="H6" s="9"/>
       <c r="I6" s="9"/>
@@ -9605,13 +9618,13 @@
       <c r="K6" s="9"/>
       <c r="V6" s="9"/>
     </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:22" x14ac:dyDescent="0.35">
       <c r="G7" s="9"/>
       <c r="H7" s="9"/>
       <c r="I7" s="9"/>
       <c r="J7" s="9"/>
       <c r="K7" s="9"/>
-      <c r="V7" s="21"/>
+      <c r="V7" s="20"/>
     </row>
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>

</xml_diff>

<commit_message>
Fix Decentraliyed optimiyation and adding air source heat pumps
</commit_message>
<xml_diff>
--- a/cea/databases/CH/components/CONVERSION.xlsx
+++ b/cea/databases/CH/components/CONVERSION.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Jimeno/Documents/GitHub/CityEnergyAnalyst/cea/databases/CH/components/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA98E919-7BBB-B546-A401-3C19C1340442}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD7A63E3-90D1-3244-B23F-93881519691C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="16680" tabRatio="993" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="21460" windowHeight="16680" tabRatio="993" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PV" sheetId="1" r:id="rId1"/>
@@ -51,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="566" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="570" uniqueCount="157">
   <si>
     <t>Description</t>
   </si>
@@ -516,6 +516,12 @@
   </si>
   <si>
     <t>None</t>
+  </si>
+  <si>
+    <t>Air source heat pump</t>
+  </si>
+  <si>
+    <t>HP3</t>
   </si>
 </sst>
 </file>
@@ -2709,10 +2715,10 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
-  <dimension ref="A1:O3"/>
+  <dimension ref="A1:O4"/>
   <sheetViews>
-    <sheetView zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="O6" sqref="O6"/>
+    <sheetView tabSelected="1" zoomScale="112" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2864,6 +2870,52 @@
         <v>6</v>
       </c>
       <c r="O3" s="2"/>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="C4" s="2">
+        <v>1</v>
+      </c>
+      <c r="D4" s="5">
+        <v>10000000000</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="G4" s="2">
+        <v>0</v>
+      </c>
+      <c r="H4" s="2">
+        <f>70.8/0.902</f>
+        <v>78.492239467849217</v>
+      </c>
+      <c r="I4" s="2">
+        <v>0.49</v>
+      </c>
+      <c r="J4" s="2">
+        <v>0</v>
+      </c>
+      <c r="K4" s="2">
+        <v>0</v>
+      </c>
+      <c r="L4" s="2">
+        <v>20</v>
+      </c>
+      <c r="M4" s="2">
+        <v>1</v>
+      </c>
+      <c r="N4" s="2">
+        <v>5</v>
+      </c>
+      <c r="O4" s="2"/>
     </row>
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
@@ -5556,8 +5608,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:P25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I21" sqref="I21"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>